<commit_message>
KIBON-75: Anpassung der Statistiken. Review
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/medu/dev/ebegu/ebegu-server/src/main/resources/reporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="20565" tabRatio="606"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -419,9 +419,6 @@
     <t>{massgEink}</t>
   </si>
   <si>
-    <t>Eingeschult</t>
-  </si>
-  <si>
     <t>{eingeschult}</t>
   </si>
   <si>
@@ -429,12 +426,15 @@
   </si>
   <si>
     <t>{betreuungsStatus}</t>
+  </si>
+  <si>
+    <t>Schulstufe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -665,6 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -713,11 +714,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -876,23 +876,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -928,23 +911,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1120,55 +1086,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BP17" sqref="BP17"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BE9" sqref="BE9:BE10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625"/>
-    <col min="3" max="3" width="15.6640625" style="1"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="8" max="16" width="8.6640625"/>
-    <col min="17" max="22" width="10.6640625"/>
-    <col min="23" max="23" width="24.1640625"/>
-    <col min="24" max="32" width="8.6640625"/>
-    <col min="33" max="38" width="10.6640625"/>
-    <col min="39" max="39" width="24.1640625"/>
-    <col min="40" max="40" width="9.1640625" customWidth="1"/>
-    <col min="42" max="42" width="6.5"/>
-    <col min="43" max="43" width="18.1640625"/>
-    <col min="45" max="45" width="23.33203125"/>
-    <col min="46" max="46" width="9.33203125"/>
-    <col min="47" max="47" width="25.5"/>
-    <col min="48" max="48" width="27.5"/>
-    <col min="49" max="49" width="10.5"/>
-    <col min="50" max="52" width="12.6640625"/>
-    <col min="53" max="53" width="16.6640625"/>
-    <col min="54" max="55" width="12.6640625"/>
+    <col min="8" max="16" width="8.7109375"/>
+    <col min="17" max="22" width="10.7109375"/>
+    <col min="23" max="23" width="24.140625"/>
+    <col min="24" max="32" width="8.7109375"/>
+    <col min="33" max="38" width="10.7109375"/>
+    <col min="39" max="39" width="24.140625"/>
+    <col min="40" max="40" width="9.140625" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125"/>
+    <col min="43" max="43" width="18.140625"/>
+    <col min="45" max="45" width="23.28515625"/>
+    <col min="46" max="46" width="9.28515625"/>
+    <col min="47" max="47" width="25.42578125"/>
+    <col min="48" max="48" width="27.42578125"/>
+    <col min="49" max="49" width="10.42578125"/>
+    <col min="50" max="52" width="12.7109375"/>
+    <col min="53" max="53" width="16.7109375"/>
+    <col min="54" max="55" width="12.7109375"/>
     <col min="56" max="56" width="22"/>
-    <col min="57" max="57" width="10.83203125" customWidth="1"/>
+    <col min="57" max="57" width="18.140625" customWidth="1"/>
     <col min="58" max="61" width="22"/>
-    <col min="62" max="63" width="12.6640625"/>
-    <col min="64" max="64" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="62" max="63" width="12.7109375"/>
+    <col min="64" max="64" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="16" hidden="1" customWidth="1"/>
     <col min="66" max="66" width="16" customWidth="1"/>
-    <col min="67" max="68" width="12.6640625"/>
-    <col min="69" max="69" width="16.83203125"/>
-    <col min="70" max="70" width="12.6640625"/>
-    <col min="71" max="71" width="19.5"/>
-    <col min="72" max="72" width="16.83203125"/>
-    <col min="73" max="75" width="12.6640625"/>
-    <col min="76" max="996" width="10.5"/>
+    <col min="67" max="68" width="12.7109375"/>
+    <col min="69" max="69" width="16.85546875"/>
+    <col min="70" max="70" width="12.7109375"/>
+    <col min="71" max="71" width="19.42578125"/>
+    <col min="72" max="72" width="16.85546875"/>
+    <col min="73" max="75" width="12.7109375"/>
+    <col min="76" max="996" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1179,10 +1145,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1162,7 @@
       <c r="BM3" s="35"/>
       <c r="BN3" s="35"/>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1171,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1214,7 +1180,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1226,92 +1192,92 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:77" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:77" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="37" t="s">
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
-      <c r="AA8" s="37"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="50"/>
-      <c r="AJ8" s="50"/>
-      <c r="AK8" s="50"/>
-      <c r="AL8" s="50"/>
-      <c r="AM8" s="50"/>
-      <c r="AN8" s="39" t="s">
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="51"/>
+      <c r="AM8" s="51"/>
+      <c r="AN8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="39"/>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39" t="s">
+      <c r="AO8" s="40"/>
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39"/>
-      <c r="AT8" s="39"/>
-      <c r="AU8" s="39"/>
-      <c r="AV8" s="39" t="s">
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="40"/>
+      <c r="AT8" s="40"/>
+      <c r="AU8" s="40"/>
+      <c r="AV8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="37" t="s">
+      <c r="AW8" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="37" t="s">
+      <c r="AX8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="37"/>
-      <c r="AZ8" s="37"/>
-      <c r="BA8" s="37"/>
-      <c r="BB8" s="37"/>
+      <c r="AY8" s="38"/>
+      <c r="AZ8" s="38"/>
+      <c r="BA8" s="38"/>
+      <c r="BB8" s="38"/>
       <c r="BC8" s="10"/>
       <c r="BD8" s="10"/>
       <c r="BE8" s="26"/>
@@ -1319,209 +1285,209 @@
       <c r="BG8" s="10"/>
       <c r="BH8" s="10"/>
       <c r="BI8" s="10"/>
-      <c r="BJ8" s="37" t="s">
+      <c r="BJ8" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="BK8" s="37"/>
-      <c r="BL8" s="37"/>
-      <c r="BM8" s="37"/>
-      <c r="BN8" s="37"/>
-      <c r="BO8" s="37"/>
-      <c r="BP8" s="37"/>
-      <c r="BQ8" s="37"/>
-      <c r="BR8" s="37"/>
-      <c r="BS8" s="37"/>
-      <c r="BT8" s="37"/>
-      <c r="BU8" s="37"/>
-      <c r="BV8" s="37"/>
-      <c r="BW8" s="37"/>
+      <c r="BK8" s="38"/>
+      <c r="BL8" s="38"/>
+      <c r="BM8" s="38"/>
+      <c r="BN8" s="38"/>
+      <c r="BO8" s="38"/>
+      <c r="BP8" s="38"/>
+      <c r="BQ8" s="38"/>
+      <c r="BR8" s="38"/>
+      <c r="BS8" s="38"/>
+      <c r="BT8" s="38"/>
+      <c r="BU8" s="38"/>
+      <c r="BV8" s="38"/>
+      <c r="BW8" s="38"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="37" t="s">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="O9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
       <c r="W9" s="14"/>
-      <c r="X9" s="51" t="s">
+      <c r="X9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="37" t="s">
+      <c r="Y9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="37" t="s">
+      <c r="Z9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="37" t="s">
+      <c r="AA9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="37" t="s">
+      <c r="AB9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="AC9" s="37" t="s">
+      <c r="AC9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="AD9" s="37" t="s">
+      <c r="AD9" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="37" t="s">
+      <c r="AE9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="AF9" s="46" t="s">
+      <c r="AF9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="46" t="s">
+      <c r="AG9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="47"/>
-      <c r="AL9" s="47"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="48"/>
+      <c r="AK9" s="48"/>
+      <c r="AL9" s="48"/>
       <c r="AM9" s="14"/>
-      <c r="AN9" s="38" t="s">
+      <c r="AN9" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="AO9" s="41" t="s">
+      <c r="AO9" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="AP9" s="39" t="s">
+      <c r="AP9" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="AQ9" s="41" t="s">
+      <c r="AQ9" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="AR9" s="41" t="s">
+      <c r="AR9" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="AS9" s="39" t="s">
+      <c r="AS9" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="AT9" s="40" t="s">
+      <c r="AT9" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="AU9" s="39" t="s">
+      <c r="AU9" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="39"/>
-      <c r="AW9" s="37"/>
-      <c r="AX9" s="37" t="s">
+      <c r="AV9" s="40"/>
+      <c r="AW9" s="38"/>
+      <c r="AX9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AY9" s="37" t="s">
+      <c r="AY9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="AZ9" s="37" t="s">
+      <c r="AZ9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="BA9" s="48" t="s">
+      <c r="BA9" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="BB9" s="37" t="s">
+      <c r="BB9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="37" t="s">
+      <c r="BC9" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="BD9" s="37" t="s">
+      <c r="BD9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="BF9" s="37" t="s">
+      <c r="BE9" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="BF9" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="37" t="s">
+      <c r="BG9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="37" t="s">
+      <c r="BH9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="37" t="s">
+      <c r="BI9" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="BJ9" s="37" t="s">
+      <c r="BJ9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="37" t="s">
+      <c r="BK9" s="38" t="s">
         <v>5</v>
       </c>
       <c r="BL9" s="24"/>
       <c r="BM9" s="24"/>
-      <c r="BN9" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="BO9" s="37" t="s">
+      <c r="BN9" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="BP9" s="37" t="s">
+      <c r="BP9" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="BQ9" s="37"/>
-      <c r="BR9" s="37"/>
-      <c r="BS9" s="37"/>
-      <c r="BT9" s="37"/>
-      <c r="BU9" s="37" t="s">
+      <c r="BQ9" s="38"/>
+      <c r="BR9" s="38"/>
+      <c r="BS9" s="38"/>
+      <c r="BT9" s="38"/>
+      <c r="BU9" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="BV9" s="37"/>
-      <c r="BW9" s="37"/>
+      <c r="BV9" s="38"/>
+      <c r="BW9" s="38"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
       <c r="Q10" s="17" t="s">
         <v>6</v>
       </c>
@@ -1543,15 +1509,15 @@
       <c r="W10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="37"/>
-      <c r="AD10" s="37"/>
-      <c r="AE10" s="37"/>
-      <c r="AF10" s="37"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
       <c r="AG10" s="17" t="s">
         <v>6</v>
       </c>
@@ -1573,38 +1539,38 @@
       <c r="AM10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="42"/>
-      <c r="AP10" s="39"/>
-      <c r="AQ10" s="42"/>
-      <c r="AR10" s="42"/>
-      <c r="AS10" s="39"/>
-      <c r="AT10" s="39"/>
-      <c r="AU10" s="39"/>
-      <c r="AV10" s="39"/>
-      <c r="AW10" s="37"/>
-      <c r="AX10" s="37"/>
-      <c r="AY10" s="37"/>
-      <c r="AZ10" s="37"/>
-      <c r="BA10" s="37"/>
-      <c r="BB10" s="37"/>
-      <c r="BC10" s="37"/>
-      <c r="BD10" s="37"/>
-      <c r="BE10" s="44"/>
-      <c r="BF10" s="37"/>
-      <c r="BG10" s="37"/>
-      <c r="BH10" s="37"/>
-      <c r="BI10" s="37"/>
-      <c r="BJ10" s="37"/>
-      <c r="BK10" s="37"/>
+      <c r="AN10" s="40"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="40"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="40"/>
+      <c r="AT10" s="40"/>
+      <c r="AU10" s="40"/>
+      <c r="AV10" s="40"/>
+      <c r="AW10" s="38"/>
+      <c r="AX10" s="38"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="38"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="38"/>
+      <c r="BC10" s="38"/>
+      <c r="BD10" s="38"/>
+      <c r="BE10" s="45"/>
+      <c r="BF10" s="38"/>
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="38"/>
+      <c r="BI10" s="38"/>
+      <c r="BJ10" s="38"/>
+      <c r="BK10" s="38"/>
       <c r="BL10" s="24" t="s">
         <v>56</v>
       </c>
       <c r="BM10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="BN10" s="45"/>
-      <c r="BO10" s="37"/>
+      <c r="BN10" s="46"/>
+      <c r="BO10" s="38"/>
       <c r="BP10" s="11" t="s">
         <v>26</v>
       </c>
@@ -1630,7 +1596,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>63</v>
       </c>
@@ -1803,7 +1769,7 @@
         <v>114</v>
       </c>
       <c r="BE11" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BF11" s="34" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
@@ -1836,7 +1802,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="BN11" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BO11" s="36" t="e">
         <f>BM11/BL11</f>
@@ -1867,7 +1833,7 @@
       <c r="BW11" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="BX11" s="53" t="s">
+      <c r="BX11" s="37" t="s">
         <v>125</v>
       </c>
       <c r="BY11" s="13"/>

</xml_diff>

<commit_message>
KIBON-217: merging dev into feature
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="20565" tabRatio="606"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="29040" windowHeight="16440" tabRatio="606"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -83,9 +78,6 @@
     <t>Geburtsdatum</t>
   </si>
   <si>
-    <t>Behinderung</t>
-  </si>
-  <si>
     <t>Baby-Faktor</t>
   </si>
   <si>
@@ -429,6 +421,9 @@
   </si>
   <si>
     <t>Schulstufe</t>
+  </si>
+  <si>
+    <t>Besondere Bedürfnisse</t>
   </si>
 </sst>
 </file>
@@ -667,14 +662,35 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -692,27 +708,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -801,9 +796,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -841,9 +836,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -878,7 +873,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,7 +908,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1093,7 +1088,7 @@
   <dimension ref="A1:BY11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BE9" sqref="BE9:BE10"/>
+      <selection activeCell="BD5" sqref="BD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1112,8 @@
     <col min="49" max="49" width="10.42578125"/>
     <col min="50" max="52" width="12.7109375"/>
     <col min="53" max="53" width="16.7109375"/>
-    <col min="54" max="55" width="12.7109375"/>
+    <col min="54" max="54" width="12.7109375"/>
+    <col min="55" max="55" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="22"/>
     <col min="57" max="57" width="18.140625" customWidth="1"/>
     <col min="58" max="61" width="22"/>
@@ -1136,7 +1132,7 @@
   <sheetData>
     <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1167,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1176,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5"/>
     </row>
@@ -1185,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
@@ -1196,88 +1192,88 @@
       <c r="C7"/>
     </row>
     <row r="8" spans="1:77" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="40"/>
+      <c r="Z8" s="40"/>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="40"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="40"/>
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="41"/>
+      <c r="AH8" s="41"/>
+      <c r="AI8" s="41"/>
+      <c r="AJ8" s="41"/>
+      <c r="AK8" s="41"/>
+      <c r="AL8" s="41"/>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38"/>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="38"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
-      <c r="AM8" s="51"/>
-      <c r="AN8" s="40" t="s">
+      <c r="AO8" s="42"/>
+      <c r="AP8" s="42"/>
+      <c r="AQ8" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="40"/>
-      <c r="AP8" s="40"/>
-      <c r="AQ8" s="40" t="s">
+      <c r="AR8" s="42"/>
+      <c r="AS8" s="42"/>
+      <c r="AT8" s="42"/>
+      <c r="AU8" s="42"/>
+      <c r="AV8" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="40"/>
-      <c r="AS8" s="40"/>
-      <c r="AT8" s="40"/>
-      <c r="AU8" s="40"/>
-      <c r="AV8" s="40" t="s">
+      <c r="AW8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX8" s="38" t="s">
+      <c r="AX8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="38"/>
-      <c r="AZ8" s="38"/>
-      <c r="BA8" s="38"/>
-      <c r="BB8" s="38"/>
+      <c r="AY8" s="40"/>
+      <c r="AZ8" s="40"/>
+      <c r="BA8" s="40"/>
+      <c r="BB8" s="40"/>
       <c r="BC8" s="10"/>
       <c r="BD8" s="10"/>
       <c r="BE8" s="26"/>
@@ -1285,491 +1281,491 @@
       <c r="BG8" s="10"/>
       <c r="BH8" s="10"/>
       <c r="BI8" s="10"/>
-      <c r="BJ8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="BK8" s="38"/>
-      <c r="BL8" s="38"/>
-      <c r="BM8" s="38"/>
-      <c r="BN8" s="38"/>
-      <c r="BO8" s="38"/>
-      <c r="BP8" s="38"/>
-      <c r="BQ8" s="38"/>
-      <c r="BR8" s="38"/>
-      <c r="BS8" s="38"/>
-      <c r="BT8" s="38"/>
-      <c r="BU8" s="38"/>
-      <c r="BV8" s="38"/>
-      <c r="BW8" s="38"/>
+      <c r="BJ8" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="BK8" s="40"/>
+      <c r="BL8" s="40"/>
+      <c r="BM8" s="40"/>
+      <c r="BN8" s="40"/>
+      <c r="BO8" s="40"/>
+      <c r="BP8" s="40"/>
+      <c r="BQ8" s="40"/>
+      <c r="BR8" s="40"/>
+      <c r="BS8" s="40"/>
+      <c r="BT8" s="40"/>
+      <c r="BU8" s="40"/>
+      <c r="BV8" s="40"/>
+      <c r="BW8" s="40"/>
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="38" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="L9" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="M9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="N9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="O9" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="38" t="s">
+      <c r="P9" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="47" t="s">
+      <c r="Q9" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="47" t="s">
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y9" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z9" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB9" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH9" s="44"/>
+      <c r="AI9" s="44"/>
+      <c r="AJ9" s="44"/>
+      <c r="AK9" s="44"/>
+      <c r="AL9" s="44"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="52" t="s">
+      <c r="AO9" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP9" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ9" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="AR9" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS9" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT9" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU9" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV9" s="42"/>
+      <c r="AW9" s="40"/>
+      <c r="AX9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="38" t="s">
+      <c r="AY9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA9" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB9" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC9" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD9" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE9" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF9" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG9" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="48"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO9" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP9" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ9" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR9" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="AS9" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT9" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU9" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV9" s="40"/>
-      <c r="AW9" s="38"/>
-      <c r="AX9" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY9" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="AZ9" s="38" t="s">
+      <c r="AZ9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="BA9" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="BB9" s="38" t="s">
+      <c r="BA9" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC9" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="BD9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD9" s="38" t="s">
+      <c r="BE9" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="BF9" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="BF9" s="38" t="s">
+      <c r="BG9" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="38" t="s">
+      <c r="BH9" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="38" t="s">
+      <c r="BI9" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="BJ9" s="38" t="s">
+      <c r="BJ9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="38" t="s">
+      <c r="BK9" s="40" t="s">
         <v>5</v>
       </c>
       <c r="BL9" s="24"/>
       <c r="BM9" s="24"/>
-      <c r="BN9" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="BO9" s="38" t="s">
+      <c r="BN9" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="BO9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="BP9" s="38" t="s">
+      <c r="BP9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="BQ9" s="38"/>
-      <c r="BR9" s="38"/>
-      <c r="BS9" s="38"/>
-      <c r="BT9" s="38"/>
-      <c r="BU9" s="38" t="s">
+      <c r="BQ9" s="40"/>
+      <c r="BR9" s="40"/>
+      <c r="BS9" s="40"/>
+      <c r="BT9" s="40"/>
+      <c r="BU9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="BV9" s="38"/>
-      <c r="BW9" s="38"/>
+      <c r="BV9" s="40"/>
+      <c r="BW9" s="40"/>
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
       <c r="Q10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="R10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="S10" s="17" t="s">
+      <c r="T10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="T10" s="17" t="s">
+      <c r="U10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="U10" s="17" t="s">
+      <c r="V10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="V10" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="W10" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
+        <v>83</v>
+      </c>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="40"/>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="40"/>
+      <c r="AC10" s="40"/>
+      <c r="AD10" s="40"/>
+      <c r="AE10" s="40"/>
+      <c r="AF10" s="40"/>
       <c r="AG10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="AH10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AI10" s="17" t="s">
+      <c r="AJ10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AJ10" s="17" t="s">
+      <c r="AK10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="AK10" s="17" t="s">
+      <c r="AL10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="AL10" s="17" t="s">
+      <c r="AM10" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN10" s="42"/>
+      <c r="AO10" s="50"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="50"/>
+      <c r="AR10" s="50"/>
+      <c r="AS10" s="42"/>
+      <c r="AT10" s="42"/>
+      <c r="AU10" s="42"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="40"/>
+      <c r="AX10" s="40"/>
+      <c r="AY10" s="40"/>
+      <c r="AZ10" s="40"/>
+      <c r="BA10" s="40"/>
+      <c r="BB10" s="40"/>
+      <c r="BC10" s="40"/>
+      <c r="BD10" s="40"/>
+      <c r="BE10" s="52"/>
+      <c r="BF10" s="40"/>
+      <c r="BG10" s="40"/>
+      <c r="BH10" s="40"/>
+      <c r="BI10" s="40"/>
+      <c r="BJ10" s="40"/>
+      <c r="BK10" s="40"/>
+      <c r="BL10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AM10" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="AN10" s="40"/>
-      <c r="AO10" s="43"/>
-      <c r="AP10" s="40"/>
-      <c r="AQ10" s="43"/>
-      <c r="AR10" s="43"/>
-      <c r="AS10" s="40"/>
-      <c r="AT10" s="40"/>
-      <c r="AU10" s="40"/>
-      <c r="AV10" s="40"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="38"/>
-      <c r="BA10" s="38"/>
-      <c r="BB10" s="38"/>
-      <c r="BC10" s="38"/>
-      <c r="BD10" s="38"/>
-      <c r="BE10" s="45"/>
-      <c r="BF10" s="38"/>
-      <c r="BG10" s="38"/>
-      <c r="BH10" s="38"/>
-      <c r="BI10" s="38"/>
-      <c r="BJ10" s="38"/>
-      <c r="BK10" s="38"/>
-      <c r="BL10" s="24" t="s">
+      <c r="BM10" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="BM10" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="BN10" s="46"/>
-      <c r="BO10" s="38"/>
+      <c r="BN10" s="53"/>
+      <c r="BO10" s="40"/>
       <c r="BP10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BQ10" s="11" t="s">
+      <c r="BR10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="BR10" s="11" t="s">
+      <c r="BS10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="BS10" s="11" t="s">
+      <c r="BT10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BT10" s="11" t="s">
+      <c r="BU10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BU10" s="11" t="s">
+      <c r="BV10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="BV10" s="11" t="s">
+      <c r="BW10" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="BW10" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="F11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="O11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="P11" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="Q11" s="32" t="e">
         <f>R11+S11+T11+U11+V11+W11</f>
         <v>#VALUE!</v>
       </c>
       <c r="R11" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="S11" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="S11" s="28" t="s">
+      <c r="T11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="T11" s="28" t="s">
+      <c r="U11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="U11" s="28" t="s">
+      <c r="V11" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="V11" s="28" t="s">
+      <c r="W11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="W11" s="28" t="s">
-        <v>83</v>
-      </c>
       <c r="X11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="Z11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z11" s="16" t="s">
+      <c r="AA11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AA11" s="16" t="s">
+      <c r="AB11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AB11" s="16" t="s">
+      <c r="AC11" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AC11" s="16" t="s">
+      <c r="AD11" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AD11" s="16" t="s">
+      <c r="AE11" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="AE11" s="16" t="s">
+      <c r="AF11" s="16" t="s">
         <v>92</v>
-      </c>
-      <c r="AF11" s="16" t="s">
-        <v>93</v>
       </c>
       <c r="AG11" s="33" t="e">
         <f>IF((AH11+AI11+AJ11+AK11+AL11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AM11,)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AH11" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI11" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="AI11" s="28" t="s">
+      <c r="AJ11" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="AJ11" s="28" t="s">
+      <c r="AK11" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AK11" s="28" t="s">
+      <c r="AL11" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="AL11" s="28" t="s">
+      <c r="AM11" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="AM11" s="28" t="s">
+      <c r="AN11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="AN11" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="AO11" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AP11" s="16" t="s">
+      <c r="AQ11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR11" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS11" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="AT11" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="AQ11" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR11" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS11" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="AT11" s="16" t="s">
-        <v>104</v>
-      </c>
       <c r="AU11" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV11" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="AV11" s="16" t="s">
+      <c r="AW11" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AW11" s="16" t="s">
+      <c r="AX11" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="AX11" s="20" t="s">
+      <c r="AY11" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="AY11" s="20" t="s">
+      <c r="AZ11" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AZ11" s="21" t="s">
+      <c r="BA11" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="BA11" s="20" t="s">
-        <v>112</v>
       </c>
       <c r="BB11" s="34" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BC11" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BD11" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="BE11" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="BF11" s="34" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
@@ -1788,10 +1784,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="BJ11" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK11" s="21" t="s">
         <v>116</v>
-      </c>
-      <c r="BK11" s="21" t="s">
-        <v>117</v>
       </c>
       <c r="BL11" s="30" t="e">
         <f>NETWORKDAYS((BJ11-DAY(BJ11)+1),(EOMONTH(BJ11,0)))</f>
@@ -1802,49 +1798,84 @@
         <v>#VALUE!</v>
       </c>
       <c r="BN11" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BO11" s="36" t="e">
         <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
       <c r="BP11" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ11" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="BQ11" s="31" t="s">
+      <c r="BR11" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="BR11" s="31" t="s">
+      <c r="BS11" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="BS11" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="BT11" s="36" t="e">
         <f>BR11*BO11</f>
         <v>#VALUE!</v>
       </c>
       <c r="BU11" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="BV11" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BV11" s="22" t="s">
+      <c r="BW11" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="BW11" s="23" t="s">
+      <c r="BX11" s="37" t="s">
         <v>124</v>
-      </c>
-      <c r="BX11" s="37" t="s">
-        <v>125</v>
       </c>
       <c r="BY11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AL9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AV10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BJ8:BW8"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BU9:BW9"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="H8:W8"/>
@@ -1861,46 +1892,11 @@
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:V9"/>
     <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AV10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BJ8:BW8"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BU9:BW9"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AL9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-324: Frage "Wird in Ihrer Familie Deutsch gesprochen?" umformulieren
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81430AD-C9C4-4634-9E01-97BE6340A59C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD99D29-E243-406F-8CF4-C28C6C4C1E9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="29040" windowHeight="16440" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Baby-Faktor</t>
   </si>
   <si>
-    <t>Muttersprache Deutsch</t>
-  </si>
-  <si>
     <t>Bis 12 Monate</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t>Fachstelle</t>
   </si>
   <si>
-    <t>{kindDeutsch}</t>
-  </si>
-  <si>
     <t>{kindErwBeduerfnisse}</t>
   </si>
   <si>
@@ -426,6 +420,12 @@
   </si>
   <si>
     <t>Besondere Bedürfnisse</t>
+  </si>
+  <si>
+    <t>SprichtAmtssprache</t>
+  </si>
+  <si>
+    <t>{kindSprichtAmtssprache}</t>
   </si>
 </sst>
 </file>
@@ -664,52 +664,52 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1123,8 +1123,8 @@
   </sheetPr>
   <dimension ref="A1:BW11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1199,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1208,7 +1208,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5"/>
     </row>
@@ -1217,7 +1217,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
@@ -1228,86 +1228,86 @@
       <c r="C7"/>
     </row>
     <row r="8" spans="1:75" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="X8" s="40"/>
-      <c r="Y8" s="40"/>
-      <c r="Z8" s="40"/>
-      <c r="AA8" s="40"/>
-      <c r="AB8" s="40"/>
-      <c r="AC8" s="40"/>
-      <c r="AD8" s="40"/>
-      <c r="AE8" s="40"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="41"/>
-      <c r="AH8" s="41"/>
-      <c r="AI8" s="41"/>
-      <c r="AJ8" s="41"/>
-      <c r="AK8" s="41"/>
-      <c r="AL8" s="42" t="s">
+      <c r="AM8" s="40"/>
+      <c r="AN8" s="40"/>
+      <c r="AO8" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AM8" s="42"/>
-      <c r="AN8" s="42"/>
-      <c r="AO8" s="42" t="s">
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40"/>
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="40"/>
+      <c r="AT8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AP8" s="42"/>
-      <c r="AQ8" s="42"/>
-      <c r="AR8" s="42"/>
-      <c r="AS8" s="42"/>
-      <c r="AT8" s="42" t="s">
+      <c r="AU8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="AU8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="AV8" s="40" t="s">
+      <c r="AV8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="AW8" s="40"/>
-      <c r="AX8" s="40"/>
-      <c r="AY8" s="40"/>
-      <c r="AZ8" s="40"/>
+      <c r="AW8" s="38"/>
+      <c r="AX8" s="38"/>
+      <c r="AY8" s="38"/>
+      <c r="AZ8" s="38"/>
       <c r="BA8" s="10"/>
       <c r="BB8" s="10"/>
       <c r="BC8" s="26"/>
@@ -1315,477 +1315,477 @@
       <c r="BE8" s="10"/>
       <c r="BF8" s="10"/>
       <c r="BG8" s="10"/>
-      <c r="BH8" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="BI8" s="40"/>
-      <c r="BJ8" s="40"/>
-      <c r="BK8" s="40"/>
-      <c r="BL8" s="40"/>
-      <c r="BM8" s="40"/>
-      <c r="BN8" s="40"/>
-      <c r="BO8" s="40"/>
-      <c r="BP8" s="40"/>
-      <c r="BQ8" s="40"/>
-      <c r="BR8" s="40"/>
-      <c r="BS8" s="40"/>
-      <c r="BT8" s="40"/>
-      <c r="BU8" s="40"/>
+      <c r="BH8" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="BI8" s="38"/>
+      <c r="BJ8" s="38"/>
+      <c r="BK8" s="38"/>
+      <c r="BL8" s="38"/>
+      <c r="BM8" s="38"/>
+      <c r="BN8" s="38"/>
+      <c r="BO8" s="38"/>
+      <c r="BP8" s="38"/>
+      <c r="BQ8" s="38"/>
+      <c r="BR8" s="38"/>
+      <c r="BS8" s="38"/>
+      <c r="BT8" s="38"/>
+      <c r="BU8" s="38"/>
     </row>
     <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="40" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="L9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="M9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="40" t="s">
+      <c r="N9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="40" t="s">
+      <c r="O9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="40" t="s">
+      <c r="P9" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="43" t="s">
+      <c r="Q9" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="Q9" s="43" t="s">
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="X9" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB9" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="48"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="48"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="45" t="s">
+      <c r="AM9" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN9" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO9" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP9" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ9" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR9" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS9" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT9" s="40"/>
+      <c r="AU9" s="38"/>
+      <c r="AV9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="40" t="s">
+      <c r="AW9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z9" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA9" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB9" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC9" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD9" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE9" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF9" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG9" s="44"/>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="44"/>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM9" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN9" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO9" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="AP9" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="AQ9" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR9" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS9" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT9" s="42"/>
-      <c r="AU9" s="40"/>
-      <c r="AV9" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW9" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX9" s="40" t="s">
+      <c r="AX9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="AY9" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ9" s="40" t="s">
+      <c r="AY9" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="AZ9" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="BA9" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="BB9" s="40" t="s">
+      <c r="BA9" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB9" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="BC9" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="BD9" s="40" t="s">
+      <c r="BE9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="40" t="s">
+      <c r="BF9" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BF9" s="40" t="s">
+      <c r="BG9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="BG9" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="BH9" s="40" t="s">
+      <c r="BH9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="BI9" s="40" t="s">
+      <c r="BI9" s="38" t="s">
         <v>5</v>
       </c>
       <c r="BJ9" s="24"/>
       <c r="BK9" s="24"/>
-      <c r="BL9" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="BM9" s="40" t="s">
+      <c r="BL9" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="BM9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="BN9" s="40" t="s">
+      <c r="BN9" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="BO9" s="40"/>
-      <c r="BP9" s="40"/>
-      <c r="BQ9" s="40"/>
-      <c r="BR9" s="40"/>
-      <c r="BS9" s="40" t="s">
+      <c r="BO9" s="38"/>
+      <c r="BP9" s="38"/>
+      <c r="BQ9" s="38"/>
+      <c r="BR9" s="38"/>
+      <c r="BS9" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="BT9" s="40"/>
-      <c r="BU9" s="40"/>
+      <c r="BT9" s="38"/>
+      <c r="BU9" s="38"/>
     </row>
     <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
       <c r="Q10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="R10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="S10" s="17" t="s">
+      <c r="T10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="T10" s="17" t="s">
+      <c r="U10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="U10" s="17" t="s">
-        <v>53</v>
-      </c>
       <c r="V10" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="40"/>
-      <c r="AA10" s="40"/>
-      <c r="AB10" s="40"/>
-      <c r="AC10" s="40"/>
-      <c r="AD10" s="40"/>
-      <c r="AE10" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
       <c r="AF10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="AG10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH10" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AH10" s="17" t="s">
+      <c r="AI10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AI10" s="17" t="s">
+      <c r="AJ10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AJ10" s="17" t="s">
+      <c r="AK10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL10" s="40"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="40"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="40"/>
+      <c r="AR10" s="40"/>
+      <c r="AS10" s="40"/>
+      <c r="AT10" s="40"/>
+      <c r="AU10" s="38"/>
+      <c r="AV10" s="38"/>
+      <c r="AW10" s="38"/>
+      <c r="AX10" s="38"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="38"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="38"/>
+      <c r="BC10" s="45"/>
+      <c r="BD10" s="38"/>
+      <c r="BE10" s="38"/>
+      <c r="BF10" s="38"/>
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="38"/>
+      <c r="BI10" s="38"/>
+      <c r="BJ10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="AK10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL10" s="42"/>
-      <c r="AM10" s="50"/>
-      <c r="AN10" s="42"/>
-      <c r="AO10" s="50"/>
-      <c r="AP10" s="50"/>
-      <c r="AQ10" s="42"/>
-      <c r="AR10" s="42"/>
-      <c r="AS10" s="42"/>
-      <c r="AT10" s="42"/>
-      <c r="AU10" s="40"/>
-      <c r="AV10" s="40"/>
-      <c r="AW10" s="40"/>
-      <c r="AX10" s="40"/>
-      <c r="AY10" s="40"/>
-      <c r="AZ10" s="40"/>
-      <c r="BA10" s="40"/>
-      <c r="BB10" s="40"/>
-      <c r="BC10" s="52"/>
-      <c r="BD10" s="40"/>
-      <c r="BE10" s="40"/>
-      <c r="BF10" s="40"/>
-      <c r="BG10" s="40"/>
-      <c r="BH10" s="40"/>
-      <c r="BI10" s="40"/>
-      <c r="BJ10" s="24" t="s">
+      <c r="BK10" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="BK10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="BL10" s="53"/>
-      <c r="BM10" s="40"/>
+      <c r="BL10" s="46"/>
+      <c r="BM10" s="38"/>
       <c r="BN10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="BO10" s="11" t="s">
+      <c r="BP10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BP10" s="11" t="s">
+      <c r="BQ10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="BQ10" s="11" t="s">
+      <c r="BR10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="BR10" s="11" t="s">
+      <c r="BS10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BS10" s="11" t="s">
+      <c r="BT10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BT10" s="11" t="s">
+      <c r="BU10" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="BU10" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="F11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="O11" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="P11" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>75</v>
       </c>
       <c r="Q11" s="32" t="e">
         <f>R11+S11+T11+U11+V11</f>
         <v>#VALUE!</v>
       </c>
       <c r="R11" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="S11" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="S11" s="28" t="s">
+      <c r="T11" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="T11" s="28" t="s">
+      <c r="U11" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="U11" s="28" t="s">
+      <c r="V11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="V11" s="28" t="s">
-        <v>80</v>
-      </c>
       <c r="W11" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="X11" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="X11" s="16" t="s">
+      <c r="Y11" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="Z11" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="Z11" s="16" t="s">
+      <c r="AA11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="AA11" s="16" t="s">
+      <c r="AB11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="AB11" s="16" t="s">
+      <c r="AC11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AC11" s="16" t="s">
+      <c r="AD11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AD11" s="16" t="s">
+      <c r="AE11" s="16" t="s">
         <v>89</v>
-      </c>
-      <c r="AE11" s="16" t="s">
-        <v>90</v>
       </c>
       <c r="AF11" s="33" t="e">
         <f>IF((AG11+AH11+AI11+AJ11+AK11)&gt;0,AG11+AH11+AI11+AJ11+AK11,)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AG11" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH11" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="AH11" s="28" t="s">
+      <c r="AI11" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="AI11" s="28" t="s">
+      <c r="AJ11" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="AJ11" s="28" t="s">
+      <c r="AK11" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="AK11" s="28" t="s">
+      <c r="AL11" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="AL11" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="AM11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN11" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="AN11" s="16" t="s">
+      <c r="AO11" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP11" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="AQ11" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="AR11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="AO11" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="AP11" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR11" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="AS11" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AT11" s="16" t="s">
+      <c r="AU11" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="AU11" s="16" t="s">
+      <c r="AV11" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="AV11" s="20" t="s">
+      <c r="AW11" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="AW11" s="20" t="s">
+      <c r="AX11" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AX11" s="21" t="s">
+      <c r="AY11" s="20" t="s">
         <v>107</v>
-      </c>
-      <c r="AY11" s="20" t="s">
-        <v>108</v>
       </c>
       <c r="AZ11" s="34" t="e">
         <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA11" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="BB11" s="20" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="BC11" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BD11" s="34" t="e">
         <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
@@ -1804,10 +1804,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="BH11" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="BI11" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BJ11" s="30" t="e">
         <f>NETWORKDAYS((BH11-DAY(BH11)+1),(EOMONTH(BH11,0)))</f>
@@ -1818,68 +1818,65 @@
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="BM11" s="36" t="e">
         <f>BK11/BJ11</f>
         <v>#VALUE!</v>
       </c>
       <c r="BN11" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="BO11" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="BP11" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="BO11" s="31" t="s">
+      <c r="BQ11" s="22" t="s">
         <v>115</v>
-      </c>
-      <c r="BP11" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="BQ11" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="BR11" s="36" t="e">
         <f>BP11*BM11</f>
         <v>#VALUE!</v>
       </c>
       <c r="BS11" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT11" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU11" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="BT11" s="22" t="s">
+      <c r="BV11" s="37" t="s">
         <v>119</v>
-      </c>
-      <c r="BU11" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="BV11" s="37" t="s">
-        <v>121</v>
       </c>
       <c r="BW11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="BN9:BR9"/>
-    <mergeCell ref="AL9:AL10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:V8"/>
+    <mergeCell ref="W8:AK8"/>
+    <mergeCell ref="AL8:AN8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="W9:W10"/>
     <mergeCell ref="AO8:AS8"/>
     <mergeCell ref="AT8:AT10"/>
     <mergeCell ref="AU8:AU10"/>
@@ -1896,27 +1893,30 @@
     <mergeCell ref="BE9:BE10"/>
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BS9:BU9"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:V8"/>
-    <mergeCell ref="W8:AK8"/>
-    <mergeCell ref="AL8:AN8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="BN9:BR9"/>
+    <mergeCell ref="AL9:AL10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BL9:BL10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1141: Nettoarbeitstage mit Tage ersetzen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F2E687-0360-4028-8CF7-18BBF00CDFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD54B88F-456D-4935-94DA-DF12BC1FA7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -666,18 +666,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -694,24 +712,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1128,54 +1128,54 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.7109375"/>
-    <col min="17" max="18" width="10.7109375"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="41.42578125" customWidth="1"/>
-    <col min="23" max="23" width="24.140625"/>
-    <col min="24" max="31" width="8.7109375"/>
-    <col min="32" max="33" width="10.7109375"/>
-    <col min="34" max="34" width="24.5703125" customWidth="1"/>
-    <col min="35" max="35" width="10.7109375"/>
-    <col min="36" max="36" width="14.42578125" customWidth="1"/>
-    <col min="37" max="37" width="41.42578125" customWidth="1"/>
-    <col min="38" max="38" width="24.140625"/>
-    <col min="39" max="39" width="9.140625" customWidth="1"/>
-    <col min="40" max="40" width="6.42578125"/>
-    <col min="41" max="41" width="18.140625"/>
-    <col min="43" max="43" width="23.28515625"/>
-    <col min="44" max="44" width="9.28515625"/>
-    <col min="45" max="45" width="25.42578125"/>
-    <col min="46" max="46" width="27.42578125"/>
-    <col min="47" max="47" width="10.42578125"/>
-    <col min="48" max="50" width="12.7109375"/>
-    <col min="51" max="51" width="16.7109375"/>
-    <col min="52" max="52" width="12.7109375"/>
-    <col min="53" max="53" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="8.6640625"/>
+    <col min="17" max="18" width="10.6640625"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625"/>
+    <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="22" max="22" width="41.44140625" customWidth="1"/>
+    <col min="23" max="23" width="24.109375"/>
+    <col min="24" max="31" width="8.6640625"/>
+    <col min="32" max="33" width="10.6640625"/>
+    <col min="34" max="34" width="24.5546875" customWidth="1"/>
+    <col min="35" max="35" width="10.6640625"/>
+    <col min="36" max="36" width="14.44140625" customWidth="1"/>
+    <col min="37" max="37" width="41.44140625" customWidth="1"/>
+    <col min="38" max="38" width="24.109375"/>
+    <col min="39" max="39" width="9.109375" customWidth="1"/>
+    <col min="40" max="40" width="6.44140625"/>
+    <col min="41" max="41" width="18.109375"/>
+    <col min="43" max="43" width="23.33203125"/>
+    <col min="44" max="44" width="9.33203125"/>
+    <col min="45" max="45" width="25.44140625"/>
+    <col min="46" max="46" width="27.44140625"/>
+    <col min="47" max="47" width="10.44140625"/>
+    <col min="48" max="50" width="12.6640625"/>
+    <col min="51" max="51" width="16.6640625"/>
+    <col min="52" max="52" width="12.6640625"/>
+    <col min="53" max="53" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="22"/>
-    <col min="55" max="55" width="18.140625" customWidth="1"/>
+    <col min="55" max="55" width="18.109375" customWidth="1"/>
     <col min="56" max="59" width="22"/>
-    <col min="60" max="61" width="12.7109375"/>
-    <col min="62" max="62" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="60" max="61" width="12.6640625"/>
+    <col min="62" max="62" width="11.33203125" hidden="1" customWidth="1"/>
     <col min="63" max="63" width="16" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="16" customWidth="1"/>
-    <col min="65" max="66" width="12.7109375"/>
-    <col min="67" max="67" width="16.85546875"/>
-    <col min="68" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="19.42578125"/>
-    <col min="70" max="70" width="16.85546875"/>
-    <col min="71" max="73" width="12.7109375"/>
-    <col min="74" max="994" width="10.42578125"/>
+    <col min="65" max="66" width="12.6640625"/>
+    <col min="67" max="67" width="16.88671875"/>
+    <col min="68" max="68" width="12.6640625"/>
+    <col min="69" max="69" width="19.44140625"/>
+    <col min="70" max="70" width="16.88671875"/>
+    <col min="71" max="73" width="12.6640625"/>
+    <col min="74" max="994" width="10.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1187,10 +1187,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>68</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="BK3" s="30"/>
       <c r="BL3" s="30"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -1236,294 +1236,294 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:75" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:75" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="37" t="s">
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
-      <c r="AA8" s="37"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
-      <c r="AM8" s="39" t="s">
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="41"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="42"/>
+      <c r="AH8" s="42"/>
+      <c r="AI8" s="42"/>
+      <c r="AJ8" s="42"/>
+      <c r="AK8" s="42"/>
+      <c r="AL8" s="42"/>
+      <c r="AM8" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="39" t="s">
+      <c r="AN8" s="43"/>
+      <c r="AO8" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39"/>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39"/>
-      <c r="AT8" s="39" t="s">
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="43"/>
+      <c r="AS8" s="43"/>
+      <c r="AT8" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="AU8" s="37" t="s">
+      <c r="AU8" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="AV8" s="46" t="s">
+      <c r="AV8" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="AW8" s="47"/>
-      <c r="AX8" s="47"/>
-      <c r="AY8" s="47"/>
-      <c r="AZ8" s="47"/>
-      <c r="BA8" s="47"/>
-      <c r="BB8" s="47"/>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="47"/>
-      <c r="BE8" s="47"/>
-      <c r="BF8" s="47"/>
-      <c r="BG8" s="49"/>
-      <c r="BH8" s="37" t="s">
+      <c r="AW8" s="37"/>
+      <c r="AX8" s="37"/>
+      <c r="AY8" s="37"/>
+      <c r="AZ8" s="37"/>
+      <c r="BA8" s="37"/>
+      <c r="BB8" s="37"/>
+      <c r="BC8" s="37"/>
+      <c r="BD8" s="37"/>
+      <c r="BE8" s="37"/>
+      <c r="BF8" s="37"/>
+      <c r="BG8" s="38"/>
+      <c r="BH8" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="BI8" s="37"/>
-      <c r="BJ8" s="37"/>
-      <c r="BK8" s="37"/>
-      <c r="BL8" s="37"/>
-      <c r="BM8" s="37"/>
-      <c r="BN8" s="37"/>
-      <c r="BO8" s="37"/>
-      <c r="BP8" s="37"/>
-      <c r="BQ8" s="37"/>
-      <c r="BR8" s="37"/>
-      <c r="BS8" s="37"/>
-      <c r="BT8" s="37"/>
-      <c r="BU8" s="37"/>
+      <c r="BI8" s="41"/>
+      <c r="BJ8" s="41"/>
+      <c r="BK8" s="41"/>
+      <c r="BL8" s="41"/>
+      <c r="BM8" s="41"/>
+      <c r="BN8" s="41"/>
+      <c r="BO8" s="41"/>
+      <c r="BP8" s="41"/>
+      <c r="BQ8" s="41"/>
+      <c r="BR8" s="41"/>
+      <c r="BS8" s="41"/>
+      <c r="BT8" s="41"/>
+      <c r="BU8" s="41"/>
     </row>
-    <row r="9" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37" t="s">
+    <row r="9" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="O9" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
       <c r="V9" s="33"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="37" t="s">
+      <c r="X9" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="Y9" s="37" t="s">
+      <c r="Y9" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="Z9" s="37" t="s">
+      <c r="Z9" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="AA9" s="37" t="s">
+      <c r="AA9" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="AB9" s="37" t="s">
+      <c r="AB9" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="AC9" s="37" t="s">
+      <c r="AC9" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="AD9" s="37" t="s">
+      <c r="AD9" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="AE9" s="46" t="s">
+      <c r="AE9" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="AF9" s="46" t="s">
+      <c r="AF9" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="AG9" s="47"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="37"/>
+      <c r="AJ9" s="37"/>
       <c r="AK9" s="33"/>
       <c r="AL9" s="13"/>
-      <c r="AM9" s="38" t="s">
+      <c r="AM9" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="AN9" s="39" t="s">
+      <c r="AN9" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="AO9" s="41" t="s">
+      <c r="AO9" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="AP9" s="41" t="s">
+      <c r="AP9" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="AQ9" s="39" t="s">
+      <c r="AQ9" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="AR9" s="40" t="s">
+      <c r="AR9" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="AS9" s="39" t="s">
+      <c r="AS9" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="AT9" s="39"/>
-      <c r="AU9" s="37"/>
-      <c r="AV9" s="37" t="s">
+      <c r="AT9" s="43"/>
+      <c r="AU9" s="41"/>
+      <c r="AV9" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="AW9" s="37" t="s">
+      <c r="AW9" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AX9" s="37" t="s">
+      <c r="AX9" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="AY9" s="48" t="s">
+      <c r="AY9" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="AZ9" s="37" t="s">
+      <c r="AZ9" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="BA9" s="37" t="s">
+      <c r="BA9" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="BB9" s="37" t="s">
+      <c r="BB9" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="BC9" s="43" t="s">
+      <c r="BC9" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="BD9" s="37" t="s">
+      <c r="BD9" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="BE9" s="37" t="s">
+      <c r="BE9" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="BF9" s="37" t="s">
+      <c r="BF9" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="BG9" s="37" t="s">
+      <c r="BG9" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="BH9" s="37" t="s">
+      <c r="BH9" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="BI9" s="37" t="s">
+      <c r="BI9" s="41" t="s">
         <v>120</v>
       </c>
       <c r="BJ9" s="34"/>
       <c r="BK9" s="34"/>
-      <c r="BL9" s="43" t="s">
+      <c r="BL9" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="BM9" s="37" t="s">
+      <c r="BM9" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="BN9" s="37" t="s">
+      <c r="BN9" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="BO9" s="37"/>
-      <c r="BP9" s="37"/>
-      <c r="BQ9" s="37"/>
-      <c r="BR9" s="37"/>
-      <c r="BS9" s="37" t="s">
+      <c r="BO9" s="41"/>
+      <c r="BP9" s="41"/>
+      <c r="BQ9" s="41"/>
+      <c r="BR9" s="41"/>
+      <c r="BS9" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="BT9" s="37"/>
-      <c r="BU9" s="37"/>
+      <c r="BT9" s="41"/>
+      <c r="BU9" s="41"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
       <c r="Q10" s="16" t="s">
         <v>88</v>
       </c>
@@ -1545,14 +1545,14 @@
       <c r="W10" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="37"/>
-      <c r="AD10" s="37"/>
-      <c r="AE10" s="37"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="41"/>
       <c r="AF10" s="16" t="s">
         <v>88</v>
       </c>
@@ -1574,37 +1574,37 @@
       <c r="AL10" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="AM10" s="39"/>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="42"/>
-      <c r="AP10" s="42"/>
-      <c r="AQ10" s="39"/>
-      <c r="AR10" s="39"/>
-      <c r="AS10" s="39"/>
-      <c r="AT10" s="39"/>
-      <c r="AU10" s="37"/>
-      <c r="AV10" s="37"/>
-      <c r="AW10" s="37"/>
-      <c r="AX10" s="37"/>
-      <c r="AY10" s="37"/>
-      <c r="AZ10" s="37"/>
-      <c r="BA10" s="37"/>
-      <c r="BB10" s="37"/>
-      <c r="BC10" s="44"/>
-      <c r="BD10" s="37"/>
-      <c r="BE10" s="37"/>
-      <c r="BF10" s="37"/>
-      <c r="BG10" s="37"/>
-      <c r="BH10" s="37"/>
-      <c r="BI10" s="37"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="48"/>
+      <c r="AP10" s="48"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="43"/>
+      <c r="AT10" s="43"/>
+      <c r="AU10" s="41"/>
+      <c r="AV10" s="41"/>
+      <c r="AW10" s="41"/>
+      <c r="AX10" s="41"/>
+      <c r="AY10" s="41"/>
+      <c r="AZ10" s="41"/>
+      <c r="BA10" s="41"/>
+      <c r="BB10" s="41"/>
+      <c r="BC10" s="50"/>
+      <c r="BD10" s="41"/>
+      <c r="BE10" s="41"/>
+      <c r="BF10" s="41"/>
+      <c r="BG10" s="41"/>
+      <c r="BH10" s="41"/>
+      <c r="BI10" s="41"/>
       <c r="BJ10" s="34" t="s">
         <v>0</v>
       </c>
       <c r="BK10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BL10" s="45"/>
-      <c r="BM10" s="37"/>
+      <c r="BL10" s="51"/>
+      <c r="BM10" s="41"/>
       <c r="BN10" s="10" t="s">
         <v>118</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1822,11 +1822,11 @@
         <v>50</v>
       </c>
       <c r="BJ11" s="25" t="e">
-        <f>NETWORKDAYS((BH11-DAY(BH11)+1),(EOMONTH(BH11,0)))</f>
+        <f>(EOMONTH(BH11,0))-(BH11-DAY(BH11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="BK11" s="25" t="e">
-        <f>NETWORKDAYS(BH11,BI11)</f>
+        <f>BI11-BH11+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="25" t="s">
@@ -1868,6 +1868,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="BN9:BR9"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AO8:AS8"/>
+    <mergeCell ref="AT8:AT10"/>
+    <mergeCell ref="AU8:AU10"/>
+    <mergeCell ref="BH8:BU8"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BS9:BU9"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="X9:X10"/>
     <mergeCell ref="AV8:BG8"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
@@ -1884,49 +1927,6 @@
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AO8:AS8"/>
-    <mergeCell ref="AT8:AT10"/>
-    <mergeCell ref="AU8:AU10"/>
-    <mergeCell ref="BH8:BU8"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BS9:BU9"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BN9:BR9"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="AD9:AD10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1171: Statistiken Kinder und KinderGesuchstellerBetreuung angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\TODO\KIBON-REPORTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD54B88F-456D-4935-94DA-DF12BC1FA7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CE70F7-A4DC-4146-A703-A6220A07482D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -206,9 +206,6 @@
     <t>{elternbeitrag}</t>
   </si>
   <si>
-    <t>{verguenstigt}</t>
-  </si>
-  <si>
     <t>{repeatRow}</t>
   </si>
   <si>
@@ -428,13 +425,28 @@
     <t>{elternbeitragTitle}</t>
   </si>
   <si>
-    <t>{gutscheinTitle}</t>
-  </si>
-  <si>
     <t>{gemeindeTitle}</t>
   </si>
   <si>
     <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{gutscheinKantonTitel}</t>
+  </si>
+  <si>
+    <t>{verguenstigungKanton}</t>
+  </si>
+  <si>
+    <t>{gutscheinGemeindeTitel}</t>
+  </si>
+  <si>
+    <t>{verguenstigungGemeinde}</t>
+  </si>
+  <si>
+    <t>{gutscheinTotalTitel}</t>
+  </si>
+  <si>
+    <t>{verguenstigungTotal}</t>
   </si>
 </sst>
 </file>
@@ -666,52 +678,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1124,60 +1136,63 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BW11"/>
+  <dimension ref="A1:BY11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625"/>
-    <col min="3" max="3" width="15.6640625" style="1"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.6640625"/>
-    <col min="17" max="18" width="10.6640625"/>
-    <col min="19" max="19" width="24.33203125" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
-    <col min="22" max="22" width="41.44140625" customWidth="1"/>
-    <col min="23" max="23" width="24.109375"/>
-    <col min="24" max="31" width="8.6640625"/>
-    <col min="32" max="33" width="10.6640625"/>
-    <col min="34" max="34" width="24.5546875" customWidth="1"/>
-    <col min="35" max="35" width="10.6640625"/>
-    <col min="36" max="36" width="14.44140625" customWidth="1"/>
-    <col min="37" max="37" width="41.44140625" customWidth="1"/>
-    <col min="38" max="38" width="24.109375"/>
-    <col min="39" max="39" width="9.109375" customWidth="1"/>
-    <col min="40" max="40" width="6.44140625"/>
-    <col min="41" max="41" width="18.109375"/>
-    <col min="43" max="43" width="23.33203125"/>
-    <col min="44" max="44" width="9.33203125"/>
-    <col min="45" max="45" width="25.44140625"/>
-    <col min="46" max="46" width="27.44140625"/>
-    <col min="47" max="47" width="10.44140625"/>
-    <col min="48" max="50" width="12.6640625"/>
-    <col min="51" max="51" width="16.6640625"/>
-    <col min="52" max="52" width="12.6640625"/>
-    <col min="53" max="53" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="8.7109375"/>
+    <col min="17" max="18" width="10.7109375"/>
+    <col min="19" max="19" width="24.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375"/>
+    <col min="21" max="21" width="14.42578125" customWidth="1"/>
+    <col min="22" max="22" width="41.42578125" customWidth="1"/>
+    <col min="23" max="23" width="24.140625"/>
+    <col min="24" max="31" width="8.7109375"/>
+    <col min="32" max="33" width="10.7109375"/>
+    <col min="34" max="34" width="24.5703125" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375"/>
+    <col min="36" max="36" width="14.42578125" customWidth="1"/>
+    <col min="37" max="37" width="41.42578125" customWidth="1"/>
+    <col min="38" max="38" width="24.140625"/>
+    <col min="39" max="39" width="9.140625" customWidth="1"/>
+    <col min="40" max="40" width="6.42578125"/>
+    <col min="41" max="41" width="18.140625"/>
+    <col min="43" max="43" width="23.28515625"/>
+    <col min="44" max="44" width="9.28515625"/>
+    <col min="45" max="45" width="25.42578125"/>
+    <col min="46" max="46" width="27.42578125"/>
+    <col min="47" max="47" width="10.42578125"/>
+    <col min="48" max="50" width="12.7109375"/>
+    <col min="51" max="51" width="16.7109375"/>
+    <col min="52" max="52" width="12.7109375"/>
+    <col min="53" max="53" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="22"/>
-    <col min="55" max="55" width="18.109375" customWidth="1"/>
+    <col min="55" max="55" width="18.140625" customWidth="1"/>
     <col min="56" max="59" width="22"/>
-    <col min="60" max="61" width="12.6640625"/>
-    <col min="62" max="62" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="60" max="61" width="12.7109375"/>
+    <col min="62" max="62" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="63" max="63" width="16" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="16" customWidth="1"/>
-    <col min="65" max="66" width="12.6640625"/>
-    <col min="67" max="67" width="16.88671875"/>
-    <col min="68" max="68" width="12.6640625"/>
-    <col min="69" max="69" width="19.44140625"/>
-    <col min="70" max="70" width="16.88671875"/>
-    <col min="71" max="73" width="12.6640625"/>
-    <col min="74" max="994" width="10.44140625"/>
+    <col min="65" max="66" width="12.7109375"/>
+    <col min="67" max="67" width="16.85546875"/>
+    <col min="68" max="68" width="12.7109375"/>
+    <col min="69" max="69" width="19.42578125"/>
+    <col min="70" max="70" width="16.85546875"/>
+    <col min="71" max="72" width="12.7109375"/>
+    <col min="73" max="73" width="13.5703125" customWidth="1"/>
+    <col min="74" max="74" width="12.7109375" customWidth="1"/>
+    <col min="75" max="75" width="12.7109375"/>
+    <col min="76" max="996" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1187,12 +1202,12 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1205,27 +1220,27 @@
       <c r="BK3" s="30"/>
       <c r="BL3" s="30"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -1236,401 +1251,411 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:75" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:77" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="C8" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="39" t="s">
+      <c r="E8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="F8" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="G8" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="H8" s="39" t="s">
+      <c r="I8" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="37"/>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="37"/>
+      <c r="AD8" s="37"/>
+      <c r="AE8" s="37"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="51"/>
+      <c r="AM8" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="AN8" s="39"/>
+      <c r="AO8" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP8" s="39"/>
+      <c r="AQ8" s="39"/>
+      <c r="AR8" s="39"/>
+      <c r="AS8" s="39"/>
+      <c r="AT8" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV8" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW8" s="47"/>
+      <c r="AX8" s="47"/>
+      <c r="AY8" s="47"/>
+      <c r="AZ8" s="47"/>
+      <c r="BA8" s="47"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="47"/>
+      <c r="BD8" s="47"/>
+      <c r="BE8" s="47"/>
+      <c r="BF8" s="47"/>
+      <c r="BG8" s="49"/>
+      <c r="BH8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI8" s="37"/>
+      <c r="BJ8" s="37"/>
+      <c r="BK8" s="37"/>
+      <c r="BL8" s="37"/>
+      <c r="BM8" s="37"/>
+      <c r="BN8" s="37"/>
+      <c r="BO8" s="37"/>
+      <c r="BP8" s="37"/>
+      <c r="BQ8" s="37"/>
+      <c r="BR8" s="37"/>
+      <c r="BS8" s="37"/>
+      <c r="BT8" s="37"/>
+      <c r="BU8" s="37"/>
+      <c r="BV8" s="37"/>
+      <c r="BW8" s="37"/>
+    </row>
+    <row r="9" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="42"/>
-      <c r="AG8" s="42"/>
-      <c r="AH8" s="42"/>
-      <c r="AI8" s="42"/>
-      <c r="AJ8" s="42"/>
-      <c r="AK8" s="42"/>
-      <c r="AL8" s="42"/>
-      <c r="AM8" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN8" s="43"/>
-      <c r="AO8" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP8" s="43"/>
-      <c r="AQ8" s="43"/>
-      <c r="AR8" s="43"/>
-      <c r="AS8" s="43"/>
-      <c r="AT8" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU8" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV8" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW8" s="37"/>
-      <c r="AX8" s="37"/>
-      <c r="AY8" s="37"/>
-      <c r="AZ8" s="37"/>
-      <c r="BA8" s="37"/>
-      <c r="BB8" s="37"/>
-      <c r="BC8" s="37"/>
-      <c r="BD8" s="37"/>
-      <c r="BE8" s="37"/>
-      <c r="BF8" s="37"/>
-      <c r="BG8" s="38"/>
-      <c r="BH8" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="BI8" s="41"/>
-      <c r="BJ8" s="41"/>
-      <c r="BK8" s="41"/>
-      <c r="BL8" s="41"/>
-      <c r="BM8" s="41"/>
-      <c r="BN8" s="41"/>
-      <c r="BO8" s="41"/>
-      <c r="BP8" s="41"/>
-      <c r="BQ8" s="41"/>
-      <c r="BR8" s="41"/>
-      <c r="BS8" s="41"/>
-      <c r="BT8" s="41"/>
-      <c r="BU8" s="41"/>
-    </row>
-    <row r="9" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="41" t="s">
+      <c r="J9" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="K9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="L9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="M9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="N9" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="O9" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="P9" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="Q9" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
       <c r="V9" s="33"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="41" t="s">
+      <c r="X9" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y9" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="Y9" s="41" t="s">
+      <c r="Z9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="Z9" s="41" t="s">
+      <c r="AA9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AA9" s="41" t="s">
+      <c r="AB9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="AB9" s="41" t="s">
+      <c r="AC9" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="AC9" s="41" t="s">
+      <c r="AD9" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="AD9" s="41" t="s">
+      <c r="AE9" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="AE9" s="36" t="s">
+      <c r="AF9" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="AF9" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG9" s="37"/>
-      <c r="AH9" s="37"/>
-      <c r="AI9" s="37"/>
-      <c r="AJ9" s="37"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
       <c r="AK9" s="33"/>
       <c r="AL9" s="13"/>
-      <c r="AM9" s="45" t="s">
+      <c r="AM9" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN9" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="AN9" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO9" s="47" t="s">
+      <c r="AO9" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP9" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="AP9" s="47" t="s">
+      <c r="AQ9" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="AQ9" s="43" t="s">
+      <c r="AR9" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="AR9" s="46" t="s">
+      <c r="AS9" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="AS9" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT9" s="43"/>
-      <c r="AU9" s="41"/>
-      <c r="AV9" s="41" t="s">
+      <c r="AT9" s="39"/>
+      <c r="AU9" s="37"/>
+      <c r="AV9" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW9" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="AW9" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX9" s="41" t="s">
+      <c r="AX9" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY9" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="AY9" s="44" t="s">
+      <c r="AZ9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="AZ9" s="41" t="s">
+      <c r="BA9" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="BA9" s="41" t="s">
+      <c r="BB9" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="BB9" s="41" t="s">
+      <c r="BC9" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="BC9" s="49" t="s">
+      <c r="BD9" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="BD9" s="41" t="s">
+      <c r="BE9" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="BE9" s="41" t="s">
+      <c r="BF9" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="BF9" s="41" t="s">
+      <c r="BG9" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="BG9" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="BH9" s="41" t="s">
+      <c r="BH9" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="BI9" s="37" t="s">
         <v>119</v>
-      </c>
-      <c r="BI9" s="41" t="s">
-        <v>120</v>
       </c>
       <c r="BJ9" s="34"/>
       <c r="BK9" s="34"/>
-      <c r="BL9" s="49" t="s">
+      <c r="BL9" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="BM9" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="BM9" s="41" t="s">
+      <c r="BN9" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="BN9" s="41" t="s">
+      <c r="BO9" s="37"/>
+      <c r="BP9" s="37"/>
+      <c r="BQ9" s="37"/>
+      <c r="BR9" s="37"/>
+      <c r="BS9" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="BO9" s="41"/>
-      <c r="BP9" s="41"/>
-      <c r="BQ9" s="41"/>
-      <c r="BR9" s="41"/>
-      <c r="BS9" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="BT9" s="41"/>
-      <c r="BU9" s="41"/>
+      <c r="BT9" s="37"/>
+      <c r="BU9" s="37"/>
+      <c r="BV9" s="37"/>
+      <c r="BW9" s="37"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
       <c r="Q10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="R10" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="R10" s="16" t="s">
+      <c r="S10" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="S10" s="16" t="s">
+      <c r="T10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="16" t="s">
+      <c r="U10" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="V10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="V10" s="16" t="s">
+      <c r="W10" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="W10" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="41"/>
-      <c r="AE10" s="41"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="37"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="37"/>
+      <c r="AE10" s="37"/>
       <c r="AF10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG10" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AH10" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AI10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AJ10" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AK10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AK10" s="16" t="s">
+      <c r="AL10" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AL10" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM10" s="43"/>
-      <c r="AN10" s="43"/>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="43"/>
-      <c r="AR10" s="43"/>
-      <c r="AS10" s="43"/>
-      <c r="AT10" s="43"/>
-      <c r="AU10" s="41"/>
-      <c r="AV10" s="41"/>
-      <c r="AW10" s="41"/>
-      <c r="AX10" s="41"/>
-      <c r="AY10" s="41"/>
-      <c r="AZ10" s="41"/>
-      <c r="BA10" s="41"/>
-      <c r="BB10" s="41"/>
-      <c r="BC10" s="50"/>
-      <c r="BD10" s="41"/>
-      <c r="BE10" s="41"/>
-      <c r="BF10" s="41"/>
-      <c r="BG10" s="41"/>
-      <c r="BH10" s="41"/>
-      <c r="BI10" s="41"/>
+      <c r="AM10" s="39"/>
+      <c r="AN10" s="39"/>
+      <c r="AO10" s="42"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="39"/>
+      <c r="AR10" s="39"/>
+      <c r="AS10" s="39"/>
+      <c r="AT10" s="39"/>
+      <c r="AU10" s="37"/>
+      <c r="AV10" s="37"/>
+      <c r="AW10" s="37"/>
+      <c r="AX10" s="37"/>
+      <c r="AY10" s="37"/>
+      <c r="AZ10" s="37"/>
+      <c r="BA10" s="37"/>
+      <c r="BB10" s="37"/>
+      <c r="BC10" s="44"/>
+      <c r="BD10" s="37"/>
+      <c r="BE10" s="37"/>
+      <c r="BF10" s="37"/>
+      <c r="BG10" s="37"/>
+      <c r="BH10" s="37"/>
+      <c r="BI10" s="37"/>
       <c r="BJ10" s="34" t="s">
         <v>0</v>
       </c>
       <c r="BK10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BL10" s="51"/>
-      <c r="BM10" s="41"/>
+      <c r="BL10" s="45"/>
+      <c r="BM10" s="37"/>
       <c r="BN10" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="BO10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="BP10" s="10" t="s">
+      <c r="BQ10" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="BQ10" s="10" t="s">
+      <c r="BR10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BS10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="BS10" s="10" t="s">
+      <c r="BT10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="BT10" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="BU10" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="BV10" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BW10" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1650,7 +1675,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>5</v>
@@ -1696,7 +1721,7 @@
         <v>23</v>
       </c>
       <c r="V11" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W11" s="23" t="s">
         <v>24</v>
@@ -1742,7 +1767,7 @@
         <v>36</v>
       </c>
       <c r="AK11" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AL11" s="23" t="s">
         <v>37</v>
@@ -1754,13 +1779,13 @@
         <v>39</v>
       </c>
       <c r="AO11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AP11" s="24" t="s">
+      <c r="AQ11" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="AQ11" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="AR11" s="15" t="s">
         <v>40</v>
@@ -1794,10 +1819,10 @@
         <v>48</v>
       </c>
       <c r="BB11" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC11" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BD11" s="29" t="e">
         <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
@@ -1830,7 +1855,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BM11" s="31" t="e">
         <f>BK11/BJ11</f>
@@ -1858,16 +1883,65 @@
       <c r="BT11" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="BU11" s="21" t="s">
+      <c r="BU11" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="BV11" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BX11" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="BV11" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="BW11" s="12"/>
+      <c r="BY11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="AO8:AS8"/>
+    <mergeCell ref="AT8:AT10"/>
+    <mergeCell ref="AU8:AU10"/>
+    <mergeCell ref="BH8:BW8"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BS9:BW9"/>
+    <mergeCell ref="AV8:BG8"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="BN9:BR9"/>
     <mergeCell ref="AM9:AM10"/>
@@ -1884,49 +1958,6 @@
     <mergeCell ref="BM9:BM10"/>
     <mergeCell ref="BL9:BL10"/>
     <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AO8:AS8"/>
-    <mergeCell ref="AT8:AT10"/>
-    <mergeCell ref="AU8:AU10"/>
-    <mergeCell ref="BH8:BU8"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BS9:BU9"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AV8:BG8"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1263: Anspruch Kanton und Anspruch Gemeinde in Statistiken ergänzen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\TODO\KIBON-REPORTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\KibonReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CE70F7-A4DC-4146-A703-A6220A07482D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630F38EB-19F9-4E59-908B-F15768C10164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -191,12 +191,6 @@
     <t>{betreuungsPensum}</t>
   </si>
   <si>
-    <t>{anspruchsPensum}</t>
-  </si>
-  <si>
-    <t>{bgPensum}</t>
-  </si>
-  <si>
     <t>{bgStunden}</t>
   </si>
   <si>
@@ -407,12 +401,6 @@
     <t>{kostenTitle}</t>
   </si>
   <si>
-    <t>{anspruchberechtigtTitle}</t>
-  </si>
-  <si>
-    <t>{bgPensumTitle}</t>
-  </si>
-  <si>
     <t>{bgPensumStdTitle}</t>
   </si>
   <si>
@@ -447,6 +435,42 @@
   </si>
   <si>
     <t>{verguenstigungTotal}</t>
+  </si>
+  <si>
+    <t>{anspruchberechtigtTotalTitle}</t>
+  </si>
+  <si>
+    <t>{anspruchberechtigtKantonTitle}</t>
+  </si>
+  <si>
+    <t>{anspruchberechtigtGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{anspruchsPensumKanton}</t>
+  </si>
+  <si>
+    <t>{anspruchsPensumGemeinde}</t>
+  </si>
+  <si>
+    <t>{anspruchsPensumTotal}</t>
+  </si>
+  <si>
+    <t>{bgPensumKantonTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumKanton}</t>
+  </si>
+  <si>
+    <t>{bgPensumGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumGemeinde}</t>
+  </si>
+  <si>
+    <t>{bgPensumTotalTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumTotal}</t>
   </si>
 </sst>
 </file>
@@ -684,12 +708,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -706,24 +748,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1136,7 +1160,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BY11"/>
+  <dimension ref="A1:CC11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1178,21 +1202,24 @@
     <col min="62" max="62" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="63" max="63" width="16" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="16" customWidth="1"/>
-    <col min="65" max="66" width="12.7109375"/>
-    <col min="67" max="67" width="16.85546875"/>
-    <col min="68" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="19.42578125"/>
-    <col min="70" max="70" width="16.85546875"/>
-    <col min="71" max="72" width="12.7109375"/>
-    <col min="73" max="73" width="13.5703125" customWidth="1"/>
-    <col min="74" max="74" width="12.7109375" customWidth="1"/>
-    <col min="75" max="75" width="12.7109375"/>
-    <col min="76" max="996" width="10.42578125"/>
+    <col min="65" max="65" width="12.7109375"/>
+    <col min="66" max="67" width="13.28515625" customWidth="1"/>
+    <col min="68" max="68" width="13.7109375" customWidth="1"/>
+    <col min="69" max="69" width="16.85546875"/>
+    <col min="70" max="71" width="12.28515625" customWidth="1"/>
+    <col min="72" max="72" width="12.7109375"/>
+    <col min="73" max="73" width="19.42578125"/>
+    <col min="74" max="74" width="16.85546875"/>
+    <col min="75" max="76" width="12.7109375"/>
+    <col min="77" max="77" width="13.5703125" customWidth="1"/>
+    <col min="78" max="78" width="12.7109375" customWidth="1"/>
+    <col min="79" max="79" width="12.7109375"/>
+    <col min="80" max="1000" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:81" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1202,12 +1229,12 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1220,27 +1247,27 @@
       <c r="BK3" s="30"/>
       <c r="BL3" s="30"/>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -1251,36 +1278,36 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:77" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="E8" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="36" t="s">
+      <c r="F8" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="G8" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="I8" s="37" t="s">
         <v>75</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>77</v>
       </c>
       <c r="J8" s="37"/>
       <c r="K8" s="37"/>
@@ -1289,15 +1316,15 @@
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
       <c r="X8" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Y8" s="37"/>
       <c r="Z8" s="37"/>
@@ -1306,46 +1333,46 @@
       <c r="AC8" s="37"/>
       <c r="AD8" s="37"/>
       <c r="AE8" s="37"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="38"/>
+      <c r="AJ8" s="38"/>
+      <c r="AK8" s="38"/>
+      <c r="AL8" s="38"/>
       <c r="AM8" s="39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN8" s="39"/>
       <c r="AO8" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AP8" s="39"/>
       <c r="AQ8" s="39"/>
       <c r="AR8" s="39"/>
       <c r="AS8" s="39"/>
       <c r="AT8" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV8" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="AU8" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="AV8" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW8" s="47"/>
-      <c r="AX8" s="47"/>
-      <c r="AY8" s="47"/>
-      <c r="AZ8" s="47"/>
-      <c r="BA8" s="47"/>
-      <c r="BB8" s="47"/>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="47"/>
-      <c r="BE8" s="47"/>
-      <c r="BF8" s="47"/>
-      <c r="BG8" s="49"/>
+      <c r="AW8" s="42"/>
+      <c r="AX8" s="42"/>
+      <c r="AY8" s="42"/>
+      <c r="AZ8" s="42"/>
+      <c r="BA8" s="42"/>
+      <c r="BB8" s="42"/>
+      <c r="BC8" s="42"/>
+      <c r="BD8" s="42"/>
+      <c r="BE8" s="42"/>
+      <c r="BF8" s="42"/>
+      <c r="BG8" s="44"/>
       <c r="BH8" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="BI8" s="37"/>
       <c r="BJ8" s="37"/>
@@ -1362,174 +1389,182 @@
       <c r="BU8" s="37"/>
       <c r="BV8" s="37"/>
       <c r="BW8" s="37"/>
+      <c r="BX8" s="37"/>
+      <c r="BY8" s="37"/>
+      <c r="BZ8" s="37"/>
+      <c r="CA8" s="37"/>
     </row>
-    <row r="9" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
       <c r="B9" s="36"/>
-      <c r="C9" s="50"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
       <c r="I9" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="L9" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="M9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="N9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="O9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="P9" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="Q9" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="P9" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q9" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
       <c r="V9" s="33"/>
       <c r="W9" s="13"/>
       <c r="X9" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y9" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z9" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Y9" s="37" t="s">
+      <c r="AA9" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="Z9" s="37" t="s">
+      <c r="AB9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="AA9" s="37" t="s">
+      <c r="AC9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="37" t="s">
+      <c r="AD9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="AC9" s="37" t="s">
+      <c r="AE9" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="AD9" s="37" t="s">
+      <c r="AF9" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="AE9" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF9" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG9" s="47"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
+      <c r="AG9" s="42"/>
+      <c r="AH9" s="42"/>
+      <c r="AI9" s="42"/>
+      <c r="AJ9" s="42"/>
       <c r="AK9" s="33"/>
       <c r="AL9" s="13"/>
-      <c r="AM9" s="38" t="s">
-        <v>96</v>
+      <c r="AM9" s="45" t="s">
+        <v>94</v>
       </c>
       <c r="AN9" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO9" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="AO9" s="41" t="s">
+      <c r="AP9" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ9" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="AP9" s="41" t="s">
+      <c r="AR9" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="AQ9" s="39" t="s">
+      <c r="AS9" s="39" t="s">
         <v>101</v>
-      </c>
-      <c r="AR9" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS9" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="AT9" s="39"/>
       <c r="AU9" s="37"/>
       <c r="AV9" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AW9" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AX9" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY9" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ9" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="AY9" s="48" t="s">
+      <c r="BA9" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="AZ9" s="37" t="s">
+      <c r="BB9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="BA9" s="37" t="s">
+      <c r="BC9" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="BB9" s="37" t="s">
+      <c r="BD9" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="BC9" s="43" t="s">
+      <c r="BE9" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="BD9" s="37" t="s">
+      <c r="BF9" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="BE9" s="37" t="s">
+      <c r="BG9" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="BF9" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="BG9" s="37" t="s">
+      <c r="BH9" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="BH9" s="37" t="s">
-        <v>118</v>
-      </c>
       <c r="BI9" s="37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BJ9" s="34"/>
       <c r="BK9" s="34"/>
-      <c r="BL9" s="43" t="s">
+      <c r="BL9" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="BM9" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="BN9" s="37" t="s">
         <v>120</v>
-      </c>
-      <c r="BM9" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="BN9" s="37" t="s">
-        <v>122</v>
       </c>
       <c r="BO9" s="37"/>
       <c r="BP9" s="37"/>
       <c r="BQ9" s="37"/>
       <c r="BR9" s="37"/>
-      <c r="BS9" s="37" t="s">
-        <v>123</v>
-      </c>
+      <c r="BS9" s="37"/>
       <c r="BT9" s="37"/>
       <c r="BU9" s="37"/>
       <c r="BV9" s="37"/>
-      <c r="BW9" s="37"/>
+      <c r="BW9" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="BX9" s="37"/>
+      <c r="BY9" s="37"/>
+      <c r="BZ9" s="37"/>
+      <c r="CA9" s="37"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
@@ -1544,25 +1579,25 @@
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
       <c r="Q10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="S10" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="R10" s="16" t="s">
+      <c r="T10" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="S10" s="16" t="s">
+      <c r="U10" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="T10" s="16" t="s">
+      <c r="V10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="W10" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="W10" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="X10" s="37"/>
       <c r="Y10" s="37"/>
@@ -1573,30 +1608,30 @@
       <c r="AD10" s="37"/>
       <c r="AE10" s="37"/>
       <c r="AF10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH10" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AI10" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AJ10" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AK10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AL10" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="AK10" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="AL10" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="AM10" s="39"/>
       <c r="AN10" s="39"/>
-      <c r="AO10" s="42"/>
-      <c r="AP10" s="42"/>
+      <c r="AO10" s="48"/>
+      <c r="AP10" s="48"/>
       <c r="AQ10" s="39"/>
       <c r="AR10" s="39"/>
       <c r="AS10" s="39"/>
@@ -1609,7 +1644,7 @@
       <c r="AZ10" s="37"/>
       <c r="BA10" s="37"/>
       <c r="BB10" s="37"/>
-      <c r="BC10" s="44"/>
+      <c r="BC10" s="50"/>
       <c r="BD10" s="37"/>
       <c r="BE10" s="37"/>
       <c r="BF10" s="37"/>
@@ -1622,40 +1657,52 @@
       <c r="BK10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BL10" s="45"/>
+      <c r="BL10" s="51"/>
       <c r="BM10" s="37"/>
       <c r="BN10" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="BO10" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="BP10" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ10" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BR10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="BS10" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="BT10" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="BV10" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="BW10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="BP10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="BQ10" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="BR10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="BT10" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="BU10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="CA10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="BV10" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="BW10" s="10" t="s">
-        <v>136</v>
-      </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1675,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>5</v>
@@ -1721,7 +1768,7 @@
         <v>23</v>
       </c>
       <c r="V11" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W11" s="23" t="s">
         <v>24</v>
@@ -1767,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="AK11" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AL11" s="23" t="s">
         <v>37</v>
@@ -1779,13 +1826,13 @@
         <v>39</v>
       </c>
       <c r="AO11" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ11" s="24" t="s">
         <v>58</v>
-      </c>
-      <c r="AP11" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ11" s="24" t="s">
-        <v>60</v>
       </c>
       <c r="AR11" s="15" t="s">
         <v>40</v>
@@ -1819,10 +1866,10 @@
         <v>48</v>
       </c>
       <c r="BB11" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="BC11" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="BD11" s="29" t="e">
         <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
@@ -1855,7 +1902,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="BM11" s="31" t="e">
         <f>BK11/BJ11</f>
@@ -1865,85 +1912,54 @@
         <v>51</v>
       </c>
       <c r="BO11" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="BP11" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="BQ11" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="BR11" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="BS11" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT11" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="BU11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BP11" s="26" t="s">
+      <c r="BV11" s="31" t="e">
+        <f>BT11*BM11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BW11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="BQ11" s="20" t="s">
+      <c r="BX11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="BR11" s="31" t="e">
-        <f>BP11*BM11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BS11" s="20" t="s">
+      <c r="BY11" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="BZ11" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="CA11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="CB11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="BT11" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="BU11" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="BV11" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="BW11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BX11" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="BY11" s="12"/>
+      <c r="CC11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AO8:AS8"/>
-    <mergeCell ref="AT8:AT10"/>
-    <mergeCell ref="AU8:AU10"/>
-    <mergeCell ref="BH8:BW8"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BS9:BW9"/>
-    <mergeCell ref="AV8:BG8"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BN9:BR9"/>
+    <mergeCell ref="BN9:BV9"/>
     <mergeCell ref="AM9:AM10"/>
     <mergeCell ref="AN9:AN10"/>
     <mergeCell ref="AQ9:AQ10"/>
@@ -1958,6 +1974,49 @@
     <mergeCell ref="BM9:BM10"/>
     <mergeCell ref="BL9:BL10"/>
     <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AO8:AS8"/>
+    <mergeCell ref="AT8:AT10"/>
+    <mergeCell ref="AU8:AU10"/>
+    <mergeCell ref="BH8:CA8"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BW9:CA9"/>
+    <mergeCell ref="AV8:BG8"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="AE9:AE10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1257: In Statistiken steht fix "BG-Pensum in Stunden"
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\KibonReports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630F38EB-19F9-4E59-908B-F15768C10164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0EDF0-2B5A-4B78-92EF-825F4D33F58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="148">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>{bgPensumTotal}</t>
+  </si>
+  <si>
+    <t>{bgPensumZeiteinheitTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumZeiteinheit}</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -708,48 +714,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1160,7 +1167,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CC11"/>
+  <dimension ref="A1:CD11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1209,15 +1216,15 @@
     <col min="70" max="71" width="12.28515625" customWidth="1"/>
     <col min="72" max="72" width="12.7109375"/>
     <col min="73" max="73" width="19.42578125"/>
-    <col min="74" max="74" width="16.85546875"/>
-    <col min="75" max="76" width="12.7109375"/>
-    <col min="77" max="77" width="13.5703125" customWidth="1"/>
-    <col min="78" max="78" width="12.7109375" customWidth="1"/>
-    <col min="79" max="79" width="12.7109375"/>
-    <col min="80" max="1000" width="10.42578125"/>
+    <col min="75" max="75" width="16.85546875"/>
+    <col min="76" max="77" width="12.7109375"/>
+    <col min="78" max="78" width="13.5703125" customWidth="1"/>
+    <col min="79" max="79" width="12.7109375" customWidth="1"/>
+    <col min="80" max="80" width="12.7109375"/>
+    <col min="81" max="1001" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:82" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1229,10 +1236,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -1247,7 +1254,7 @@
       <c r="BK3" s="30"/>
       <c r="BL3" s="30"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1256,7 +1263,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1265,7 +1272,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1278,17 +1285,17 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:81" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="50" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -1316,13 +1323,13 @@
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
       <c r="X8" s="37" t="s">
         <v>92</v>
       </c>
@@ -1333,13 +1340,13 @@
       <c r="AC8" s="37"/>
       <c r="AD8" s="37"/>
       <c r="AE8" s="37"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
-      <c r="AI8" s="38"/>
-      <c r="AJ8" s="38"/>
-      <c r="AK8" s="38"/>
-      <c r="AL8" s="38"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="51"/>
       <c r="AM8" s="39" t="s">
         <v>93</v>
       </c>
@@ -1357,20 +1364,20 @@
       <c r="AU8" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="AV8" s="41" t="s">
+      <c r="AV8" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="AW8" s="42"/>
-      <c r="AX8" s="42"/>
-      <c r="AY8" s="42"/>
-      <c r="AZ8" s="42"/>
-      <c r="BA8" s="42"/>
-      <c r="BB8" s="42"/>
-      <c r="BC8" s="42"/>
-      <c r="BD8" s="42"/>
-      <c r="BE8" s="42"/>
-      <c r="BF8" s="42"/>
-      <c r="BG8" s="44"/>
+      <c r="AW8" s="47"/>
+      <c r="AX8" s="47"/>
+      <c r="AY8" s="47"/>
+      <c r="AZ8" s="47"/>
+      <c r="BA8" s="47"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="47"/>
+      <c r="BD8" s="47"/>
+      <c r="BE8" s="47"/>
+      <c r="BF8" s="47"/>
+      <c r="BG8" s="49"/>
       <c r="BH8" s="37" t="s">
         <v>115</v>
       </c>
@@ -1393,11 +1400,12 @@
       <c r="BY8" s="37"/>
       <c r="BZ8" s="37"/>
       <c r="CA8" s="37"/>
+      <c r="CB8" s="37"/>
     </row>
-    <row r="9" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
       <c r="B9" s="36"/>
-      <c r="C9" s="40"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
@@ -1424,16 +1432,16 @@
       <c r="O9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="P9" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
       <c r="V9" s="33"/>
       <c r="W9" s="13"/>
       <c r="X9" s="37" t="s">
@@ -1457,34 +1465,34 @@
       <c r="AD9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="AE9" s="41" t="s">
+      <c r="AE9" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="AF9" s="41" t="s">
+      <c r="AF9" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="AG9" s="42"/>
-      <c r="AH9" s="42"/>
-      <c r="AI9" s="42"/>
-      <c r="AJ9" s="42"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
       <c r="AK9" s="33"/>
       <c r="AL9" s="13"/>
-      <c r="AM9" s="45" t="s">
+      <c r="AM9" s="38" t="s">
         <v>94</v>
       </c>
       <c r="AN9" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="AO9" s="47" t="s">
+      <c r="AO9" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="AP9" s="47" t="s">
+      <c r="AP9" s="41" t="s">
         <v>98</v>
       </c>
       <c r="AQ9" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="AR9" s="46" t="s">
+      <c r="AR9" s="40" t="s">
         <v>100</v>
       </c>
       <c r="AS9" s="39" t="s">
@@ -1501,7 +1509,7 @@
       <c r="AX9" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="AY9" s="43" t="s">
+      <c r="AY9" s="48" t="s">
         <v>106</v>
       </c>
       <c r="AZ9" s="37" t="s">
@@ -1513,7 +1521,7 @@
       <c r="BB9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="BC9" s="49" t="s">
+      <c r="BC9" s="43" t="s">
         <v>110</v>
       </c>
       <c r="BD9" s="37" t="s">
@@ -1536,7 +1544,7 @@
       </c>
       <c r="BJ9" s="34"/>
       <c r="BK9" s="34"/>
-      <c r="BL9" s="49" t="s">
+      <c r="BL9" s="43" t="s">
         <v>118</v>
       </c>
       <c r="BM9" s="37" t="s">
@@ -1553,18 +1561,19 @@
       <c r="BT9" s="37"/>
       <c r="BU9" s="37"/>
       <c r="BV9" s="37"/>
-      <c r="BW9" s="37" t="s">
+      <c r="BW9" s="37"/>
+      <c r="BX9" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="BX9" s="37"/>
       <c r="BY9" s="37"/>
       <c r="BZ9" s="37"/>
       <c r="CA9" s="37"/>
+      <c r="CB9" s="37"/>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
-      <c r="C10" s="40"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
@@ -1630,8 +1639,8 @@
       </c>
       <c r="AM10" s="39"/>
       <c r="AN10" s="39"/>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
+      <c r="AO10" s="42"/>
+      <c r="AP10" s="42"/>
       <c r="AQ10" s="39"/>
       <c r="AR10" s="39"/>
       <c r="AS10" s="39"/>
@@ -1644,7 +1653,7 @@
       <c r="AZ10" s="37"/>
       <c r="BA10" s="37"/>
       <c r="BB10" s="37"/>
-      <c r="BC10" s="50"/>
+      <c r="BC10" s="44"/>
       <c r="BD10" s="37"/>
       <c r="BE10" s="37"/>
       <c r="BF10" s="37"/>
@@ -1657,7 +1666,7 @@
       <c r="BK10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BL10" s="51"/>
+      <c r="BL10" s="45"/>
       <c r="BM10" s="37"/>
       <c r="BN10" s="10" t="s">
         <v>115</v>
@@ -1684,25 +1693,28 @@
         <v>122</v>
       </c>
       <c r="BV10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1932,75 +1944,35 @@
       <c r="BU11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BV11" s="31" t="e">
+      <c r="BV11" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="BW11" s="31" t="e">
         <f>BT11*BM11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BW11" s="20" t="s">
+      <c r="BX11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="BX11" s="20" t="s">
+      <c r="BY11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="BY11" s="20" t="s">
+      <c r="BZ11" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="BZ11" s="20" t="s">
+      <c r="CA11" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="CA11" s="21" t="s">
+      <c r="CB11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CB11" s="32" t="s">
+      <c r="CC11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="CC11" s="12"/>
+      <c r="CD11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BN9:BV9"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AF9:AJ9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AO8:AS8"/>
-    <mergeCell ref="AT8:AT10"/>
-    <mergeCell ref="AU8:AU10"/>
-    <mergeCell ref="BH8:CA8"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BW9:CA9"/>
-    <mergeCell ref="AV8:BG8"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:W8"/>
@@ -2017,6 +1989,49 @@
     <mergeCell ref="Q9:U9"/>
     <mergeCell ref="X9:X10"/>
     <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AO8:AS8"/>
+    <mergeCell ref="AT8:AT10"/>
+    <mergeCell ref="AU8:AU10"/>
+    <mergeCell ref="BH8:CB8"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BX9:CB9"/>
+    <mergeCell ref="AV8:BG8"/>
+    <mergeCell ref="AF9:AJ9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="BN9:BW9"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="AD9:AD10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1490 Freiwilligenarbeit in Statistik. Werte überschreiten aktuell noch das definierte Maximum der Gemeinde
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0EDF0-2B5A-4B78-92EF-825F4D33F58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CDB02-E782-4F90-ADE3-1636EF6B3E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="151">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -477,6 +477,15 @@
   </si>
   <si>
     <t>{bgPensumZeiteinheit}</t>
+  </si>
+  <si>
+    <t>{gesFreiwilligenarbeitTitle}</t>
+  </si>
+  <si>
+    <t>{gs2EwpFreiwillig}</t>
+  </si>
+  <si>
+    <t>{gs1EwpFreiwillig}</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -708,18 +717,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -738,25 +769,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1167,7 +1179,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CD11"/>
+  <dimension ref="A1:CF11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1182,49 +1194,51 @@
     <col min="20" max="20" width="10.7109375"/>
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
     <col min="22" max="22" width="41.42578125" customWidth="1"/>
-    <col min="23" max="23" width="24.140625"/>
-    <col min="24" max="31" width="8.7109375"/>
-    <col min="32" max="33" width="10.7109375"/>
-    <col min="34" max="34" width="24.5703125" customWidth="1"/>
-    <col min="35" max="35" width="10.7109375"/>
-    <col min="36" max="36" width="14.42578125" customWidth="1"/>
-    <col min="37" max="37" width="41.42578125" customWidth="1"/>
-    <col min="38" max="38" width="24.140625"/>
-    <col min="39" max="39" width="9.140625" customWidth="1"/>
-    <col min="40" max="40" width="6.42578125"/>
-    <col min="41" max="41" width="18.140625"/>
-    <col min="43" max="43" width="23.28515625"/>
-    <col min="44" max="44" width="9.28515625"/>
-    <col min="45" max="45" width="25.42578125"/>
-    <col min="46" max="46" width="27.42578125"/>
-    <col min="47" max="47" width="10.42578125"/>
-    <col min="48" max="50" width="12.7109375"/>
-    <col min="51" max="51" width="16.7109375"/>
-    <col min="52" max="52" width="12.7109375"/>
-    <col min="53" max="53" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="22"/>
-    <col min="55" max="55" width="18.140625" customWidth="1"/>
-    <col min="56" max="59" width="22"/>
-    <col min="60" max="61" width="12.7109375"/>
-    <col min="62" max="62" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="16" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="16" customWidth="1"/>
-    <col min="65" max="65" width="12.7109375"/>
-    <col min="66" max="67" width="13.28515625" customWidth="1"/>
-    <col min="68" max="68" width="13.7109375" customWidth="1"/>
-    <col min="69" max="69" width="16.85546875"/>
-    <col min="70" max="71" width="12.28515625" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375"/>
-    <col min="73" max="73" width="19.42578125"/>
-    <col min="75" max="75" width="16.85546875"/>
-    <col min="76" max="77" width="12.7109375"/>
-    <col min="78" max="78" width="13.5703125" customWidth="1"/>
-    <col min="79" max="79" width="12.7109375" customWidth="1"/>
-    <col min="80" max="80" width="12.7109375"/>
-    <col min="81" max="1001" width="10.42578125"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="24.140625"/>
+    <col min="25" max="32" width="8.7109375"/>
+    <col min="33" max="34" width="10.7109375"/>
+    <col min="35" max="35" width="24.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375"/>
+    <col min="37" max="37" width="14.42578125" customWidth="1"/>
+    <col min="38" max="38" width="41.42578125" customWidth="1"/>
+    <col min="39" max="39" width="27.140625" customWidth="1"/>
+    <col min="40" max="40" width="24.140625"/>
+    <col min="41" max="41" width="9.140625" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125"/>
+    <col min="43" max="43" width="18.140625"/>
+    <col min="45" max="45" width="23.28515625"/>
+    <col min="46" max="46" width="9.28515625"/>
+    <col min="47" max="47" width="25.42578125"/>
+    <col min="48" max="48" width="27.42578125"/>
+    <col min="49" max="49" width="10.42578125"/>
+    <col min="50" max="52" width="12.7109375"/>
+    <col min="53" max="53" width="16.7109375"/>
+    <col min="54" max="54" width="12.7109375"/>
+    <col min="55" max="55" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22"/>
+    <col min="57" max="57" width="18.140625" customWidth="1"/>
+    <col min="58" max="61" width="22"/>
+    <col min="62" max="63" width="12.7109375"/>
+    <col min="64" max="64" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="16" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="16" customWidth="1"/>
+    <col min="67" max="67" width="12.7109375"/>
+    <col min="68" max="69" width="13.28515625" customWidth="1"/>
+    <col min="70" max="70" width="13.7109375" customWidth="1"/>
+    <col min="71" max="71" width="16.85546875"/>
+    <col min="72" max="73" width="12.28515625" customWidth="1"/>
+    <col min="74" max="74" width="12.7109375"/>
+    <col min="75" max="75" width="19.42578125"/>
+    <col min="77" max="77" width="16.85546875"/>
+    <col min="78" max="79" width="12.7109375"/>
+    <col min="80" max="80" width="13.5703125" customWidth="1"/>
+    <col min="81" max="81" width="12.7109375" customWidth="1"/>
+    <col min="82" max="82" width="12.7109375"/>
+    <col min="83" max="1003" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:84" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1236,10 +1250,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -1250,11 +1264,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BJ3" s="30"/>
-      <c r="BK3" s="30"/>
       <c r="BL3" s="30"/>
+      <c r="BM3" s="30"/>
+      <c r="BN3" s="30"/>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1263,7 +1277,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1272,7 +1286,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1285,308 +1299,312 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:82" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:84" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="37" t="s">
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="40"/>
+      <c r="Y8" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
-      <c r="AA8" s="37"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
-      <c r="AM8" s="39" t="s">
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="40"/>
+      <c r="AH8" s="40"/>
+      <c r="AI8" s="40"/>
+      <c r="AJ8" s="40"/>
+      <c r="AK8" s="40"/>
+      <c r="AL8" s="40"/>
+      <c r="AM8" s="40"/>
+      <c r="AN8" s="40"/>
+      <c r="AO8" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="39" t="s">
+      <c r="AP8" s="41"/>
+      <c r="AQ8" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39"/>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39"/>
-      <c r="AT8" s="39" t="s">
+      <c r="AR8" s="41"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="41"/>
+      <c r="AV8" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="AU8" s="37" t="s">
+      <c r="AW8" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="AV8" s="46" t="s">
+      <c r="AX8" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="AW8" s="47"/>
-      <c r="AX8" s="47"/>
-      <c r="AY8" s="47"/>
-      <c r="AZ8" s="47"/>
-      <c r="BA8" s="47"/>
-      <c r="BB8" s="47"/>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="47"/>
-      <c r="BE8" s="47"/>
-      <c r="BF8" s="47"/>
-      <c r="BG8" s="49"/>
-      <c r="BH8" s="37" t="s">
+      <c r="AY8" s="43"/>
+      <c r="AZ8" s="43"/>
+      <c r="BA8" s="43"/>
+      <c r="BB8" s="43"/>
+      <c r="BC8" s="43"/>
+      <c r="BD8" s="43"/>
+      <c r="BE8" s="43"/>
+      <c r="BF8" s="43"/>
+      <c r="BG8" s="43"/>
+      <c r="BH8" s="43"/>
+      <c r="BI8" s="46"/>
+      <c r="BJ8" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="BI8" s="37"/>
-      <c r="BJ8" s="37"/>
-      <c r="BK8" s="37"/>
-      <c r="BL8" s="37"/>
-      <c r="BM8" s="37"/>
-      <c r="BN8" s="37"/>
-      <c r="BO8" s="37"/>
-      <c r="BP8" s="37"/>
-      <c r="BQ8" s="37"/>
-      <c r="BR8" s="37"/>
-      <c r="BS8" s="37"/>
-      <c r="BT8" s="37"/>
-      <c r="BU8" s="37"/>
-      <c r="BV8" s="37"/>
-      <c r="BW8" s="37"/>
-      <c r="BX8" s="37"/>
-      <c r="BY8" s="37"/>
-      <c r="BZ8" s="37"/>
-      <c r="CA8" s="37"/>
-      <c r="CB8" s="37"/>
+      <c r="BK8" s="39"/>
+      <c r="BL8" s="39"/>
+      <c r="BM8" s="39"/>
+      <c r="BN8" s="39"/>
+      <c r="BO8" s="39"/>
+      <c r="BP8" s="39"/>
+      <c r="BQ8" s="39"/>
+      <c r="BR8" s="39"/>
+      <c r="BS8" s="39"/>
+      <c r="BT8" s="39"/>
+      <c r="BU8" s="39"/>
+      <c r="BV8" s="39"/>
+      <c r="BW8" s="39"/>
+      <c r="BX8" s="39"/>
+      <c r="BY8" s="39"/>
+      <c r="BZ8" s="39"/>
+      <c r="CA8" s="39"/>
+      <c r="CB8" s="39"/>
+      <c r="CC8" s="39"/>
+      <c r="CD8" s="39"/>
     </row>
-    <row r="9" spans="1:82" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37" t="s">
+    <row r="9" spans="1:84" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="O9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
       <c r="V9" s="33"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="37" t="s">
+      <c r="W9" s="36"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="Y9" s="37" t="s">
+      <c r="Z9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="37" t="s">
+      <c r="AA9" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="AA9" s="37" t="s">
+      <c r="AB9" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="AB9" s="37" t="s">
+      <c r="AC9" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="AC9" s="37" t="s">
+      <c r="AD9" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="AD9" s="37" t="s">
+      <c r="AE9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="AE9" s="46" t="s">
+      <c r="AF9" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="AF9" s="46" t="s">
+      <c r="AG9" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="AG9" s="47"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="33"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="38" t="s">
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="43"/>
+      <c r="AJ9" s="43"/>
+      <c r="AK9" s="43"/>
+      <c r="AL9" s="33"/>
+      <c r="AM9" s="36"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="AN9" s="39" t="s">
+      <c r="AP9" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="AO9" s="41" t="s">
+      <c r="AQ9" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="AP9" s="41" t="s">
+      <c r="AR9" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="AQ9" s="39" t="s">
+      <c r="AS9" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="AR9" s="40" t="s">
+      <c r="AT9" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="AS9" s="39" t="s">
+      <c r="AU9" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="AT9" s="39"/>
-      <c r="AU9" s="37"/>
-      <c r="AV9" s="37" t="s">
+      <c r="AV9" s="41"/>
+      <c r="AW9" s="39"/>
+      <c r="AX9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AW9" s="37" t="s">
+      <c r="AY9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="AX9" s="37" t="s">
+      <c r="AZ9" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="AY9" s="48" t="s">
+      <c r="BA9" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="AZ9" s="37" t="s">
+      <c r="BB9" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="BA9" s="37" t="s">
+      <c r="BC9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="BB9" s="37" t="s">
+      <c r="BD9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="BC9" s="43" t="s">
+      <c r="BE9" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="BD9" s="37" t="s">
+      <c r="BF9" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="BE9" s="37" t="s">
+      <c r="BG9" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="BF9" s="37" t="s">
+      <c r="BH9" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="BG9" s="37" t="s">
+      <c r="BI9" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="BH9" s="37" t="s">
+      <c r="BJ9" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="BI9" s="37" t="s">
+      <c r="BK9" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="BJ9" s="34"/>
-      <c r="BK9" s="34"/>
-      <c r="BL9" s="43" t="s">
+      <c r="BL9" s="34"/>
+      <c r="BM9" s="34"/>
+      <c r="BN9" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="BM9" s="37" t="s">
+      <c r="BO9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="BN9" s="37" t="s">
+      <c r="BP9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="BO9" s="37"/>
-      <c r="BP9" s="37"/>
-      <c r="BQ9" s="37"/>
-      <c r="BR9" s="37"/>
-      <c r="BS9" s="37"/>
-      <c r="BT9" s="37"/>
-      <c r="BU9" s="37"/>
-      <c r="BV9" s="37"/>
-      <c r="BW9" s="37"/>
-      <c r="BX9" s="37" t="s">
+      <c r="BQ9" s="39"/>
+      <c r="BR9" s="39"/>
+      <c r="BS9" s="39"/>
+      <c r="BT9" s="39"/>
+      <c r="BU9" s="39"/>
+      <c r="BV9" s="39"/>
+      <c r="BW9" s="39"/>
+      <c r="BX9" s="39"/>
+      <c r="BY9" s="39"/>
+      <c r="BZ9" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="BY9" s="37"/>
-      <c r="BZ9" s="37"/>
-      <c r="CA9" s="37"/>
-      <c r="CB9" s="37"/>
+      <c r="CA9" s="39"/>
+      <c r="CB9" s="39"/>
+      <c r="CC9" s="39"/>
+      <c r="CD9" s="39"/>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
       <c r="Q10" s="16" t="s">
         <v>85</v>
       </c>
@@ -1608,113 +1626,119 @@
       <c r="W10" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="37"/>
-      <c r="AD10" s="37"/>
-      <c r="AE10" s="37"/>
-      <c r="AF10" s="16" t="s">
+      <c r="X10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
+      <c r="AG10" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AH10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AI10" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AJ10" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AK10" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AK10" s="16" t="s">
+      <c r="AL10" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AL10" s="17" t="s">
+      <c r="AM10" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="AM10" s="39"/>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="42"/>
-      <c r="AP10" s="42"/>
-      <c r="AQ10" s="39"/>
-      <c r="AR10" s="39"/>
-      <c r="AS10" s="39"/>
-      <c r="AT10" s="39"/>
-      <c r="AU10" s="37"/>
-      <c r="AV10" s="37"/>
-      <c r="AW10" s="37"/>
-      <c r="AX10" s="37"/>
-      <c r="AY10" s="37"/>
-      <c r="AZ10" s="37"/>
-      <c r="BA10" s="37"/>
-      <c r="BB10" s="37"/>
-      <c r="BC10" s="44"/>
-      <c r="BD10" s="37"/>
-      <c r="BE10" s="37"/>
-      <c r="BF10" s="37"/>
-      <c r="BG10" s="37"/>
-      <c r="BH10" s="37"/>
-      <c r="BI10" s="37"/>
-      <c r="BJ10" s="34" t="s">
+      <c r="AN10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="41"/>
+      <c r="AQ10" s="50"/>
+      <c r="AR10" s="50"/>
+      <c r="AS10" s="41"/>
+      <c r="AT10" s="41"/>
+      <c r="AU10" s="41"/>
+      <c r="AV10" s="41"/>
+      <c r="AW10" s="39"/>
+      <c r="AX10" s="39"/>
+      <c r="AY10" s="39"/>
+      <c r="AZ10" s="39"/>
+      <c r="BA10" s="39"/>
+      <c r="BB10" s="39"/>
+      <c r="BC10" s="39"/>
+      <c r="BD10" s="39"/>
+      <c r="BE10" s="52"/>
+      <c r="BF10" s="39"/>
+      <c r="BG10" s="39"/>
+      <c r="BH10" s="39"/>
+      <c r="BI10" s="39"/>
+      <c r="BJ10" s="39"/>
+      <c r="BK10" s="39"/>
+      <c r="BL10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="BK10" s="35" t="s">
+      <c r="BM10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BL10" s="45"/>
-      <c r="BM10" s="37"/>
-      <c r="BN10" s="10" t="s">
+      <c r="BN10" s="53"/>
+      <c r="BO10" s="39"/>
+      <c r="BP10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="BO10" s="10" t="s">
+      <c r="BQ10" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="BP10" s="10" t="s">
+      <c r="BR10" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="BQ10" s="10" t="s">
+      <c r="BS10" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BT10" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="BS10" s="10" t="s">
+      <c r="BU10" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="BT10" s="10" t="s">
+      <c r="BV10" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="BU10" s="10" t="s">
+      <c r="BW10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="BV10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CC10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="CB10" s="10" t="s">
+      <c r="CD10" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1764,7 +1788,7 @@
         <v>19</v>
       </c>
       <c r="Q11" s="27" t="e">
-        <f>R11+S11+T11+U11+V11+W11</f>
+        <f>R11+S11+T11+U11+V11+X11+W11</f>
         <v>#VALUE!</v>
       </c>
       <c r="R11" s="23" t="s">
@@ -1785,199 +1809,248 @@
       <c r="W11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="X11" s="15" t="s">
+      <c r="X11" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Y11" s="15" t="s">
+      <c r="Z11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="Z11" s="15" t="s">
+      <c r="AA11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AA11" s="15" t="s">
+      <c r="AB11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AB11" s="15" t="s">
+      <c r="AC11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AC11" s="15" t="s">
+      <c r="AD11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AD11" s="15" t="s">
+      <c r="AE11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AE11" s="15" t="s">
+      <c r="AF11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AF11" s="28" t="e">
-        <f>IF((AG11+AH11+AI11+AJ11+AK11+AL11)&gt;0,AG11+AH11+AI11+AJ11+AK11+AL11,)</f>
+      <c r="AG11" s="28" t="e">
+        <f>IF((AH11+AI11+AJ11+AK11+AL11+AN11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AN11+AM11,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AG11" s="23" t="s">
+      <c r="AH11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AH11" s="23" t="s">
+      <c r="AI11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AI11" s="23" t="s">
+      <c r="AJ11" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AJ11" s="23" t="s">
+      <c r="AK11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AK11" s="23" t="s">
+      <c r="AL11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AL11" s="23" t="s">
+      <c r="AM11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AM11" s="15" t="s">
+      <c r="AN11" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AN11" s="15" t="s">
+      <c r="AP11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AO11" s="24" t="s">
+      <c r="AQ11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AP11" s="24" t="s">
+      <c r="AR11" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AQ11" s="24" t="s">
+      <c r="AS11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AR11" s="15" t="s">
+      <c r="AT11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AS11" s="15" t="s">
+      <c r="AU11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="AT11" s="15" t="s">
+      <c r="AV11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AU11" s="15" t="s">
+      <c r="AW11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AV11" s="18" t="s">
+      <c r="AX11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AW11" s="18" t="s">
+      <c r="AY11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="AX11" s="19" t="s">
+      <c r="AZ11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="AY11" s="18" t="s">
+      <c r="BA11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="AZ11" s="29" t="e">
-        <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
+      <c r="BB11" s="29" t="e">
+        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA11" s="18" t="s">
+      <c r="BC11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="BB11" s="18" t="s">
+      <c r="BD11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="BC11" s="18" t="s">
+      <c r="BE11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BD11" s="29" t="e">
-        <f>IF(BH11&lt;=EOMONTH(AX11,12),"X","")</f>
+      <c r="BF11" s="29" t="e">
+        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE11" s="29" t="e">
-        <f>IF(AND(BH11&gt;=EOMONTH(AX11,13),BH11&lt;=EOMONTH(AX11,48)),"X","")</f>
+      <c r="BG11" s="29" t="e">
+        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,13),BJ11&lt;=EOMONTH(AZ11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BF11" s="29" t="e">
-        <f>IF(AND(BH11&gt;=EOMONTH(AX11,48),BH11&lt;=EOMONTH(AX11,72)),"X","")</f>
+      <c r="BH11" s="29" t="e">
+        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,48),BJ11&lt;=EOMONTH(AZ11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BG11" s="29" t="e">
-        <f>IF(BH11&gt;=EOMONTH(AX11,73),"X","")</f>
+      <c r="BI11" s="29" t="e">
+        <f>IF(BJ11&gt;=EOMONTH(AZ11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="19" t="s">
+      <c r="BJ11" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="BI11" s="19" t="s">
+      <c r="BK11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="BJ11" s="25" t="e">
-        <f>(EOMONTH(BH11,0))-(BH11-DAY(BH11)+1)+1</f>
+      <c r="BL11" s="25" t="e">
+        <f>(EOMONTH(BJ11,0))-(BJ11-DAY(BJ11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BK11" s="25" t="e">
-        <f>BI11-BH11+1</f>
+      <c r="BM11" s="25" t="e">
+        <f>BK11-BJ11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BL11" s="25" t="s">
+      <c r="BN11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="BM11" s="31" t="e">
-        <f>BK11/BJ11</f>
+      <c r="BO11" s="31" t="e">
+        <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="26" t="s">
+      <c r="BP11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="BO11" s="26" t="s">
+      <c r="BQ11" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="BP11" s="26" t="s">
+      <c r="BR11" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="BQ11" s="26" t="s">
+      <c r="BS11" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="BR11" s="26" t="s">
+      <c r="BT11" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="BS11" s="26" t="s">
+      <c r="BU11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="BT11" s="26" t="s">
+      <c r="BV11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="BU11" s="20" t="s">
+      <c r="BW11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BV11" s="52" t="s">
+      <c r="BX11" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="BW11" s="31" t="e">
-        <f>BT11*BM11</f>
+      <c r="BY11" s="31" t="e">
+        <f>BV11*BO11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BX11" s="20" t="s">
+      <c r="BZ11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="BY11" s="20" t="s">
+      <c r="CA11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="BZ11" s="20" t="s">
+      <c r="CB11" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="CA11" s="20" t="s">
+      <c r="CC11" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="CB11" s="21" t="s">
+      <c r="CD11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CC11" s="32" t="s">
+      <c r="CE11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="CD11" s="12"/>
+      <c r="CF11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="BP9:BY9"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AV10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="BJ8:CD8"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BZ9:CD9"/>
+    <mergeCell ref="AX8:BI8"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="AO8:AP8"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
@@ -1987,51 +2060,8 @@
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="AO8:AS8"/>
-    <mergeCell ref="AT8:AT10"/>
-    <mergeCell ref="AU8:AU10"/>
-    <mergeCell ref="BH8:CB8"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BX9:CB9"/>
-    <mergeCell ref="AV8:BG8"/>
-    <mergeCell ref="AF9:AJ9"/>
     <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BN9:BW9"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AF9:AF10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1044 Sozialhilfebezüger in Antragsteller-Kinder-Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CDB02-E782-4F90-ADE3-1636EF6B3E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A2D7C-C3B6-40A7-8C02-9D359498883E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="153">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>{gs1EwpFreiwillig}</t>
+  </si>
+  <si>
+    <t>{sozialhilfebezuegerTitle}</t>
+  </si>
+  <si>
+    <t>{sozialhilfebezueger}</t>
   </si>
 </sst>
 </file>
@@ -652,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -727,47 +733,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1179,66 +1197,66 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CF11"/>
+  <dimension ref="A1:CG11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.7109375"/>
-    <col min="17" max="18" width="10.7109375"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="41.42578125" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" customWidth="1"/>
-    <col min="24" max="24" width="24.140625"/>
-    <col min="25" max="32" width="8.7109375"/>
-    <col min="33" max="34" width="10.7109375"/>
-    <col min="35" max="35" width="24.5703125" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375"/>
-    <col min="37" max="37" width="14.42578125" customWidth="1"/>
-    <col min="38" max="38" width="41.42578125" customWidth="1"/>
-    <col min="39" max="39" width="27.140625" customWidth="1"/>
-    <col min="40" max="40" width="24.140625"/>
-    <col min="41" max="41" width="9.140625" customWidth="1"/>
-    <col min="42" max="42" width="6.42578125"/>
-    <col min="43" max="43" width="18.140625"/>
-    <col min="45" max="45" width="23.28515625"/>
-    <col min="46" max="46" width="9.28515625"/>
-    <col min="47" max="47" width="25.42578125"/>
-    <col min="48" max="48" width="27.42578125"/>
-    <col min="49" max="49" width="10.42578125"/>
-    <col min="50" max="52" width="12.7109375"/>
-    <col min="53" max="53" width="16.7109375"/>
-    <col min="54" max="54" width="12.7109375"/>
-    <col min="55" max="55" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="22"/>
-    <col min="57" max="57" width="18.140625" customWidth="1"/>
-    <col min="58" max="61" width="22"/>
-    <col min="62" max="63" width="12.7109375"/>
-    <col min="64" max="64" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="16" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="16" customWidth="1"/>
-    <col min="67" max="67" width="12.7109375"/>
-    <col min="68" max="69" width="13.28515625" customWidth="1"/>
-    <col min="70" max="70" width="13.7109375" customWidth="1"/>
-    <col min="71" max="71" width="16.85546875"/>
-    <col min="72" max="73" width="12.28515625" customWidth="1"/>
-    <col min="74" max="74" width="12.7109375"/>
-    <col min="75" max="75" width="19.42578125"/>
-    <col min="77" max="77" width="16.85546875"/>
-    <col min="78" max="79" width="12.7109375"/>
-    <col min="80" max="80" width="13.5703125" customWidth="1"/>
-    <col min="81" max="81" width="12.7109375" customWidth="1"/>
-    <col min="82" max="82" width="12.7109375"/>
-    <col min="83" max="1003" width="10.42578125"/>
+    <col min="9" max="16" width="8.6640625"/>
+    <col min="17" max="18" width="10.6640625"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625"/>
+    <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="22" max="22" width="41.44140625" customWidth="1"/>
+    <col min="23" max="23" width="26.88671875" customWidth="1"/>
+    <col min="24" max="24" width="24.109375"/>
+    <col min="25" max="32" width="8.6640625"/>
+    <col min="33" max="34" width="10.6640625"/>
+    <col min="35" max="35" width="24.5546875" customWidth="1"/>
+    <col min="36" max="36" width="10.6640625"/>
+    <col min="37" max="37" width="14.44140625" customWidth="1"/>
+    <col min="38" max="38" width="41.44140625" customWidth="1"/>
+    <col min="39" max="39" width="27.109375" customWidth="1"/>
+    <col min="40" max="40" width="24.109375"/>
+    <col min="41" max="41" width="9.109375" customWidth="1"/>
+    <col min="42" max="42" width="6.44140625"/>
+    <col min="43" max="43" width="18.109375"/>
+    <col min="45" max="45" width="23.33203125"/>
+    <col min="46" max="46" width="9.33203125"/>
+    <col min="47" max="47" width="25.44140625"/>
+    <col min="49" max="49" width="27.44140625"/>
+    <col min="50" max="50" width="10.44140625"/>
+    <col min="51" max="53" width="12.6640625"/>
+    <col min="54" max="54" width="16.6640625"/>
+    <col min="55" max="55" width="12.6640625"/>
+    <col min="56" max="56" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22"/>
+    <col min="58" max="58" width="18.109375" customWidth="1"/>
+    <col min="59" max="62" width="22"/>
+    <col min="63" max="64" width="12.6640625"/>
+    <col min="65" max="65" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="16" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="16" customWidth="1"/>
+    <col min="68" max="68" width="12.6640625"/>
+    <col min="69" max="70" width="13.33203125" customWidth="1"/>
+    <col min="71" max="71" width="13.6640625" customWidth="1"/>
+    <col min="72" max="72" width="16.88671875"/>
+    <col min="73" max="74" width="12.33203125" customWidth="1"/>
+    <col min="75" max="75" width="12.6640625"/>
+    <col min="76" max="76" width="19.44140625"/>
+    <col min="78" max="78" width="16.88671875"/>
+    <col min="79" max="80" width="12.6640625"/>
+    <col min="81" max="81" width="13.5546875" customWidth="1"/>
+    <col min="82" max="82" width="12.6640625" customWidth="1"/>
+    <col min="83" max="83" width="12.6640625"/>
+    <col min="84" max="1004" width="10.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:85" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1250,10 +1268,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -1264,11 +1282,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BL3" s="30"/>
       <c r="BM3" s="30"/>
       <c r="BN3" s="30"/>
+      <c r="BO3" s="30"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1277,7 +1295,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1286,7 +1304,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1299,17 +1317,17 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:84" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="52" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="38" t="s">
@@ -1337,14 +1355,14 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
       <c r="P8" s="39"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="40"/>
-      <c r="X8" s="40"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
       <c r="Y8" s="39" t="s">
         <v>92</v>
       </c>
@@ -1355,49 +1373,49 @@
       <c r="AD8" s="39"/>
       <c r="AE8" s="39"/>
       <c r="AF8" s="39"/>
-      <c r="AG8" s="40"/>
-      <c r="AH8" s="40"/>
-      <c r="AI8" s="40"/>
-      <c r="AJ8" s="40"/>
-      <c r="AK8" s="40"/>
-      <c r="AL8" s="40"/>
-      <c r="AM8" s="40"/>
-      <c r="AN8" s="40"/>
+      <c r="AG8" s="53"/>
+      <c r="AH8" s="53"/>
+      <c r="AI8" s="53"/>
+      <c r="AJ8" s="53"/>
+      <c r="AK8" s="53"/>
+      <c r="AL8" s="53"/>
+      <c r="AM8" s="53"/>
+      <c r="AN8" s="53"/>
       <c r="AO8" s="41" t="s">
         <v>93</v>
       </c>
       <c r="AP8" s="41"/>
-      <c r="AQ8" s="41" t="s">
+      <c r="AQ8" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="AR8" s="41"/>
-      <c r="AS8" s="41"/>
-      <c r="AT8" s="41"/>
-      <c r="AU8" s="41"/>
-      <c r="AV8" s="41" t="s">
+      <c r="AR8" s="55"/>
+      <c r="AS8" s="55"/>
+      <c r="AT8" s="55"/>
+      <c r="AU8" s="55"/>
+      <c r="AV8" s="40"/>
+      <c r="AW8" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="AW8" s="39" t="s">
+      <c r="AX8" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="AX8" s="42" t="s">
+      <c r="AY8" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="AY8" s="43"/>
-      <c r="AZ8" s="43"/>
-      <c r="BA8" s="43"/>
-      <c r="BB8" s="43"/>
-      <c r="BC8" s="43"/>
-      <c r="BD8" s="43"/>
-      <c r="BE8" s="43"/>
-      <c r="BF8" s="43"/>
-      <c r="BG8" s="43"/>
-      <c r="BH8" s="43"/>
-      <c r="BI8" s="46"/>
-      <c r="BJ8" s="39" t="s">
+      <c r="AZ8" s="49"/>
+      <c r="BA8" s="49"/>
+      <c r="BB8" s="49"/>
+      <c r="BC8" s="49"/>
+      <c r="BD8" s="49"/>
+      <c r="BE8" s="49"/>
+      <c r="BF8" s="49"/>
+      <c r="BG8" s="49"/>
+      <c r="BH8" s="49"/>
+      <c r="BI8" s="49"/>
+      <c r="BJ8" s="51"/>
+      <c r="BK8" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="BK8" s="39"/>
       <c r="BL8" s="39"/>
       <c r="BM8" s="39"/>
       <c r="BN8" s="39"/>
@@ -1417,11 +1435,12 @@
       <c r="CB8" s="39"/>
       <c r="CC8" s="39"/>
       <c r="CD8" s="39"/>
+      <c r="CE8" s="39"/>
     </row>
-    <row r="9" spans="1:84" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
-      <c r="C9" s="44"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
@@ -1448,16 +1467,16 @@
       <c r="O9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
       <c r="V9" s="33"/>
       <c r="W9" s="36"/>
       <c r="X9" s="13"/>
@@ -1482,96 +1501,98 @@
       <c r="AE9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="AF9" s="42" t="s">
+      <c r="AF9" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="AG9" s="42" t="s">
+      <c r="AG9" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="AH9" s="43"/>
-      <c r="AI9" s="43"/>
-      <c r="AJ9" s="43"/>
-      <c r="AK9" s="43"/>
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="49"/>
+      <c r="AJ9" s="49"/>
+      <c r="AK9" s="49"/>
       <c r="AL9" s="33"/>
       <c r="AM9" s="36"/>
       <c r="AN9" s="13"/>
-      <c r="AO9" s="47" t="s">
+      <c r="AO9" s="40" t="s">
         <v>94</v>
       </c>
       <c r="AP9" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="AQ9" s="49" t="s">
+      <c r="AQ9" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="AR9" s="49" t="s">
+      <c r="AR9" s="43" t="s">
         <v>98</v>
       </c>
       <c r="AS9" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="AT9" s="48" t="s">
+      <c r="AT9" s="42" t="s">
         <v>100</v>
       </c>
       <c r="AU9" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="AV9" s="41"/>
-      <c r="AW9" s="39"/>
-      <c r="AX9" s="39" t="s">
+      <c r="AV9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW9" s="41"/>
+      <c r="AX9" s="39"/>
+      <c r="AY9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AY9" s="39" t="s">
+      <c r="AZ9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="AZ9" s="39" t="s">
+      <c r="BA9" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="BA9" s="45" t="s">
+      <c r="BB9" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="BB9" s="39" t="s">
+      <c r="BC9" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="BC9" s="39" t="s">
+      <c r="BD9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="BD9" s="39" t="s">
+      <c r="BE9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="BE9" s="51" t="s">
+      <c r="BF9" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="BF9" s="39" t="s">
+      <c r="BG9" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="BG9" s="39" t="s">
+      <c r="BH9" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="BH9" s="39" t="s">
+      <c r="BI9" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="BI9" s="39" t="s">
+      <c r="BJ9" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="BJ9" s="39" t="s">
+      <c r="BK9" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="BK9" s="39" t="s">
+      <c r="BL9" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="BL9" s="34"/>
       <c r="BM9" s="34"/>
-      <c r="BN9" s="51" t="s">
+      <c r="BN9" s="34"/>
+      <c r="BO9" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="BO9" s="39" t="s">
+      <c r="BP9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="BP9" s="39" t="s">
+      <c r="BQ9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="BQ9" s="39"/>
       <c r="BR9" s="39"/>
       <c r="BS9" s="39"/>
       <c r="BT9" s="39"/>
@@ -1580,18 +1601,19 @@
       <c r="BW9" s="39"/>
       <c r="BX9" s="39"/>
       <c r="BY9" s="39"/>
-      <c r="BZ9" s="39" t="s">
+      <c r="BZ9" s="39"/>
+      <c r="CA9" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="CA9" s="39"/>
       <c r="CB9" s="39"/>
       <c r="CC9" s="39"/>
       <c r="CD9" s="39"/>
+      <c r="CE9" s="39"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
-      <c r="C10" s="44"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
@@ -1663,13 +1685,13 @@
       </c>
       <c r="AO10" s="41"/>
       <c r="AP10" s="41"/>
-      <c r="AQ10" s="50"/>
-      <c r="AR10" s="50"/>
+      <c r="AQ10" s="44"/>
+      <c r="AR10" s="44"/>
       <c r="AS10" s="41"/>
       <c r="AT10" s="41"/>
       <c r="AU10" s="41"/>
-      <c r="AV10" s="41"/>
-      <c r="AW10" s="39"/>
+      <c r="AV10" s="57"/>
+      <c r="AW10" s="41"/>
       <c r="AX10" s="39"/>
       <c r="AY10" s="39"/>
       <c r="AZ10" s="39"/>
@@ -1677,68 +1699,69 @@
       <c r="BB10" s="39"/>
       <c r="BC10" s="39"/>
       <c r="BD10" s="39"/>
-      <c r="BE10" s="52"/>
-      <c r="BF10" s="39"/>
+      <c r="BE10" s="39"/>
+      <c r="BF10" s="46"/>
       <c r="BG10" s="39"/>
       <c r="BH10" s="39"/>
       <c r="BI10" s="39"/>
       <c r="BJ10" s="39"/>
       <c r="BK10" s="39"/>
-      <c r="BL10" s="34" t="s">
+      <c r="BL10" s="39"/>
+      <c r="BM10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="BM10" s="35" t="s">
+      <c r="BN10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BN10" s="53"/>
-      <c r="BO10" s="39"/>
-      <c r="BP10" s="10" t="s">
+      <c r="BO10" s="47"/>
+      <c r="BP10" s="39"/>
+      <c r="BQ10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="BQ10" s="10" t="s">
+      <c r="BR10" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BS10" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="BS10" s="10" t="s">
+      <c r="BT10" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="BT10" s="10" t="s">
+      <c r="BU10" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="BU10" s="10" t="s">
+      <c r="BV10" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="BV10" s="10" t="s">
+      <c r="BW10" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="CB10" s="10" t="s">
+      <c r="CC10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="CC10" s="10" t="s">
+      <c r="CD10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="CD10" s="10" t="s">
+      <c r="CE10" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1883,169 +1906,131 @@
         <v>41</v>
       </c>
       <c r="AV11" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="AW11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AW11" s="15" t="s">
+      <c r="AX11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AX11" s="18" t="s">
+      <c r="AY11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AY11" s="18" t="s">
+      <c r="AZ11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="AZ11" s="19" t="s">
+      <c r="BA11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="BA11" s="18" t="s">
+      <c r="BB11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="BB11" s="29" t="e">
-        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
+      <c r="BC11" s="29" t="e">
+        <f>IF(BK11&lt;=EOMONTH(BA11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC11" s="18" t="s">
+      <c r="BD11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="BD11" s="18" t="s">
+      <c r="BE11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="BE11" s="18" t="s">
+      <c r="BF11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BF11" s="29" t="e">
-        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
+      <c r="BG11" s="29" t="e">
+        <f>IF(BK11&lt;=EOMONTH(BA11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BG11" s="29" t="e">
-        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,13),BJ11&lt;=EOMONTH(AZ11,48)),"X","")</f>
+      <c r="BH11" s="29" t="e">
+        <f>IF(AND(BK11&gt;=EOMONTH(BA11,13),BK11&lt;=EOMONTH(BA11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="29" t="e">
-        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,48),BJ11&lt;=EOMONTH(AZ11,72)),"X","")</f>
+      <c r="BI11" s="29" t="e">
+        <f>IF(AND(BK11&gt;=EOMONTH(BA11,48),BK11&lt;=EOMONTH(BA11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI11" s="29" t="e">
-        <f>IF(BJ11&gt;=EOMONTH(AZ11,73),"X","")</f>
+      <c r="BJ11" s="29" t="e">
+        <f>IF(BK11&gt;=EOMONTH(BA11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BJ11" s="19" t="s">
+      <c r="BK11" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="BK11" s="19" t="s">
+      <c r="BL11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="BL11" s="25" t="e">
-        <f>(EOMONTH(BJ11,0))-(BJ11-DAY(BJ11)+1)+1</f>
+      <c r="BM11" s="25" t="e">
+        <f>(EOMONTH(BK11,0))-(BK11-DAY(BK11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BM11" s="25" t="e">
-        <f>BK11-BJ11+1</f>
+      <c r="BN11" s="25" t="e">
+        <f>BL11-BK11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="25" t="s">
+      <c r="BO11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="BO11" s="31" t="e">
-        <f>BM11/BL11</f>
+      <c r="BP11" s="31" t="e">
+        <f>BN11/BM11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BP11" s="26" t="s">
+      <c r="BQ11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="BQ11" s="26" t="s">
+      <c r="BR11" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="BR11" s="26" t="s">
+      <c r="BS11" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="BS11" s="26" t="s">
+      <c r="BT11" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="BT11" s="26" t="s">
+      <c r="BU11" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="BU11" s="26" t="s">
+      <c r="BV11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="BV11" s="26" t="s">
+      <c r="BW11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="BW11" s="20" t="s">
+      <c r="BX11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BX11" s="37" t="s">
+      <c r="BY11" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="BY11" s="31" t="e">
-        <f>BV11*BO11</f>
+      <c r="BZ11" s="31" t="e">
+        <f>BW11*BP11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BZ11" s="20" t="s">
+      <c r="CA11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="CA11" s="20" t="s">
+      <c r="CB11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="CB11" s="20" t="s">
+      <c r="CC11" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="CC11" s="20" t="s">
+      <c r="CD11" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="CD11" s="21" t="s">
+      <c r="CE11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CE11" s="32" t="s">
+      <c r="CF11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="CF11" s="12"/>
+      <c r="CG11" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BP9:BY9"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AV10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="BJ8:CD8"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BZ9:CD9"/>
-    <mergeCell ref="AX8:BI8"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="60">
+    <mergeCell ref="AQ8:AV8"/>
+    <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:X8"/>
@@ -2062,6 +2047,48 @@
     <mergeCell ref="Q9:U9"/>
     <mergeCell ref="Y9:Y10"/>
     <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="AX8:AX10"/>
+    <mergeCell ref="BK8:CE8"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="CA9:CE9"/>
+    <mergeCell ref="AY8:BJ8"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="BQ9:BZ9"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="AE9:AE10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1699 add "Integration" to AntragstellerKinderStatistik and KinderStatistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A2D7C-C3B6-40A7-8C02-9D359498883E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF9CC2-0DC0-4DF5-9FBC-749B4C752231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="12675" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="155">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>{sozialhilfebezueger}</t>
+  </si>
+  <si>
+    <t>{kindIntegrationTitle}</t>
+  </si>
+  <si>
+    <t>{kindIntegration}</t>
   </si>
 </sst>
 </file>
@@ -727,18 +733,51 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -748,44 +787,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1197,66 +1203,67 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CG11"/>
+  <dimension ref="A1:CH11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625"/>
-    <col min="3" max="3" width="15.6640625" style="1"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.6640625"/>
-    <col min="17" max="18" width="10.6640625"/>
-    <col min="19" max="19" width="24.33203125" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
-    <col min="22" max="22" width="41.44140625" customWidth="1"/>
-    <col min="23" max="23" width="26.88671875" customWidth="1"/>
-    <col min="24" max="24" width="24.109375"/>
-    <col min="25" max="32" width="8.6640625"/>
-    <col min="33" max="34" width="10.6640625"/>
-    <col min="35" max="35" width="24.5546875" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625"/>
-    <col min="37" max="37" width="14.44140625" customWidth="1"/>
-    <col min="38" max="38" width="41.44140625" customWidth="1"/>
-    <col min="39" max="39" width="27.109375" customWidth="1"/>
-    <col min="40" max="40" width="24.109375"/>
-    <col min="41" max="41" width="9.109375" customWidth="1"/>
-    <col min="42" max="42" width="6.44140625"/>
-    <col min="43" max="43" width="18.109375"/>
-    <col min="45" max="45" width="23.33203125"/>
-    <col min="46" max="46" width="9.33203125"/>
-    <col min="47" max="47" width="25.44140625"/>
-    <col min="49" max="49" width="27.44140625"/>
-    <col min="50" max="50" width="10.44140625"/>
-    <col min="51" max="53" width="12.6640625"/>
-    <col min="54" max="54" width="16.6640625"/>
-    <col min="55" max="55" width="12.6640625"/>
-    <col min="56" max="56" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22"/>
-    <col min="58" max="58" width="18.109375" customWidth="1"/>
-    <col min="59" max="62" width="22"/>
-    <col min="63" max="64" width="12.6640625"/>
-    <col min="65" max="65" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="16" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="16" customWidth="1"/>
-    <col min="68" max="68" width="12.6640625"/>
-    <col min="69" max="70" width="13.33203125" customWidth="1"/>
-    <col min="71" max="71" width="13.6640625" customWidth="1"/>
-    <col min="72" max="72" width="16.88671875"/>
-    <col min="73" max="74" width="12.33203125" customWidth="1"/>
-    <col min="75" max="75" width="12.6640625"/>
-    <col min="76" max="76" width="19.44140625"/>
-    <col min="78" max="78" width="16.88671875"/>
-    <col min="79" max="80" width="12.6640625"/>
-    <col min="81" max="81" width="13.5546875" customWidth="1"/>
-    <col min="82" max="82" width="12.6640625" customWidth="1"/>
-    <col min="83" max="83" width="12.6640625"/>
-    <col min="84" max="1004" width="10.44140625"/>
+    <col min="9" max="16" width="8.7109375"/>
+    <col min="17" max="18" width="10.7109375"/>
+    <col min="19" max="19" width="24.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375"/>
+    <col min="21" max="21" width="14.42578125" customWidth="1"/>
+    <col min="22" max="22" width="41.42578125" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="24.140625"/>
+    <col min="25" max="32" width="8.7109375"/>
+    <col min="33" max="34" width="10.7109375"/>
+    <col min="35" max="35" width="24.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375"/>
+    <col min="37" max="37" width="14.42578125" customWidth="1"/>
+    <col min="38" max="38" width="41.42578125" customWidth="1"/>
+    <col min="39" max="39" width="27.140625" customWidth="1"/>
+    <col min="40" max="40" width="24.140625"/>
+    <col min="41" max="41" width="9.140625" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125"/>
+    <col min="43" max="43" width="18.140625"/>
+    <col min="45" max="45" width="23.28515625"/>
+    <col min="46" max="46" width="9.28515625"/>
+    <col min="47" max="47" width="25.42578125"/>
+    <col min="49" max="49" width="27.42578125"/>
+    <col min="50" max="50" width="10.42578125"/>
+    <col min="51" max="53" width="12.7109375"/>
+    <col min="54" max="54" width="16.7109375"/>
+    <col min="55" max="55" width="20.5703125" customWidth="1"/>
+    <col min="56" max="56" width="12.7109375"/>
+    <col min="57" max="57" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="22"/>
+    <col min="59" max="59" width="18.140625" customWidth="1"/>
+    <col min="60" max="63" width="22"/>
+    <col min="64" max="65" width="12.7109375"/>
+    <col min="66" max="66" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="16" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="16" customWidth="1"/>
+    <col min="69" max="69" width="12.7109375"/>
+    <col min="70" max="71" width="13.28515625" customWidth="1"/>
+    <col min="72" max="72" width="13.7109375" customWidth="1"/>
+    <col min="73" max="73" width="16.85546875"/>
+    <col min="74" max="75" width="12.28515625" customWidth="1"/>
+    <col min="76" max="76" width="12.7109375"/>
+    <col min="77" max="77" width="19.42578125"/>
+    <col min="79" max="79" width="16.85546875"/>
+    <col min="80" max="81" width="12.7109375"/>
+    <col min="82" max="82" width="13.5703125" customWidth="1"/>
+    <col min="83" max="83" width="12.7109375" customWidth="1"/>
+    <col min="84" max="84" width="12.7109375"/>
+    <col min="85" max="1005" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:86" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1268,10 +1275,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:86" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -1282,11 +1289,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BM3" s="30"/>
       <c r="BN3" s="30"/>
       <c r="BO3" s="30"/>
+      <c r="BP3" s="30"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1295,7 +1302,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1304,7 +1311,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1317,316 +1324,320 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:85" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:86" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
-      <c r="U8" s="53"/>
-      <c r="V8" s="53"/>
-      <c r="W8" s="53"/>
-      <c r="X8" s="53"/>
-      <c r="Y8" s="39" t="s">
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="53"/>
-      <c r="AH8" s="53"/>
-      <c r="AI8" s="53"/>
-      <c r="AJ8" s="53"/>
-      <c r="AK8" s="53"/>
-      <c r="AL8" s="53"/>
-      <c r="AM8" s="53"/>
-      <c r="AN8" s="53"/>
-      <c r="AO8" s="41" t="s">
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="46"/>
+      <c r="AB8" s="46"/>
+      <c r="AC8" s="46"/>
+      <c r="AD8" s="46"/>
+      <c r="AE8" s="46"/>
+      <c r="AF8" s="46"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+      <c r="AJ8" s="47"/>
+      <c r="AK8" s="47"/>
+      <c r="AL8" s="47"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="47"/>
+      <c r="AO8" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="AP8" s="41"/>
-      <c r="AQ8" s="54" t="s">
+      <c r="AP8" s="48"/>
+      <c r="AQ8" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="AR8" s="55"/>
-      <c r="AS8" s="55"/>
-      <c r="AT8" s="55"/>
-      <c r="AU8" s="55"/>
-      <c r="AV8" s="40"/>
-      <c r="AW8" s="41" t="s">
+      <c r="AR8" s="42"/>
+      <c r="AS8" s="42"/>
+      <c r="AT8" s="42"/>
+      <c r="AU8" s="42"/>
+      <c r="AV8" s="43"/>
+      <c r="AW8" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="AX8" s="39" t="s">
+      <c r="AX8" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="AY8" s="48" t="s">
+      <c r="AY8" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="AZ8" s="49"/>
-      <c r="BA8" s="49"/>
-      <c r="BB8" s="49"/>
-      <c r="BC8" s="49"/>
-      <c r="BD8" s="49"/>
-      <c r="BE8" s="49"/>
-      <c r="BF8" s="49"/>
-      <c r="BG8" s="49"/>
-      <c r="BH8" s="49"/>
-      <c r="BI8" s="49"/>
-      <c r="BJ8" s="51"/>
-      <c r="BK8" s="39" t="s">
+      <c r="AZ8" s="39"/>
+      <c r="BA8" s="39"/>
+      <c r="BB8" s="39"/>
+      <c r="BC8" s="39"/>
+      <c r="BD8" s="39"/>
+      <c r="BE8" s="39"/>
+      <c r="BF8" s="39"/>
+      <c r="BG8" s="39"/>
+      <c r="BH8" s="39"/>
+      <c r="BI8" s="39"/>
+      <c r="BJ8" s="39"/>
+      <c r="BK8" s="50"/>
+      <c r="BL8" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="BL8" s="39"/>
-      <c r="BM8" s="39"/>
-      <c r="BN8" s="39"/>
-      <c r="BO8" s="39"/>
-      <c r="BP8" s="39"/>
-      <c r="BQ8" s="39"/>
-      <c r="BR8" s="39"/>
-      <c r="BS8" s="39"/>
-      <c r="BT8" s="39"/>
-      <c r="BU8" s="39"/>
-      <c r="BV8" s="39"/>
-      <c r="BW8" s="39"/>
-      <c r="BX8" s="39"/>
-      <c r="BY8" s="39"/>
-      <c r="BZ8" s="39"/>
-      <c r="CA8" s="39"/>
-      <c r="CB8" s="39"/>
-      <c r="CC8" s="39"/>
-      <c r="CD8" s="39"/>
-      <c r="CE8" s="39"/>
+      <c r="BM8" s="46"/>
+      <c r="BN8" s="46"/>
+      <c r="BO8" s="46"/>
+      <c r="BP8" s="46"/>
+      <c r="BQ8" s="46"/>
+      <c r="BR8" s="46"/>
+      <c r="BS8" s="46"/>
+      <c r="BT8" s="46"/>
+      <c r="BU8" s="46"/>
+      <c r="BV8" s="46"/>
+      <c r="BW8" s="46"/>
+      <c r="BX8" s="46"/>
+      <c r="BY8" s="46"/>
+      <c r="BZ8" s="46"/>
+      <c r="CA8" s="46"/>
+      <c r="CB8" s="46"/>
+      <c r="CC8" s="46"/>
+      <c r="CD8" s="46"/>
+      <c r="CE8" s="46"/>
+      <c r="CF8" s="46"/>
     </row>
-    <row r="9" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39" t="s">
+    <row r="9" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="48" t="s">
+      <c r="P9" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="48" t="s">
+      <c r="Q9" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
       <c r="V9" s="33"/>
       <c r="W9" s="36"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="39" t="s">
+      <c r="Y9" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="Z9" s="39" t="s">
+      <c r="Z9" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="AA9" s="39" t="s">
+      <c r="AA9" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="AB9" s="39" t="s">
+      <c r="AB9" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="AC9" s="39" t="s">
+      <c r="AC9" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="AD9" s="39" t="s">
+      <c r="AD9" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="39" t="s">
+      <c r="AE9" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="AF9" s="48" t="s">
+      <c r="AF9" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="AG9" s="48" t="s">
+      <c r="AG9" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="AH9" s="49"/>
-      <c r="AI9" s="49"/>
-      <c r="AJ9" s="49"/>
-      <c r="AK9" s="49"/>
+      <c r="AH9" s="39"/>
+      <c r="AI9" s="39"/>
+      <c r="AJ9" s="39"/>
+      <c r="AK9" s="39"/>
       <c r="AL9" s="33"/>
       <c r="AM9" s="36"/>
       <c r="AN9" s="13"/>
-      <c r="AO9" s="40" t="s">
+      <c r="AO9" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="AP9" s="41" t="s">
+      <c r="AP9" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AQ9" s="43" t="s">
+      <c r="AQ9" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="AR9" s="43" t="s">
+      <c r="AR9" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="AS9" s="41" t="s">
+      <c r="AS9" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AT9" s="42" t="s">
+      <c r="AT9" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="AU9" s="41" t="s">
+      <c r="AU9" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="AV9" s="56" t="s">
+      <c r="AV9" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="AW9" s="41"/>
-      <c r="AX9" s="39"/>
-      <c r="AY9" s="39" t="s">
+      <c r="AW9" s="48"/>
+      <c r="AX9" s="46"/>
+      <c r="AY9" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="AZ9" s="39" t="s">
+      <c r="AZ9" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="BA9" s="39" t="s">
+      <c r="BA9" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="BB9" s="50" t="s">
+      <c r="BB9" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="BC9" s="39" t="s">
+      <c r="BC9" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="BD9" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="BD9" s="39" t="s">
+      <c r="BE9" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="BE9" s="39" t="s">
+      <c r="BF9" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="BF9" s="45" t="s">
+      <c r="BG9" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="BG9" s="39" t="s">
+      <c r="BH9" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="BH9" s="39" t="s">
+      <c r="BI9" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="BI9" s="39" t="s">
+      <c r="BJ9" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="BJ9" s="39" t="s">
+      <c r="BK9" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="BK9" s="39" t="s">
+      <c r="BL9" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="BL9" s="39" t="s">
+      <c r="BM9" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="BM9" s="34"/>
       <c r="BN9" s="34"/>
-      <c r="BO9" s="45" t="s">
+      <c r="BO9" s="34"/>
+      <c r="BP9" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="BP9" s="39" t="s">
+      <c r="BQ9" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="BQ9" s="39" t="s">
+      <c r="BR9" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="BR9" s="39"/>
-      <c r="BS9" s="39"/>
-      <c r="BT9" s="39"/>
-      <c r="BU9" s="39"/>
-      <c r="BV9" s="39"/>
-      <c r="BW9" s="39"/>
-      <c r="BX9" s="39"/>
-      <c r="BY9" s="39"/>
-      <c r="BZ9" s="39"/>
-      <c r="CA9" s="39" t="s">
+      <c r="BS9" s="46"/>
+      <c r="BT9" s="46"/>
+      <c r="BU9" s="46"/>
+      <c r="BV9" s="46"/>
+      <c r="BW9" s="46"/>
+      <c r="BX9" s="46"/>
+      <c r="BY9" s="46"/>
+      <c r="BZ9" s="46"/>
+      <c r="CA9" s="46"/>
+      <c r="CB9" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="CB9" s="39"/>
-      <c r="CC9" s="39"/>
-      <c r="CD9" s="39"/>
-      <c r="CE9" s="39"/>
+      <c r="CC9" s="46"/>
+      <c r="CD9" s="46"/>
+      <c r="CE9" s="46"/>
+      <c r="CF9" s="46"/>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
+    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
       <c r="Q10" s="16" t="s">
         <v>85</v>
       </c>
@@ -1651,14 +1662,14 @@
       <c r="X10" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="46"/>
+      <c r="AB10" s="46"/>
+      <c r="AC10" s="46"/>
+      <c r="AD10" s="46"/>
+      <c r="AE10" s="46"/>
+      <c r="AF10" s="46"/>
       <c r="AG10" s="16" t="s">
         <v>85</v>
       </c>
@@ -1683,85 +1694,86 @@
       <c r="AN10" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="AO10" s="41"/>
-      <c r="AP10" s="41"/>
-      <c r="AQ10" s="44"/>
-      <c r="AR10" s="44"/>
-      <c r="AS10" s="41"/>
-      <c r="AT10" s="41"/>
-      <c r="AU10" s="41"/>
-      <c r="AV10" s="57"/>
-      <c r="AW10" s="41"/>
-      <c r="AX10" s="39"/>
-      <c r="AY10" s="39"/>
-      <c r="AZ10" s="39"/>
-      <c r="BA10" s="39"/>
-      <c r="BB10" s="39"/>
-      <c r="BC10" s="39"/>
-      <c r="BD10" s="39"/>
-      <c r="BE10" s="39"/>
+      <c r="AO10" s="48"/>
+      <c r="AP10" s="48"/>
+      <c r="AQ10" s="55"/>
+      <c r="AR10" s="55"/>
+      <c r="AS10" s="48"/>
+      <c r="AT10" s="48"/>
+      <c r="AU10" s="48"/>
+      <c r="AV10" s="45"/>
+      <c r="AW10" s="48"/>
+      <c r="AX10" s="46"/>
+      <c r="AY10" s="46"/>
+      <c r="AZ10" s="46"/>
+      <c r="BA10" s="46"/>
+      <c r="BB10" s="46"/>
+      <c r="BC10" s="46"/>
+      <c r="BD10" s="46"/>
+      <c r="BE10" s="46"/>
       <c r="BF10" s="46"/>
-      <c r="BG10" s="39"/>
-      <c r="BH10" s="39"/>
-      <c r="BI10" s="39"/>
-      <c r="BJ10" s="39"/>
-      <c r="BK10" s="39"/>
-      <c r="BL10" s="39"/>
-      <c r="BM10" s="34" t="s">
+      <c r="BG10" s="57"/>
+      <c r="BH10" s="46"/>
+      <c r="BI10" s="46"/>
+      <c r="BJ10" s="46"/>
+      <c r="BK10" s="46"/>
+      <c r="BL10" s="46"/>
+      <c r="BM10" s="46"/>
+      <c r="BN10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="BN10" s="35" t="s">
+      <c r="BO10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BO10" s="47"/>
-      <c r="BP10" s="39"/>
-      <c r="BQ10" s="10" t="s">
+      <c r="BP10" s="52"/>
+      <c r="BQ10" s="46"/>
+      <c r="BR10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BS10" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="BS10" s="10" t="s">
+      <c r="BT10" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="BT10" s="10" t="s">
+      <c r="BU10" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="BU10" s="10" t="s">
+      <c r="BV10" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="BV10" s="10" t="s">
+      <c r="BW10" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="CB10" s="10" t="s">
+      <c r="CC10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="CC10" s="10" t="s">
+      <c r="CD10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="CD10" s="10" t="s">
+      <c r="CE10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="CE10" s="10" t="s">
+      <c r="CF10" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1926,109 +1938,159 @@
       <c r="BB11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="BC11" s="29" t="e">
-        <f>IF(BK11&lt;=EOMONTH(BA11,12),"X","")</f>
+      <c r="BC11" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="BD11" s="29" t="e">
+        <f>IF(BL11&lt;=EOMONTH(BA11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BD11" s="18" t="s">
+      <c r="BE11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="BE11" s="18" t="s">
+      <c r="BF11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="BF11" s="18" t="s">
+      <c r="BG11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BG11" s="29" t="e">
-        <f>IF(BK11&lt;=EOMONTH(BA11,12),"X","")</f>
+      <c r="BH11" s="29" t="e">
+        <f>IF(BL11&lt;=EOMONTH(BA11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="29" t="e">
-        <f>IF(AND(BK11&gt;=EOMONTH(BA11,13),BK11&lt;=EOMONTH(BA11,48)),"X","")</f>
+      <c r="BI11" s="29" t="e">
+        <f>IF(AND(BL11&gt;=EOMONTH(BA11,13),BL11&lt;=EOMONTH(BA11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI11" s="29" t="e">
-        <f>IF(AND(BK11&gt;=EOMONTH(BA11,48),BK11&lt;=EOMONTH(BA11,72)),"X","")</f>
+      <c r="BJ11" s="29" t="e">
+        <f>IF(AND(BL11&gt;=EOMONTH(BA11,48),BL11&lt;=EOMONTH(BA11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BJ11" s="29" t="e">
-        <f>IF(BK11&gt;=EOMONTH(BA11,73),"X","")</f>
+      <c r="BK11" s="29" t="e">
+        <f>IF(BL11&gt;=EOMONTH(BA11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BK11" s="19" t="s">
+      <c r="BL11" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="BL11" s="19" t="s">
+      <c r="BM11" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="BM11" s="25" t="e">
-        <f>(EOMONTH(BK11,0))-(BK11-DAY(BK11)+1)+1</f>
+      <c r="BN11" s="25" t="e">
+        <f>(EOMONTH(BL11,0))-(BL11-DAY(BL11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="25" t="e">
-        <f>BL11-BK11+1</f>
+      <c r="BO11" s="25" t="e">
+        <f>BM11-BL11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="25" t="s">
+      <c r="BP11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="BP11" s="31" t="e">
-        <f>BN11/BM11</f>
+      <c r="BQ11" s="31" t="e">
+        <f>BO11/BN11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BQ11" s="26" t="s">
+      <c r="BR11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="BR11" s="26" t="s">
+      <c r="BS11" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="BS11" s="26" t="s">
+      <c r="BT11" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="BT11" s="26" t="s">
+      <c r="BU11" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="BU11" s="26" t="s">
+      <c r="BV11" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="BV11" s="26" t="s">
+      <c r="BW11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="BW11" s="26" t="s">
+      <c r="BX11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="BX11" s="20" t="s">
+      <c r="BY11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BY11" s="37" t="s">
+      <c r="BZ11" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="BZ11" s="31" t="e">
-        <f>BW11*BP11</f>
+      <c r="CA11" s="31" t="e">
+        <f>BX11*BQ11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="CA11" s="20" t="s">
+      <c r="CB11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="CB11" s="20" t="s">
+      <c r="CC11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="CC11" s="20" t="s">
+      <c r="CD11" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="CD11" s="20" t="s">
+      <c r="CE11" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="CE11" s="21" t="s">
+      <c r="CF11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CF11" s="32" t="s">
+      <c r="CG11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="CG11" s="12"/>
+      <c r="CH11" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="61">
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="AX8:AX10"/>
+    <mergeCell ref="BL8:CF8"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="CB9:CF9"/>
+    <mergeCell ref="AY8:BK8"/>
+    <mergeCell ref="BR9:CA9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="BQ9:BQ10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="G8:G10"/>
     <mergeCell ref="AQ8:AV8"/>
     <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="F8:F10"/>
@@ -2043,52 +2105,6 @@
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="AX8:AX10"/>
-    <mergeCell ref="BK8:CE8"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="CA9:CE9"/>
-    <mergeCell ref="AY8:BJ8"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="BQ9:BZ9"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="AE9:AE10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1946: Ergänzt die Report mit genaue EKV Informationen und nimmt der Anfang Jahr anstatt der basis für TagesschuleRechnungstellung
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF9CC2-0DC0-4DF5-9FBC-749B4C752231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E944BB8-EC3D-4BD3-A719-7DC19D112C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="12675" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="161">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -158,9 +158,6 @@
     <t>{einkommensjahr}</t>
   </si>
   <si>
-    <t>{ekvVorhanden}</t>
-  </si>
-  <si>
     <t>{stvGeprueft}</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>{einkommensjahrTitle}</t>
   </si>
   <si>
-    <t>{einkommensverschlechterungTitle}</t>
-  </si>
-  <si>
     <t>{geprueftSTVTitle}</t>
   </si>
   <si>
@@ -498,6 +492,30 @@
   </si>
   <si>
     <t>{kindIntegration}</t>
+  </si>
+  <si>
+    <t>{ekvVorhandenBasisJahr1}</t>
+  </si>
+  <si>
+    <t>{ekvVorhandenBasisJahr2}</t>
+  </si>
+  <si>
+    <t>{ekvAnnuliertBasisJahr1}</t>
+  </si>
+  <si>
+    <t>{ekvAnnuliertBasisJahr2}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr1Title}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr2Title}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr1AnnuliertTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr2AnnuliertTitle}</t>
   </si>
 </sst>
 </file>
@@ -664,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -733,65 +751,71 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1203,9 +1227,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CH11"/>
+  <dimension ref="A1:CK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV18" sqref="AV18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1234,38 +1260,40 @@
     <col min="45" max="45" width="23.28515625"/>
     <col min="46" max="46" width="9.28515625"/>
     <col min="47" max="47" width="25.42578125"/>
-    <col min="49" max="49" width="27.42578125"/>
-    <col min="50" max="50" width="10.42578125"/>
-    <col min="51" max="53" width="12.7109375"/>
-    <col min="54" max="54" width="16.7109375"/>
-    <col min="55" max="55" width="20.5703125" customWidth="1"/>
-    <col min="56" max="56" width="12.7109375"/>
-    <col min="57" max="57" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="22"/>
-    <col min="59" max="59" width="18.140625" customWidth="1"/>
-    <col min="60" max="63" width="22"/>
-    <col min="64" max="65" width="12.7109375"/>
-    <col min="66" max="66" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="16" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="16" customWidth="1"/>
-    <col min="69" max="69" width="12.7109375"/>
-    <col min="70" max="71" width="13.28515625" customWidth="1"/>
-    <col min="72" max="72" width="13.7109375" customWidth="1"/>
-    <col min="73" max="73" width="16.85546875"/>
-    <col min="74" max="75" width="12.28515625" customWidth="1"/>
-    <col min="76" max="76" width="12.7109375"/>
-    <col min="77" max="77" width="19.42578125"/>
-    <col min="79" max="79" width="16.85546875"/>
-    <col min="80" max="81" width="12.7109375"/>
-    <col min="82" max="82" width="13.5703125" customWidth="1"/>
-    <col min="83" max="83" width="12.7109375" customWidth="1"/>
-    <col min="84" max="84" width="12.7109375"/>
-    <col min="85" max="1005" width="10.42578125"/>
+    <col min="48" max="48" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="27.42578125"/>
+    <col min="53" max="53" width="10.42578125"/>
+    <col min="54" max="56" width="12.7109375"/>
+    <col min="57" max="57" width="16.7109375"/>
+    <col min="58" max="58" width="20.5703125" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375"/>
+    <col min="60" max="60" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22"/>
+    <col min="62" max="62" width="18.140625" customWidth="1"/>
+    <col min="63" max="66" width="22"/>
+    <col min="67" max="68" width="12.7109375"/>
+    <col min="69" max="69" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="16" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="16" customWidth="1"/>
+    <col min="72" max="72" width="12.7109375"/>
+    <col min="73" max="74" width="13.28515625" customWidth="1"/>
+    <col min="75" max="75" width="13.7109375" customWidth="1"/>
+    <col min="76" max="76" width="16.85546875"/>
+    <col min="77" max="78" width="12.28515625" customWidth="1"/>
+    <col min="79" max="79" width="12.7109375"/>
+    <col min="80" max="80" width="19.42578125"/>
+    <col min="82" max="82" width="16.85546875"/>
+    <col min="83" max="84" width="12.7109375"/>
+    <col min="85" max="85" width="13.5703125" customWidth="1"/>
+    <col min="86" max="86" width="12.7109375" customWidth="1"/>
+    <col min="87" max="87" width="12.7109375"/>
+    <col min="88" max="1008" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:89" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1275,12 +1303,12 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1289,31 +1317,31 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BN3" s="30"/>
-      <c r="BO3" s="30"/>
-      <c r="BP3" s="30"/>
+      <c r="BQ3" s="30"/>
+      <c r="BR3" s="30"/>
+      <c r="BS3" s="30"/>
     </row>
-    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -1324,456 +1352,471 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:86" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:89" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="C8" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="40" t="s">
+      <c r="E8" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="F8" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="G8" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="40" t="s">
+      <c r="I8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
+      <c r="Y8" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="57"/>
+      <c r="AH8" s="57"/>
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="57"/>
+      <c r="AK8" s="57"/>
+      <c r="AL8" s="57"/>
+      <c r="AM8" s="57"/>
+      <c r="AN8" s="57"/>
+      <c r="AO8" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP8" s="39"/>
+      <c r="AQ8" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR8" s="54"/>
+      <c r="AS8" s="54"/>
+      <c r="AT8" s="54"/>
+      <c r="AU8" s="54"/>
+      <c r="AV8" s="54"/>
+      <c r="AW8" s="54"/>
+      <c r="AX8" s="54"/>
+      <c r="AY8" s="50"/>
+      <c r="AZ8" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA8" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB8" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC8" s="47"/>
+      <c r="BD8" s="47"/>
+      <c r="BE8" s="47"/>
+      <c r="BF8" s="47"/>
+      <c r="BG8" s="47"/>
+      <c r="BH8" s="47"/>
+      <c r="BI8" s="47"/>
+      <c r="BJ8" s="47"/>
+      <c r="BK8" s="47"/>
+      <c r="BL8" s="47"/>
+      <c r="BM8" s="47"/>
+      <c r="BN8" s="48"/>
+      <c r="BO8" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="BP8" s="38"/>
+      <c r="BQ8" s="38"/>
+      <c r="BR8" s="38"/>
+      <c r="BS8" s="38"/>
+      <c r="BT8" s="38"/>
+      <c r="BU8" s="38"/>
+      <c r="BV8" s="38"/>
+      <c r="BW8" s="38"/>
+      <c r="BX8" s="38"/>
+      <c r="BY8" s="38"/>
+      <c r="BZ8" s="38"/>
+      <c r="CA8" s="38"/>
+      <c r="CB8" s="38"/>
+      <c r="CC8" s="38"/>
+      <c r="CD8" s="38"/>
+      <c r="CE8" s="38"/>
+      <c r="CF8" s="38"/>
+      <c r="CG8" s="38"/>
+      <c r="CH8" s="38"/>
+      <c r="CI8" s="38"/>
+    </row>
+    <row r="9" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46"/>
-      <c r="AG8" s="47"/>
-      <c r="AH8" s="47"/>
-      <c r="AI8" s="47"/>
-      <c r="AJ8" s="47"/>
-      <c r="AK8" s="47"/>
-      <c r="AL8" s="47"/>
-      <c r="AM8" s="47"/>
-      <c r="AN8" s="47"/>
-      <c r="AO8" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR8" s="42"/>
-      <c r="AS8" s="42"/>
-      <c r="AT8" s="42"/>
-      <c r="AU8" s="42"/>
-      <c r="AV8" s="43"/>
-      <c r="AW8" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX8" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="AY8" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="AZ8" s="39"/>
-      <c r="BA8" s="39"/>
-      <c r="BB8" s="39"/>
-      <c r="BC8" s="39"/>
-      <c r="BD8" s="39"/>
-      <c r="BE8" s="39"/>
-      <c r="BF8" s="39"/>
-      <c r="BG8" s="39"/>
-      <c r="BH8" s="39"/>
-      <c r="BI8" s="39"/>
-      <c r="BJ8" s="39"/>
-      <c r="BK8" s="50"/>
-      <c r="BL8" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM8" s="46"/>
-      <c r="BN8" s="46"/>
-      <c r="BO8" s="46"/>
-      <c r="BP8" s="46"/>
-      <c r="BQ8" s="46"/>
-      <c r="BR8" s="46"/>
-      <c r="BS8" s="46"/>
-      <c r="BT8" s="46"/>
-      <c r="BU8" s="46"/>
-      <c r="BV8" s="46"/>
-      <c r="BW8" s="46"/>
-      <c r="BX8" s="46"/>
-      <c r="BY8" s="46"/>
-      <c r="BZ8" s="46"/>
-      <c r="CA8" s="46"/>
-      <c r="CB8" s="46"/>
-      <c r="CC8" s="46"/>
-      <c r="CD8" s="46"/>
-      <c r="CE8" s="46"/>
-      <c r="CF8" s="46"/>
-    </row>
-    <row r="9" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="46" t="s">
+      <c r="J9" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="K9" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="L9" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="M9" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="N9" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="46" t="s">
+      <c r="O9" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="O9" s="46" t="s">
+      <c r="P9" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="38" t="s">
+      <c r="Q9" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
       <c r="V9" s="33"/>
       <c r="W9" s="36"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="46" t="s">
+      <c r="Y9" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z9" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="Z9" s="46" t="s">
+      <c r="AA9" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="AA9" s="46" t="s">
+      <c r="AB9" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="AB9" s="46" t="s">
+      <c r="AC9" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="AC9" s="46" t="s">
+      <c r="AD9" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="AD9" s="46" t="s">
+      <c r="AE9" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="46" t="s">
+      <c r="AF9" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="AF9" s="38" t="s">
+      <c r="AG9" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="AG9" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH9" s="39"/>
-      <c r="AI9" s="39"/>
-      <c r="AJ9" s="39"/>
-      <c r="AK9" s="39"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
+      <c r="AK9" s="47"/>
       <c r="AL9" s="33"/>
       <c r="AM9" s="36"/>
       <c r="AN9" s="13"/>
-      <c r="AO9" s="43" t="s">
+      <c r="AO9" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP9" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="AP9" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ9" s="54" t="s">
+      <c r="AQ9" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR9" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="AR9" s="54" t="s">
+      <c r="AS9" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="AS9" s="48" t="s">
+      <c r="AT9" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="AT9" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU9" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV9" s="44" t="s">
+      <c r="AU9" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="AV9" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="AW9" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="AX9" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="AY9" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ9" s="39"/>
+      <c r="BA9" s="38"/>
+      <c r="BB9" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC9" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD9" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="BE9" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="BF9" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="AW9" s="48"/>
-      <c r="AX9" s="46"/>
-      <c r="AY9" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="AZ9" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="BA9" s="46" t="s">
+      <c r="BG9" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="BB9" s="56" t="s">
+      <c r="BH9" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="BC9" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="BD9" s="46" t="s">
+      <c r="BI9" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="BE9" s="46" t="s">
+      <c r="BJ9" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="BF9" s="46" t="s">
+      <c r="BK9" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="BG9" s="51" t="s">
+      <c r="BL9" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="BH9" s="46" t="s">
+      <c r="BM9" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="BI9" s="46" t="s">
+      <c r="BN9" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="BJ9" s="46" t="s">
+      <c r="BO9" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="BP9" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="BQ9" s="34"/>
+      <c r="BR9" s="34"/>
+      <c r="BS9" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT9" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU9" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="BV9" s="38"/>
+      <c r="BW9" s="38"/>
+      <c r="BX9" s="38"/>
+      <c r="BY9" s="38"/>
+      <c r="BZ9" s="38"/>
+      <c r="CA9" s="38"/>
+      <c r="CB9" s="38"/>
+      <c r="CC9" s="38"/>
+      <c r="CD9" s="38"/>
+      <c r="CE9" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="CF9" s="38"/>
+      <c r="CG9" s="38"/>
+      <c r="CH9" s="38"/>
+      <c r="CI9" s="38"/>
+    </row>
+    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="W10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="X10" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN10" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="AO10" s="39"/>
+      <c r="AP10" s="39"/>
+      <c r="AQ10" s="45"/>
+      <c r="AR10" s="45"/>
+      <c r="AS10" s="39"/>
+      <c r="AT10" s="39"/>
+      <c r="AU10" s="39"/>
+      <c r="AV10" s="59"/>
+      <c r="AW10" s="59"/>
+      <c r="AX10" s="59"/>
+      <c r="AY10" s="56"/>
+      <c r="AZ10" s="39"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="38"/>
+      <c r="BC10" s="38"/>
+      <c r="BD10" s="38"/>
+      <c r="BE10" s="38"/>
+      <c r="BF10" s="38"/>
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="38"/>
+      <c r="BI10" s="38"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="38"/>
+      <c r="BL10" s="38"/>
+      <c r="BM10" s="38"/>
+      <c r="BN10" s="38"/>
+      <c r="BO10" s="38"/>
+      <c r="BP10" s="38"/>
+      <c r="BQ10" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR10" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS10" s="49"/>
+      <c r="BT10" s="38"/>
+      <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="BK9" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="BL9" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="BM9" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="BN9" s="34"/>
-      <c r="BO9" s="34"/>
-      <c r="BP9" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="BQ9" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="BR9" s="46" t="s">
+      <c r="BV10" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="BW10" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BX10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="BY10" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="BZ10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="CA10" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="CB10" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="BS9" s="46"/>
-      <c r="BT9" s="46"/>
-      <c r="BU9" s="46"/>
-      <c r="BV9" s="46"/>
-      <c r="BW9" s="46"/>
-      <c r="BX9" s="46"/>
-      <c r="BY9" s="46"/>
-      <c r="BZ9" s="46"/>
-      <c r="CA9" s="46"/>
-      <c r="CB9" s="46" t="s">
+      <c r="CC10" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="CD10" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="CC9" s="46"/>
-      <c r="CD9" s="46"/>
-      <c r="CE9" s="46"/>
-      <c r="CF9" s="46"/>
+      <c r="CE10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="CF10" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="CG10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="CH10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="CI10" s="10" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="W10" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="X10" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="46"/>
-      <c r="AB10" s="46"/>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ10" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK10" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL10" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM10" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AN10" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="55"/>
-      <c r="AR10" s="55"/>
-      <c r="AS10" s="48"/>
-      <c r="AT10" s="48"/>
-      <c r="AU10" s="48"/>
-      <c r="AV10" s="45"/>
-      <c r="AW10" s="48"/>
-      <c r="AX10" s="46"/>
-      <c r="AY10" s="46"/>
-      <c r="AZ10" s="46"/>
-      <c r="BA10" s="46"/>
-      <c r="BB10" s="46"/>
-      <c r="BC10" s="46"/>
-      <c r="BD10" s="46"/>
-      <c r="BE10" s="46"/>
-      <c r="BF10" s="46"/>
-      <c r="BG10" s="57"/>
-      <c r="BH10" s="46"/>
-      <c r="BI10" s="46"/>
-      <c r="BJ10" s="46"/>
-      <c r="BK10" s="46"/>
-      <c r="BL10" s="46"/>
-      <c r="BM10" s="46"/>
-      <c r="BN10" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="BO10" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP10" s="52"/>
-      <c r="BQ10" s="46"/>
-      <c r="BR10" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="BS10" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="BT10" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="BU10" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="BV10" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="BW10" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="BX10" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="BY10" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="BZ10" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="CA10" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="CB10" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="CC10" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="CD10" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="CE10" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="CF10" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1793,7 +1836,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>5</v>
@@ -1839,13 +1882,13 @@
         <v>23</v>
       </c>
       <c r="V11" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W11" s="23" t="s">
         <v>24</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Y11" s="15" t="s">
         <v>25</v>
@@ -1888,13 +1931,13 @@
         <v>36</v>
       </c>
       <c r="AL11" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AM11" s="23" t="s">
         <v>37</v>
       </c>
       <c r="AN11" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AO11" s="15" t="s">
         <v>38</v>
@@ -1903,184 +1946,165 @@
         <v>39</v>
       </c>
       <c r="AQ11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AR11" s="24" t="s">
+      <c r="AS11" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="AS11" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="AT11" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AU11" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AW11" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX11" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AY11" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="AV11" s="15" t="s">
+      <c r="BA11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="BD11" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="BF11" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="AW11" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX11" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY11" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="AZ11" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="BA11" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB11" s="18" t="s">
+      <c r="BG11" s="29" t="e">
+        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="BC11" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="BD11" s="29" t="e">
-        <f>IF(BL11&lt;=EOMONTH(BA11,12),"X","")</f>
+      <c r="BI11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK11" s="29" t="e">
+        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE11" s="18" t="s">
+      <c r="BL11" s="29" t="e">
+        <f>IF(AND(BO11&gt;=EOMONTH(BD11,13),BO11&lt;=EOMONTH(BD11,48)),"X","")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BM11" s="29" t="e">
+        <f>IF(AND(BO11&gt;=EOMONTH(BD11,48),BO11&lt;=EOMONTH(BD11,72)),"X","")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BN11" s="29" t="e">
+        <f>IF(BO11&gt;=EOMONTH(BD11,73),"X","")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BO11" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="BF11" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="BG11" s="18" t="s">
+      <c r="BP11" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="BQ11" s="25" t="e">
+        <f>(EOMONTH(BO11,0))-(BO11-DAY(BO11)+1)+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BR11" s="25" t="e">
+        <f>BP11-BO11+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BS11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="BH11" s="29" t="e">
-        <f>IF(BL11&lt;=EOMONTH(BA11,12),"X","")</f>
+      <c r="BT11" s="31" t="e">
+        <f>BR11/BQ11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI11" s="29" t="e">
-        <f>IF(AND(BL11&gt;=EOMONTH(BA11,13),BL11&lt;=EOMONTH(BA11,48)),"X","")</f>
+      <c r="BU11" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV11" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW11" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="BX11" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="BY11" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="BZ11" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="CA11" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="CB11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="CC11" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="CD11" s="31" t="e">
+        <f>CA11*BT11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BJ11" s="29" t="e">
-        <f>IF(AND(BL11&gt;=EOMONTH(BA11,48),BL11&lt;=EOMONTH(BA11,72)),"X","")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BK11" s="29" t="e">
-        <f>IF(BL11&gt;=EOMONTH(BA11,73),"X","")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL11" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM11" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN11" s="25" t="e">
-        <f>(EOMONTH(BL11,0))-(BL11-DAY(BL11)+1)+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BO11" s="25" t="e">
-        <f>BM11-BL11+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BP11" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="BQ11" s="31" t="e">
-        <f>BO11/BN11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BR11" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="BS11" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="BT11" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="BU11" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="BV11" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="BW11" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="BX11" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="BY11" s="20" t="s">
+      <c r="CE11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BZ11" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="CA11" s="31" t="e">
-        <f>BX11*BQ11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="CB11" s="20" t="s">
+      <c r="CF11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="CC11" s="20" t="s">
+      <c r="CG11" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="CH11" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="CI11" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="CJ11" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="CD11" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="CE11" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="CF11" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="CG11" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="CH11" s="12"/>
+      <c r="CK11" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="AX8:AX10"/>
-    <mergeCell ref="BL8:CF8"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="CB9:CF9"/>
-    <mergeCell ref="AY8:BK8"/>
-    <mergeCell ref="BR9:CA9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="BQ9:BQ10"/>
-    <mergeCell ref="BP9:BP10"/>
+  <mergeCells count="64">
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="AO9:AO10"/>
     <mergeCell ref="AP9:AP10"/>
     <mergeCell ref="P9:P10"/>
@@ -2091,20 +2115,51 @@
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="Q9:U9"/>
     <mergeCell ref="G8:G10"/>
-    <mergeCell ref="AQ8:AV8"/>
-    <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:X8"/>
     <mergeCell ref="Y8:AN8"/>
     <mergeCell ref="AO8:AP8"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="BB8:BN8"/>
+    <mergeCell ref="BU9:CD9"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="AQ8:AY8"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="AZ8:AZ10"/>
+    <mergeCell ref="BA8:BA10"/>
+    <mergeCell ref="BO8:CI8"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1989 make column einkommensverschlechterung annuliert wider
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E944BB8-EC3D-4BD3-A719-7DC19D112C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586D0B25-817A-4E01-9618-F246C5DC1D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -751,6 +751,21 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -758,6 +773,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -766,55 +784,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1229,9 +1229,7 @@
   </sheetPr>
   <dimension ref="A1:CK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV18" sqref="AV18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1261,7 +1259,7 @@
     <col min="46" max="46" width="9.28515625"/>
     <col min="47" max="47" width="25.42578125"/>
     <col min="48" max="48" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="35.28515625" customWidth="1"/>
     <col min="52" max="52" width="27.42578125"/>
     <col min="53" max="53" width="10.42578125"/>
     <col min="54" max="56" width="12.7109375"/>
@@ -1356,328 +1354,328 @@
       <c r="C7"/>
     </row>
     <row r="8" spans="1:89" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="H8" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="57"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="57"/>
-      <c r="Y8" s="38" t="s">
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38"/>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="38"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="57"/>
-      <c r="AH8" s="57"/>
-      <c r="AI8" s="57"/>
-      <c r="AJ8" s="57"/>
-      <c r="AK8" s="57"/>
-      <c r="AL8" s="57"/>
-      <c r="AM8" s="57"/>
-      <c r="AN8" s="57"/>
-      <c r="AO8" s="39" t="s">
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="43"/>
+      <c r="AE8" s="43"/>
+      <c r="AF8" s="43"/>
+      <c r="AG8" s="54"/>
+      <c r="AH8" s="54"/>
+      <c r="AI8" s="54"/>
+      <c r="AJ8" s="54"/>
+      <c r="AK8" s="54"/>
+      <c r="AL8" s="54"/>
+      <c r="AM8" s="54"/>
+      <c r="AN8" s="54"/>
+      <c r="AO8" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="53" t="s">
+      <c r="AP8" s="44"/>
+      <c r="AQ8" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="54"/>
-      <c r="AS8" s="54"/>
-      <c r="AT8" s="54"/>
-      <c r="AU8" s="54"/>
-      <c r="AV8" s="54"/>
-      <c r="AW8" s="54"/>
-      <c r="AX8" s="54"/>
-      <c r="AY8" s="50"/>
-      <c r="AZ8" s="39" t="s">
+      <c r="AR8" s="39"/>
+      <c r="AS8" s="39"/>
+      <c r="AT8" s="39"/>
+      <c r="AU8" s="39"/>
+      <c r="AV8" s="39"/>
+      <c r="AW8" s="39"/>
+      <c r="AX8" s="39"/>
+      <c r="AY8" s="40"/>
+      <c r="AZ8" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="38" t="s">
+      <c r="BA8" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="46" t="s">
+      <c r="BB8" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="47"/>
-      <c r="BE8" s="47"/>
-      <c r="BF8" s="47"/>
-      <c r="BG8" s="47"/>
-      <c r="BH8" s="47"/>
-      <c r="BI8" s="47"/>
-      <c r="BJ8" s="47"/>
-      <c r="BK8" s="47"/>
-      <c r="BL8" s="47"/>
-      <c r="BM8" s="47"/>
-      <c r="BN8" s="48"/>
-      <c r="BO8" s="38" t="s">
+      <c r="BC8" s="50"/>
+      <c r="BD8" s="50"/>
+      <c r="BE8" s="50"/>
+      <c r="BF8" s="50"/>
+      <c r="BG8" s="50"/>
+      <c r="BH8" s="50"/>
+      <c r="BI8" s="50"/>
+      <c r="BJ8" s="50"/>
+      <c r="BK8" s="50"/>
+      <c r="BL8" s="50"/>
+      <c r="BM8" s="50"/>
+      <c r="BN8" s="51"/>
+      <c r="BO8" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="38"/>
-      <c r="BQ8" s="38"/>
-      <c r="BR8" s="38"/>
-      <c r="BS8" s="38"/>
-      <c r="BT8" s="38"/>
-      <c r="BU8" s="38"/>
-      <c r="BV8" s="38"/>
-      <c r="BW8" s="38"/>
-      <c r="BX8" s="38"/>
-      <c r="BY8" s="38"/>
-      <c r="BZ8" s="38"/>
-      <c r="CA8" s="38"/>
-      <c r="CB8" s="38"/>
-      <c r="CC8" s="38"/>
-      <c r="CD8" s="38"/>
-      <c r="CE8" s="38"/>
-      <c r="CF8" s="38"/>
-      <c r="CG8" s="38"/>
-      <c r="CH8" s="38"/>
-      <c r="CI8" s="38"/>
+      <c r="BP8" s="43"/>
+      <c r="BQ8" s="43"/>
+      <c r="BR8" s="43"/>
+      <c r="BS8" s="43"/>
+      <c r="BT8" s="43"/>
+      <c r="BU8" s="43"/>
+      <c r="BV8" s="43"/>
+      <c r="BW8" s="43"/>
+      <c r="BX8" s="43"/>
+      <c r="BY8" s="43"/>
+      <c r="BZ8" s="43"/>
+      <c r="CA8" s="43"/>
+      <c r="CB8" s="43"/>
+      <c r="CC8" s="43"/>
+      <c r="CD8" s="43"/>
+      <c r="CE8" s="43"/>
+      <c r="CF8" s="43"/>
+      <c r="CG8" s="43"/>
+      <c r="CH8" s="43"/>
+      <c r="CI8" s="43"/>
     </row>
     <row r="9" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="38" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N9" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="38" t="s">
+      <c r="O9" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="50"/>
       <c r="V9" s="33"/>
       <c r="W9" s="36"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="38" t="s">
+      <c r="Y9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="38" t="s">
+      <c r="Z9" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="38" t="s">
+      <c r="AA9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="38" t="s">
+      <c r="AB9" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="38" t="s">
+      <c r="AC9" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="38" t="s">
+      <c r="AD9" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="38" t="s">
+      <c r="AE9" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="46" t="s">
+      <c r="AF9" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="46" t="s">
+      <c r="AG9" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="47"/>
+      <c r="AH9" s="50"/>
+      <c r="AI9" s="50"/>
+      <c r="AJ9" s="50"/>
+      <c r="AK9" s="50"/>
       <c r="AL9" s="33"/>
       <c r="AM9" s="36"/>
       <c r="AN9" s="13"/>
-      <c r="AO9" s="50" t="s">
+      <c r="AO9" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="39" t="s">
+      <c r="AP9" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="44" t="s">
+      <c r="AQ9" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="44" t="s">
+      <c r="AR9" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="39" t="s">
+      <c r="AS9" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="43" t="s">
+      <c r="AT9" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="39" t="s">
+      <c r="AU9" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="AV9" s="58" t="s">
+      <c r="AV9" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="AW9" s="58" t="s">
+      <c r="AW9" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="AX9" s="58" t="s">
+      <c r="AX9" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="AY9" s="55" t="s">
+      <c r="AY9" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="AZ9" s="39"/>
-      <c r="BA9" s="38"/>
-      <c r="BB9" s="38" t="s">
+      <c r="AZ9" s="44"/>
+      <c r="BA9" s="43"/>
+      <c r="BB9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="38" t="s">
+      <c r="BC9" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="38" t="s">
+      <c r="BD9" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="40" t="s">
+      <c r="BE9" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="40" t="s">
+      <c r="BF9" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="BG9" s="38" t="s">
+      <c r="BG9" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="38" t="s">
+      <c r="BH9" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="38" t="s">
+      <c r="BI9" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="41" t="s">
+      <c r="BJ9" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="38" t="s">
+      <c r="BK9" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="38" t="s">
+      <c r="BL9" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="38" t="s">
+      <c r="BM9" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="38" t="s">
+      <c r="BN9" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="38" t="s">
+      <c r="BO9" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="38" t="s">
+      <c r="BP9" s="43" t="s">
         <v>115</v>
       </c>
       <c r="BQ9" s="34"/>
       <c r="BR9" s="34"/>
-      <c r="BS9" s="41" t="s">
+      <c r="BS9" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="38" t="s">
+      <c r="BT9" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="38" t="s">
+      <c r="BU9" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="38"/>
-      <c r="BW9" s="38"/>
-      <c r="BX9" s="38"/>
-      <c r="BY9" s="38"/>
-      <c r="BZ9" s="38"/>
-      <c r="CA9" s="38"/>
-      <c r="CB9" s="38"/>
-      <c r="CC9" s="38"/>
-      <c r="CD9" s="38"/>
-      <c r="CE9" s="38" t="s">
+      <c r="BV9" s="43"/>
+      <c r="BW9" s="43"/>
+      <c r="BX9" s="43"/>
+      <c r="BY9" s="43"/>
+      <c r="BZ9" s="43"/>
+      <c r="CA9" s="43"/>
+      <c r="CB9" s="43"/>
+      <c r="CC9" s="43"/>
+      <c r="CD9" s="43"/>
+      <c r="CE9" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="38"/>
-      <c r="CG9" s="38"/>
-      <c r="CH9" s="38"/>
-      <c r="CI9" s="38"/>
+      <c r="CF9" s="43"/>
+      <c r="CG9" s="43"/>
+      <c r="CH9" s="43"/>
+      <c r="CI9" s="43"/>
     </row>
     <row r="10" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
       <c r="Q10" s="16" t="s">
         <v>84</v>
       </c>
@@ -1702,14 +1700,14 @@
       <c r="X10" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
       <c r="AG10" s="16" t="s">
         <v>84</v>
       </c>
@@ -1734,42 +1732,42 @@
       <c r="AN10" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="AO10" s="39"/>
-      <c r="AP10" s="39"/>
-      <c r="AQ10" s="45"/>
-      <c r="AR10" s="45"/>
-      <c r="AS10" s="39"/>
-      <c r="AT10" s="39"/>
-      <c r="AU10" s="39"/>
-      <c r="AV10" s="59"/>
-      <c r="AW10" s="59"/>
-      <c r="AX10" s="59"/>
-      <c r="AY10" s="56"/>
-      <c r="AZ10" s="39"/>
-      <c r="BA10" s="38"/>
-      <c r="BB10" s="38"/>
-      <c r="BC10" s="38"/>
-      <c r="BD10" s="38"/>
-      <c r="BE10" s="38"/>
-      <c r="BF10" s="38"/>
-      <c r="BG10" s="38"/>
-      <c r="BH10" s="38"/>
-      <c r="BI10" s="38"/>
-      <c r="BJ10" s="42"/>
-      <c r="BK10" s="38"/>
-      <c r="BL10" s="38"/>
-      <c r="BM10" s="38"/>
-      <c r="BN10" s="38"/>
-      <c r="BO10" s="38"/>
-      <c r="BP10" s="38"/>
+      <c r="AO10" s="44"/>
+      <c r="AP10" s="44"/>
+      <c r="AQ10" s="59"/>
+      <c r="AR10" s="59"/>
+      <c r="AS10" s="44"/>
+      <c r="AT10" s="44"/>
+      <c r="AU10" s="44"/>
+      <c r="AV10" s="57"/>
+      <c r="AW10" s="57"/>
+      <c r="AX10" s="57"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="44"/>
+      <c r="BA10" s="43"/>
+      <c r="BB10" s="43"/>
+      <c r="BC10" s="43"/>
+      <c r="BD10" s="43"/>
+      <c r="BE10" s="43"/>
+      <c r="BF10" s="43"/>
+      <c r="BG10" s="43"/>
+      <c r="BH10" s="43"/>
+      <c r="BI10" s="43"/>
+      <c r="BJ10" s="48"/>
+      <c r="BK10" s="43"/>
+      <c r="BL10" s="43"/>
+      <c r="BM10" s="43"/>
+      <c r="BN10" s="43"/>
+      <c r="BO10" s="43"/>
+      <c r="BP10" s="43"/>
       <c r="BQ10" s="34" t="s">
         <v>0</v>
       </c>
       <c r="BR10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="49"/>
-      <c r="BT10" s="38"/>
+      <c r="BS10" s="52"/>
+      <c r="BT10" s="43"/>
       <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
@@ -2096,7 +2094,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="O9:O10"/>
     <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="AW9:AW10"/>
     <mergeCell ref="AX9:AX10"/>
@@ -2108,17 +2105,20 @@
     <mergeCell ref="AO9:AO10"/>
     <mergeCell ref="AP9:AP10"/>
     <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
-    <mergeCell ref="Q9:U9"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:X8"/>
     <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
     <mergeCell ref="AO8:AP8"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="Y9:Y10"/>
@@ -2130,13 +2130,18 @@
     <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="AD9:AD10"/>
     <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
     <mergeCell ref="CE9:CI9"/>
     <mergeCell ref="BB8:BN8"/>
     <mergeCell ref="BU9:CD9"/>
     <mergeCell ref="BT9:BT10"/>
     <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BO8:CI8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BH9:BH10"/>
     <mergeCell ref="AQ8:AY8"/>
     <mergeCell ref="AY9:AY10"/>
     <mergeCell ref="BI9:BI10"/>
@@ -2144,22 +2149,15 @@
     <mergeCell ref="AS9:AS10"/>
     <mergeCell ref="AT9:AT10"/>
     <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
     <mergeCell ref="AZ8:AZ10"/>
     <mergeCell ref="BA8:BA10"/>
-    <mergeCell ref="BO8:CI8"/>
     <mergeCell ref="BB9:BB10"/>
     <mergeCell ref="BC9:BC10"/>
     <mergeCell ref="BD9:BD10"/>
     <mergeCell ref="BE9:BE10"/>
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
     <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2760: Translator mit gewunsche Anpassungen im Report und einen kleinen Variable Name Korrigiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586D0B25-817A-4E01-9618-F246C5DC1D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B7B40-3159-46B9-83D4-292D8B46702E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="160">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -399,9 +399,6 @@
   </si>
   <si>
     <t>{bgMonatspensumTitle}</t>
-  </si>
-  <si>
-    <t>{vollkostenTitle}</t>
   </si>
   <si>
     <t>{elternbeitragTitle}</t>
@@ -682,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -697,19 +694,18 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -717,105 +713,72 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1227,9 +1190,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CK11"/>
+  <dimension ref="A1:CJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CF15" sqref="CF15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1289,7 +1254,7 @@
     <col min="88" max="1008" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:88" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1301,10 +1266,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1315,11 +1280,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BQ3" s="30"/>
-      <c r="BR3" s="30"/>
-      <c r="BS3" s="30"/>
+      <c r="BQ3" s="24"/>
+      <c r="BR3" s="24"/>
+      <c r="BS3" s="24"/>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1328,7 +1293,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1337,7 +1302,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1350,798 +1315,749 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:89" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+    <row r="8" spans="1:88" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" s="53" t="s">
+      <c r="G8" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="43" t="s">
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="43"/>
-      <c r="AC8" s="43"/>
-      <c r="AD8" s="43"/>
-      <c r="AE8" s="43"/>
-      <c r="AF8" s="43"/>
-      <c r="AG8" s="54"/>
-      <c r="AH8" s="54"/>
-      <c r="AI8" s="54"/>
-      <c r="AJ8" s="54"/>
-      <c r="AK8" s="54"/>
-      <c r="AL8" s="54"/>
-      <c r="AM8" s="54"/>
-      <c r="AN8" s="54"/>
-      <c r="AO8" s="44" t="s">
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="30"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="30"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="37"/>
+      <c r="AI8" s="37"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="37"/>
+      <c r="AN8" s="37"/>
+      <c r="AO8" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="38" t="s">
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39"/>
-      <c r="AT8" s="39"/>
-      <c r="AU8" s="39"/>
-      <c r="AV8" s="39"/>
-      <c r="AW8" s="39"/>
-      <c r="AX8" s="39"/>
-      <c r="AY8" s="40"/>
-      <c r="AZ8" s="44" t="s">
+      <c r="AR8" s="41"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="41"/>
+      <c r="AV8" s="41"/>
+      <c r="AW8" s="41"/>
+      <c r="AX8" s="41"/>
+      <c r="AY8" s="31"/>
+      <c r="AZ8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="43" t="s">
+      <c r="BA8" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="49" t="s">
+      <c r="BB8" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="50"/>
-      <c r="BD8" s="50"/>
-      <c r="BE8" s="50"/>
-      <c r="BF8" s="50"/>
-      <c r="BG8" s="50"/>
-      <c r="BH8" s="50"/>
-      <c r="BI8" s="50"/>
-      <c r="BJ8" s="50"/>
-      <c r="BK8" s="50"/>
-      <c r="BL8" s="50"/>
-      <c r="BM8" s="50"/>
-      <c r="BN8" s="51"/>
-      <c r="BO8" s="43" t="s">
+      <c r="BC8" s="34"/>
+      <c r="BD8" s="34"/>
+      <c r="BE8" s="34"/>
+      <c r="BF8" s="34"/>
+      <c r="BG8" s="34"/>
+      <c r="BH8" s="34"/>
+      <c r="BI8" s="34"/>
+      <c r="BJ8" s="34"/>
+      <c r="BK8" s="34"/>
+      <c r="BL8" s="34"/>
+      <c r="BM8" s="34"/>
+      <c r="BN8" s="38"/>
+      <c r="BO8" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="43"/>
-      <c r="BQ8" s="43"/>
-      <c r="BR8" s="43"/>
-      <c r="BS8" s="43"/>
-      <c r="BT8" s="43"/>
-      <c r="BU8" s="43"/>
-      <c r="BV8" s="43"/>
-      <c r="BW8" s="43"/>
-      <c r="BX8" s="43"/>
-      <c r="BY8" s="43"/>
-      <c r="BZ8" s="43"/>
-      <c r="CA8" s="43"/>
-      <c r="CB8" s="43"/>
-      <c r="CC8" s="43"/>
-      <c r="CD8" s="43"/>
-      <c r="CE8" s="43"/>
-      <c r="CF8" s="43"/>
-      <c r="CG8" s="43"/>
-      <c r="CH8" s="43"/>
-      <c r="CI8" s="43"/>
+      <c r="BP8" s="30"/>
+      <c r="BQ8" s="30"/>
+      <c r="BR8" s="30"/>
+      <c r="BS8" s="30"/>
+      <c r="BT8" s="30"/>
+      <c r="BU8" s="30"/>
+      <c r="BV8" s="30"/>
+      <c r="BW8" s="30"/>
+      <c r="BX8" s="30"/>
+      <c r="BY8" s="30"/>
+      <c r="BZ8" s="30"/>
+      <c r="CA8" s="30"/>
+      <c r="CB8" s="30"/>
+      <c r="CC8" s="30"/>
+      <c r="CD8" s="30"/>
+      <c r="CE8" s="30"/>
+      <c r="CF8" s="30"/>
+      <c r="CG8" s="30"/>
+      <c r="CH8" s="30"/>
+      <c r="CI8" s="30"/>
     </row>
-    <row r="9" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="43" t="s">
+    <row r="9" spans="1:88" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="49" t="s">
+      <c r="P9" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="49" t="s">
+      <c r="Q9" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50"/>
-      <c r="V9" s="33"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="43" t="s">
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="43" t="s">
+      <c r="Z9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="43" t="s">
+      <c r="AA9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="43" t="s">
+      <c r="AB9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="43" t="s">
+      <c r="AC9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="43" t="s">
+      <c r="AD9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="43" t="s">
+      <c r="AE9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="49" t="s">
+      <c r="AF9" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="49" t="s">
+      <c r="AG9" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="50"/>
-      <c r="AI9" s="50"/>
-      <c r="AJ9" s="50"/>
-      <c r="AK9" s="50"/>
-      <c r="AL9" s="33"/>
-      <c r="AM9" s="36"/>
-      <c r="AN9" s="13"/>
-      <c r="AO9" s="40" t="s">
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="34"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="12"/>
+      <c r="AO9" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="44" t="s">
+      <c r="AP9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="58" t="s">
+      <c r="AQ9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="58" t="s">
+      <c r="AR9" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="44" t="s">
+      <c r="AS9" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="45" t="s">
+      <c r="AT9" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="44" t="s">
+      <c r="AU9" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="AV9" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="AV9" s="56" t="s">
+      <c r="AW9" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="AW9" s="56" t="s">
+      <c r="AX9" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="AX9" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="AY9" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="AZ9" s="44"/>
-      <c r="BA9" s="43"/>
-      <c r="BB9" s="43" t="s">
+      <c r="AY9" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ9" s="32"/>
+      <c r="BA9" s="30"/>
+      <c r="BB9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="43" t="s">
+      <c r="BC9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="43" t="s">
+      <c r="BD9" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="46" t="s">
+      <c r="BE9" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="BG9" s="43" t="s">
+      <c r="BF9" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG9" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="43" t="s">
+      <c r="BH9" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="43" t="s">
+      <c r="BI9" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="47" t="s">
+      <c r="BJ9" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="43" t="s">
+      <c r="BK9" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="43" t="s">
+      <c r="BL9" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="43" t="s">
+      <c r="BM9" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="43" t="s">
+      <c r="BN9" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="43" t="s">
+      <c r="BO9" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="43" t="s">
+      <c r="BP9" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="BQ9" s="34"/>
-      <c r="BR9" s="34"/>
-      <c r="BS9" s="47" t="s">
+      <c r="BQ9" s="27"/>
+      <c r="BR9" s="27"/>
+      <c r="BS9" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="43" t="s">
+      <c r="BT9" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="43" t="s">
+      <c r="BU9" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="43"/>
-      <c r="BW9" s="43"/>
-      <c r="BX9" s="43"/>
-      <c r="BY9" s="43"/>
-      <c r="BZ9" s="43"/>
-      <c r="CA9" s="43"/>
-      <c r="CB9" s="43"/>
-      <c r="CC9" s="43"/>
-      <c r="CD9" s="43"/>
-      <c r="CE9" s="43" t="s">
+      <c r="BV9" s="30"/>
+      <c r="BW9" s="30"/>
+      <c r="BX9" s="30"/>
+      <c r="BY9" s="30"/>
+      <c r="BZ9" s="30"/>
+      <c r="CA9" s="30"/>
+      <c r="CB9" s="30"/>
+      <c r="CC9" s="30"/>
+      <c r="CD9" s="30"/>
+      <c r="CE9" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="43"/>
-      <c r="CG9" s="43"/>
-      <c r="CH9" s="43"/>
-      <c r="CI9" s="43"/>
+      <c r="CF9" s="30"/>
+      <c r="CG9" s="30"/>
+      <c r="CH9" s="30"/>
+      <c r="CI9" s="30"/>
     </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="16" t="s">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="16" t="s">
+      <c r="R10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="16" t="s">
+      <c r="S10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="T10" s="16" t="s">
+      <c r="T10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="V10" s="16" t="s">
+      <c r="V10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="W10" s="17" t="s">
+      <c r="W10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43"/>
-      <c r="AD10" s="43"/>
-      <c r="AE10" s="43"/>
-      <c r="AF10" s="43"/>
-      <c r="AG10" s="16" t="s">
+      <c r="X10" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AH10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AI10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AJ10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AK10" s="16" t="s">
+      <c r="AK10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AL10" s="16" t="s">
+      <c r="AL10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="AM10" s="17" t="s">
+      <c r="AM10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="AN10" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="AO10" s="44"/>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="59"/>
-      <c r="AR10" s="59"/>
-      <c r="AS10" s="44"/>
-      <c r="AT10" s="44"/>
-      <c r="AU10" s="44"/>
-      <c r="AV10" s="57"/>
-      <c r="AW10" s="57"/>
-      <c r="AX10" s="57"/>
-      <c r="AY10" s="42"/>
-      <c r="AZ10" s="44"/>
-      <c r="BA10" s="43"/>
-      <c r="BB10" s="43"/>
-      <c r="BC10" s="43"/>
-      <c r="BD10" s="43"/>
-      <c r="BE10" s="43"/>
-      <c r="BF10" s="43"/>
-      <c r="BG10" s="43"/>
-      <c r="BH10" s="43"/>
-      <c r="BI10" s="43"/>
-      <c r="BJ10" s="48"/>
-      <c r="BK10" s="43"/>
-      <c r="BL10" s="43"/>
-      <c r="BM10" s="43"/>
-      <c r="BN10" s="43"/>
-      <c r="BO10" s="43"/>
-      <c r="BP10" s="43"/>
-      <c r="BQ10" s="34" t="s">
+      <c r="AN10" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AO10" s="32"/>
+      <c r="AP10" s="32"/>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="32"/>
+      <c r="AT10" s="32"/>
+      <c r="AU10" s="32"/>
+      <c r="AV10" s="29"/>
+      <c r="AW10" s="29"/>
+      <c r="AX10" s="29"/>
+      <c r="AY10" s="43"/>
+      <c r="AZ10" s="32"/>
+      <c r="BA10" s="30"/>
+      <c r="BB10" s="30"/>
+      <c r="BC10" s="30"/>
+      <c r="BD10" s="30"/>
+      <c r="BE10" s="30"/>
+      <c r="BF10" s="30"/>
+      <c r="BG10" s="30"/>
+      <c r="BH10" s="30"/>
+      <c r="BI10" s="30"/>
+      <c r="BJ10" s="39"/>
+      <c r="BK10" s="30"/>
+      <c r="BL10" s="30"/>
+      <c r="BM10" s="30"/>
+      <c r="BN10" s="30"/>
+      <c r="BO10" s="30"/>
+      <c r="BP10" s="30"/>
+      <c r="BQ10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="BR10" s="35" t="s">
+      <c r="BR10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="52"/>
-      <c r="BT10" s="43"/>
+      <c r="BS10" s="39"/>
+      <c r="BT10" s="30"/>
       <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
       <c r="BV10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="BW10" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="BW10" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="BX10" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BY10" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BZ10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CA10" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="CB10" s="10" t="s">
         <v>120</v>
       </c>
       <c r="CC10" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="CD10" s="10" t="s">
         <v>121</v>
       </c>
       <c r="CE10" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="CF10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="CF10" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="CG10" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="CH10" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="CI10" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="27" t="e">
+      <c r="Q11" s="20" t="e">
         <f>R11+S11+T11+U11+V11+X11+W11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="R11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="23" t="s">
+      <c r="S11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="T11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="23" t="s">
+      <c r="U11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="V11" s="23" t="s">
+      <c r="V11" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="W11" s="23" t="s">
+      <c r="W11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="X11" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y11" s="15" t="s">
+      <c r="X11" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="15" t="s">
+      <c r="Z11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AA11" s="15" t="s">
+      <c r="AA11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AB11" s="15" t="s">
+      <c r="AB11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AC11" s="15" t="s">
+      <c r="AC11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AD11" s="15" t="s">
+      <c r="AD11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AE11" s="15" t="s">
+      <c r="AE11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AF11" s="15" t="s">
+      <c r="AF11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AG11" s="28" t="e">
+      <c r="AG11" s="20" t="e">
         <f>IF((AH11+AI11+AJ11+AK11+AL11+AN11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AN11+AM11,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="23" t="s">
+      <c r="AH11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AI11" s="23" t="s">
+      <c r="AI11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AJ11" s="23" t="s">
+      <c r="AJ11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AK11" s="23" t="s">
+      <c r="AK11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AL11" s="23" t="s">
+      <c r="AL11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AM11" s="23" t="s">
+      <c r="AM11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AN11" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="AO11" s="15" t="s">
+      <c r="AN11" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="AO11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AP11" s="15" t="s">
+      <c r="AP11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AQ11" s="24" t="s">
+      <c r="AQ11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AR11" s="24" t="s">
+      <c r="AR11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AS11" s="24" t="s">
+      <c r="AS11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AT11" s="15" t="s">
+      <c r="AT11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AU11" s="15" t="s">
+      <c r="AU11" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV11" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AV11" s="15" t="s">
+      <c r="AW11" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="AW11" s="15" t="s">
+      <c r="AX11" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="AX11" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AY11" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="AZ11" s="15" t="s">
+      <c r="AY11" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="BA11" s="15" t="s">
+      <c r="BA11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="BB11" s="18" t="s">
+      <c r="BB11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BC11" s="18" t="s">
+      <c r="BC11" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BD11" s="19" t="s">
+      <c r="BD11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="BE11" s="18" t="s">
+      <c r="BE11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BF11" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="BG11" s="29" t="e">
+      <c r="BF11" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="BG11" s="16" t="e">
         <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="18" t="s">
+      <c r="BH11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BI11" s="18" t="s">
+      <c r="BI11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="BJ11" s="18" t="s">
+      <c r="BJ11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="BK11" s="29" t="e">
+      <c r="BK11" s="16" t="e">
         <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BL11" s="29" t="e">
+      <c r="BL11" s="16" t="e">
         <f>IF(AND(BO11&gt;=EOMONTH(BD11,13),BO11&lt;=EOMONTH(BD11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BM11" s="29" t="e">
+      <c r="BM11" s="16" t="e">
         <f>IF(AND(BO11&gt;=EOMONTH(BD11,48),BO11&lt;=EOMONTH(BD11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="29" t="e">
+      <c r="BN11" s="16" t="e">
         <f>IF(BO11&gt;=EOMONTH(BD11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="19" t="s">
+      <c r="BO11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="BP11" s="19" t="s">
+      <c r="BP11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="BQ11" s="25" t="e">
+      <c r="BQ11" s="22" t="e">
         <f>(EOMONTH(BO11,0))-(BO11-DAY(BO11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BR11" s="25" t="e">
+      <c r="BR11" s="22" t="e">
         <f>BP11-BO11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BS11" s="25" t="s">
+      <c r="BS11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="BT11" s="31" t="e">
+      <c r="BT11" s="23" t="e">
         <f>BR11/BQ11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BU11" s="26" t="s">
+      <c r="BU11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="BV11" s="26" t="s">
+      <c r="BV11" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BW11" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="BW11" s="26" t="s">
+      <c r="BX11" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="BX11" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY11" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="BZ11" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="CA11" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="CB11" s="20" t="s">
+      <c r="BY11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="BZ11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="CA11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="CB11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="CC11" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="CD11" s="31" t="e">
+      <c r="CC11" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="CD11" s="23" t="e">
         <f>CA11*BT11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="CE11" s="20" t="s">
+      <c r="CE11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CF11" s="20" t="s">
+      <c r="CF11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CG11" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="CH11" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="CI11" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="CJ11" s="32" t="s">
+      <c r="CG11" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="CH11" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="CI11" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="CJ11" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="CK11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="BB8:BN8"/>
-    <mergeCell ref="BU9:CD9"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BO8:CI8"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BH9:BH10"/>
     <mergeCell ref="AQ8:AY8"/>
     <mergeCell ref="AY9:AY10"/>
     <mergeCell ref="BI9:BI10"/>
@@ -2158,6 +2074,54 @@
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BJ9:BJ10"/>
     <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="BB8:BN8"/>
+    <mergeCell ref="BU9:CD9"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BO8:CI8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2795 keinPlatzImSchulhort in Statistik zeigen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B7B40-3159-46B9-83D4-292D8B46702E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74B131-4375-497C-AE34-DB5DD672E828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>{einkommensverschlechterungBasisJahr2AnnuliertTitle}</t>
+  </si>
+  <si>
+    <t>{keinPlatzImSchulhortTitle}</t>
+  </si>
+  <si>
+    <t>{keinPlatzImSchulhort}</t>
   </si>
 </sst>
 </file>
@@ -732,53 +738,53 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1190,71 +1196,69 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CJ11"/>
+  <dimension ref="A1:CK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CF15" sqref="CF15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.7109375"/>
-    <col min="17" max="18" width="10.7109375"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="41.42578125" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" customWidth="1"/>
-    <col min="24" max="24" width="24.140625"/>
-    <col min="25" max="32" width="8.7109375"/>
-    <col min="33" max="34" width="10.7109375"/>
-    <col min="35" max="35" width="24.5703125" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375"/>
-    <col min="37" max="37" width="14.42578125" customWidth="1"/>
-    <col min="38" max="38" width="41.42578125" customWidth="1"/>
-    <col min="39" max="39" width="27.140625" customWidth="1"/>
-    <col min="40" max="40" width="24.140625"/>
-    <col min="41" max="41" width="9.140625" customWidth="1"/>
-    <col min="42" max="42" width="6.42578125"/>
-    <col min="43" max="43" width="18.140625"/>
-    <col min="45" max="45" width="23.28515625"/>
-    <col min="46" max="46" width="9.28515625"/>
-    <col min="47" max="47" width="25.42578125"/>
-    <col min="48" max="48" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="35.28515625" customWidth="1"/>
-    <col min="52" max="52" width="27.42578125"/>
-    <col min="53" max="53" width="10.42578125"/>
-    <col min="54" max="56" width="12.7109375"/>
-    <col min="57" max="57" width="16.7109375"/>
-    <col min="58" max="58" width="20.5703125" customWidth="1"/>
-    <col min="59" max="59" width="12.7109375"/>
-    <col min="60" max="60" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="8.6640625"/>
+    <col min="17" max="18" width="10.6640625"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625"/>
+    <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="22" max="22" width="41.44140625" customWidth="1"/>
+    <col min="23" max="23" width="26.88671875" customWidth="1"/>
+    <col min="24" max="24" width="24.109375"/>
+    <col min="25" max="32" width="8.6640625"/>
+    <col min="33" max="34" width="10.6640625"/>
+    <col min="35" max="35" width="24.5546875" customWidth="1"/>
+    <col min="36" max="36" width="10.6640625"/>
+    <col min="37" max="37" width="14.44140625" customWidth="1"/>
+    <col min="38" max="38" width="41.44140625" customWidth="1"/>
+    <col min="39" max="39" width="27.109375" customWidth="1"/>
+    <col min="40" max="40" width="24.109375"/>
+    <col min="41" max="41" width="9.109375" customWidth="1"/>
+    <col min="42" max="42" width="6.44140625"/>
+    <col min="43" max="43" width="18.109375"/>
+    <col min="45" max="45" width="23.33203125"/>
+    <col min="46" max="46" width="9.33203125"/>
+    <col min="47" max="47" width="25.44140625"/>
+    <col min="48" max="48" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="35.33203125" customWidth="1"/>
+    <col min="52" max="52" width="27.44140625"/>
+    <col min="53" max="53" width="10.44140625"/>
+    <col min="54" max="56" width="12.6640625"/>
+    <col min="57" max="57" width="16.6640625"/>
+    <col min="58" max="58" width="20.5546875" customWidth="1"/>
+    <col min="59" max="59" width="12.6640625"/>
+    <col min="60" max="60" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="22"/>
-    <col min="62" max="62" width="18.140625" customWidth="1"/>
+    <col min="62" max="62" width="18.109375" customWidth="1"/>
     <col min="63" max="66" width="22"/>
-    <col min="67" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="16" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="16" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375"/>
-    <col min="73" max="74" width="13.28515625" customWidth="1"/>
-    <col min="75" max="75" width="13.7109375" customWidth="1"/>
-    <col min="76" max="76" width="16.85546875"/>
-    <col min="77" max="78" width="12.28515625" customWidth="1"/>
-    <col min="79" max="79" width="12.7109375"/>
-    <col min="80" max="80" width="19.42578125"/>
-    <col min="82" max="82" width="16.85546875"/>
-    <col min="83" max="84" width="12.7109375"/>
-    <col min="85" max="85" width="13.5703125" customWidth="1"/>
-    <col min="86" max="86" width="12.7109375" customWidth="1"/>
-    <col min="87" max="87" width="12.7109375"/>
-    <col min="88" max="1008" width="10.42578125"/>
+    <col min="68" max="69" width="12.6640625"/>
+    <col min="70" max="70" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="16" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="16" customWidth="1"/>
+    <col min="73" max="73" width="12.6640625"/>
+    <col min="74" max="75" width="13.33203125" customWidth="1"/>
+    <col min="76" max="76" width="13.6640625" customWidth="1"/>
+    <col min="77" max="77" width="16.88671875"/>
+    <col min="78" max="79" width="12.33203125" customWidth="1"/>
+    <col min="80" max="80" width="12.6640625"/>
+    <col min="81" max="81" width="19.44140625"/>
+    <col min="83" max="83" width="16.88671875"/>
+    <col min="84" max="85" width="12.6640625"/>
+    <col min="86" max="86" width="13.5546875" customWidth="1"/>
+    <col min="87" max="87" width="12.6640625" customWidth="1"/>
+    <col min="88" max="88" width="12.6640625"/>
+    <col min="89" max="1009" width="10.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:89" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1266,10 +1270,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1280,11 +1284,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BQ3" s="24"/>
       <c r="BR3" s="24"/>
       <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1293,7 +1297,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1302,7 +1306,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1315,332 +1319,336 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:88" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:89" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="30" t="s">
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="37"/>
-      <c r="AI8" s="37"/>
-      <c r="AJ8" s="37"/>
-      <c r="AK8" s="37"/>
-      <c r="AL8" s="37"/>
-      <c r="AM8" s="37"/>
-      <c r="AN8" s="37"/>
-      <c r="AO8" s="32" t="s">
+      <c r="Z8" s="33"/>
+      <c r="AA8" s="33"/>
+      <c r="AB8" s="33"/>
+      <c r="AC8" s="33"/>
+      <c r="AD8" s="33"/>
+      <c r="AE8" s="33"/>
+      <c r="AF8" s="33"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="35"/>
+      <c r="AI8" s="35"/>
+      <c r="AJ8" s="35"/>
+      <c r="AK8" s="35"/>
+      <c r="AL8" s="35"/>
+      <c r="AM8" s="35"/>
+      <c r="AN8" s="35"/>
+      <c r="AO8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="32"/>
-      <c r="AQ8" s="40" t="s">
+      <c r="AP8" s="34"/>
+      <c r="AQ8" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="41"/>
-      <c r="AS8" s="41"/>
-      <c r="AT8" s="41"/>
-      <c r="AU8" s="41"/>
-      <c r="AV8" s="41"/>
-      <c r="AW8" s="41"/>
-      <c r="AX8" s="41"/>
-      <c r="AY8" s="31"/>
-      <c r="AZ8" s="32" t="s">
+      <c r="AR8" s="29"/>
+      <c r="AS8" s="29"/>
+      <c r="AT8" s="29"/>
+      <c r="AU8" s="29"/>
+      <c r="AV8" s="29"/>
+      <c r="AW8" s="29"/>
+      <c r="AX8" s="29"/>
+      <c r="AY8" s="30"/>
+      <c r="AZ8" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="30" t="s">
+      <c r="BA8" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="33" t="s">
+      <c r="BB8" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="34"/>
-      <c r="BD8" s="34"/>
-      <c r="BE8" s="34"/>
-      <c r="BF8" s="34"/>
-      <c r="BG8" s="34"/>
-      <c r="BH8" s="34"/>
-      <c r="BI8" s="34"/>
-      <c r="BJ8" s="34"/>
-      <c r="BK8" s="34"/>
-      <c r="BL8" s="34"/>
-      <c r="BM8" s="34"/>
+      <c r="BC8" s="38"/>
+      <c r="BD8" s="38"/>
+      <c r="BE8" s="38"/>
+      <c r="BF8" s="38"/>
+      <c r="BG8" s="38"/>
+      <c r="BH8" s="38"/>
+      <c r="BI8" s="38"/>
+      <c r="BJ8" s="38"/>
+      <c r="BK8" s="38"/>
+      <c r="BL8" s="38"/>
+      <c r="BM8" s="38"/>
       <c r="BN8" s="38"/>
-      <c r="BO8" s="30" t="s">
+      <c r="BO8" s="43"/>
+      <c r="BP8" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="30"/>
-      <c r="BQ8" s="30"/>
-      <c r="BR8" s="30"/>
-      <c r="BS8" s="30"/>
-      <c r="BT8" s="30"/>
-      <c r="BU8" s="30"/>
-      <c r="BV8" s="30"/>
-      <c r="BW8" s="30"/>
-      <c r="BX8" s="30"/>
-      <c r="BY8" s="30"/>
-      <c r="BZ8" s="30"/>
-      <c r="CA8" s="30"/>
-      <c r="CB8" s="30"/>
-      <c r="CC8" s="30"/>
-      <c r="CD8" s="30"/>
-      <c r="CE8" s="30"/>
-      <c r="CF8" s="30"/>
-      <c r="CG8" s="30"/>
-      <c r="CH8" s="30"/>
-      <c r="CI8" s="30"/>
+      <c r="BQ8" s="33"/>
+      <c r="BR8" s="33"/>
+      <c r="BS8" s="33"/>
+      <c r="BT8" s="33"/>
+      <c r="BU8" s="33"/>
+      <c r="BV8" s="33"/>
+      <c r="BW8" s="33"/>
+      <c r="BX8" s="33"/>
+      <c r="BY8" s="33"/>
+      <c r="BZ8" s="33"/>
+      <c r="CA8" s="33"/>
+      <c r="CB8" s="33"/>
+      <c r="CC8" s="33"/>
+      <c r="CD8" s="33"/>
+      <c r="CE8" s="33"/>
+      <c r="CF8" s="33"/>
+      <c r="CG8" s="33"/>
+      <c r="CH8" s="33"/>
+      <c r="CI8" s="33"/>
+      <c r="CJ8" s="33"/>
     </row>
-    <row r="9" spans="1:88" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="30" t="s">
+    <row r="9" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="12"/>
-      <c r="Y9" s="30" t="s">
+      <c r="Y9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="30" t="s">
+      <c r="Z9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="30" t="s">
+      <c r="AA9" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="30" t="s">
+      <c r="AB9" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="30" t="s">
+      <c r="AC9" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="30" t="s">
+      <c r="AD9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="30" t="s">
+      <c r="AE9" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="33" t="s">
+      <c r="AF9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="33" t="s">
+      <c r="AG9" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="34"/>
-      <c r="AI9" s="34"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="34"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
+      <c r="AJ9" s="38"/>
+      <c r="AK9" s="38"/>
       <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
       <c r="AN9" s="12"/>
-      <c r="AO9" s="31" t="s">
+      <c r="AO9" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="32" t="s">
+      <c r="AP9" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="28" t="s">
+      <c r="AQ9" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="28" t="s">
+      <c r="AR9" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="32" t="s">
+      <c r="AS9" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="32" t="s">
+      <c r="AT9" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="32" t="s">
+      <c r="AU9" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="28" t="s">
+      <c r="AV9" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="28" t="s">
+      <c r="AW9" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="28" t="s">
+      <c r="AX9" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="42" t="s">
+      <c r="AY9" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="32"/>
-      <c r="BA9" s="30"/>
-      <c r="BB9" s="30" t="s">
+      <c r="AZ9" s="34"/>
+      <c r="BA9" s="33"/>
+      <c r="BB9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="30" t="s">
+      <c r="BC9" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="30" t="s">
+      <c r="BD9" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="30" t="s">
+      <c r="BE9" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="30" t="s">
+      <c r="BF9" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="30" t="s">
+      <c r="BG9" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="30" t="s">
+      <c r="BH9" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="30" t="s">
+      <c r="BI9" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="37" t="s">
+      <c r="BJ9" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="30" t="s">
+      <c r="BK9" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="30" t="s">
+      <c r="BL9" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="30" t="s">
+      <c r="BM9" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="30" t="s">
+      <c r="BN9" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="30" t="s">
+      <c r="BO9" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="BP9" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="30" t="s">
+      <c r="BQ9" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BQ9" s="27"/>
       <c r="BR9" s="27"/>
-      <c r="BS9" s="37" t="s">
+      <c r="BS9" s="27"/>
+      <c r="BT9" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="30" t="s">
+      <c r="BU9" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="30" t="s">
+      <c r="BV9" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="30"/>
-      <c r="BW9" s="30"/>
-      <c r="BX9" s="30"/>
-      <c r="BY9" s="30"/>
-      <c r="BZ9" s="30"/>
-      <c r="CA9" s="30"/>
-      <c r="CB9" s="30"/>
-      <c r="CC9" s="30"/>
-      <c r="CD9" s="30"/>
-      <c r="CE9" s="30" t="s">
+      <c r="BW9" s="33"/>
+      <c r="BX9" s="33"/>
+      <c r="BY9" s="33"/>
+      <c r="BZ9" s="33"/>
+      <c r="CA9" s="33"/>
+      <c r="CB9" s="33"/>
+      <c r="CC9" s="33"/>
+      <c r="CD9" s="33"/>
+      <c r="CE9" s="33"/>
+      <c r="CF9" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="30"/>
-      <c r="CG9" s="30"/>
-      <c r="CH9" s="30"/>
-      <c r="CI9" s="30"/>
+      <c r="CG9" s="33"/>
+      <c r="CH9" s="33"/>
+      <c r="CI9" s="33"/>
+      <c r="CJ9" s="33"/>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
+    <row r="10" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
       <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1665,14 +1673,14 @@
       <c r="X10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
       <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1697,89 +1705,90 @@
       <c r="AN10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="32"/>
-      <c r="AP10" s="32"/>
-      <c r="AQ10" s="29"/>
-      <c r="AR10" s="29"/>
-      <c r="AS10" s="32"/>
-      <c r="AT10" s="32"/>
-      <c r="AU10" s="32"/>
-      <c r="AV10" s="29"/>
-      <c r="AW10" s="29"/>
-      <c r="AX10" s="29"/>
-      <c r="AY10" s="43"/>
-      <c r="AZ10" s="32"/>
-      <c r="BA10" s="30"/>
-      <c r="BB10" s="30"/>
-      <c r="BC10" s="30"/>
-      <c r="BD10" s="30"/>
-      <c r="BE10" s="30"/>
-      <c r="BF10" s="30"/>
-      <c r="BG10" s="30"/>
-      <c r="BH10" s="30"/>
-      <c r="BI10" s="30"/>
-      <c r="BJ10" s="39"/>
-      <c r="BK10" s="30"/>
-      <c r="BL10" s="30"/>
-      <c r="BM10" s="30"/>
-      <c r="BN10" s="30"/>
-      <c r="BO10" s="30"/>
-      <c r="BP10" s="30"/>
-      <c r="BQ10" s="27" t="s">
+      <c r="AO10" s="34"/>
+      <c r="AP10" s="34"/>
+      <c r="AQ10" s="42"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="34"/>
+      <c r="AT10" s="34"/>
+      <c r="AU10" s="34"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="42"/>
+      <c r="AX10" s="42"/>
+      <c r="AY10" s="32"/>
+      <c r="AZ10" s="34"/>
+      <c r="BA10" s="33"/>
+      <c r="BB10" s="33"/>
+      <c r="BC10" s="33"/>
+      <c r="BD10" s="33"/>
+      <c r="BE10" s="33"/>
+      <c r="BF10" s="33"/>
+      <c r="BG10" s="33"/>
+      <c r="BH10" s="33"/>
+      <c r="BI10" s="33"/>
+      <c r="BJ10" s="36"/>
+      <c r="BK10" s="33"/>
+      <c r="BL10" s="33"/>
+      <c r="BM10" s="33"/>
+      <c r="BN10" s="33"/>
+      <c r="BO10" s="36"/>
+      <c r="BP10" s="33"/>
+      <c r="BQ10" s="33"/>
+      <c r="BR10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="BR10" s="27" t="s">
+      <c r="BS10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="39"/>
-      <c r="BT10" s="30"/>
-      <c r="BU10" s="10" t="s">
+      <c r="BT10" s="36"/>
+      <c r="BU10" s="33"/>
+      <c r="BV10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="BV10" s="10" t="s">
+      <c r="BW10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="CB10" s="10" t="s">
+      <c r="CC10" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="CC10" s="10" t="s">
+      <c r="CD10" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="CD10" s="10" t="s">
+      <c r="CE10" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="CE10" s="10" t="s">
+      <c r="CF10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="CF10" s="10" t="s">
+      <c r="CG10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="CG10" s="10" t="s">
+      <c r="CH10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="CH10" s="10" t="s">
+      <c r="CI10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="CI10" s="10" t="s">
+      <c r="CJ10" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
@@ -1957,7 +1966,7 @@
         <v>151</v>
       </c>
       <c r="BG11" s="16" t="e">
-        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
+        <f>IF(BP11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BH11" s="16" t="s">
@@ -1970,94 +1979,146 @@
         <v>58</v>
       </c>
       <c r="BK11" s="16" t="e">
-        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
+        <f>IF(BP11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="16" t="e">
-        <f>IF(AND(BO11&gt;=EOMONTH(BD11,13),BO11&lt;=EOMONTH(BD11,48)),"X","")</f>
+        <f>IF(AND(BP11&gt;=EOMONTH(BD11,13),BP11&lt;=EOMONTH(BD11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BM11" s="16" t="e">
-        <f>IF(AND(BO11&gt;=EOMONTH(BD11,48),BO11&lt;=EOMONTH(BD11,72)),"X","")</f>
+        <f>IF(AND(BP11&gt;=EOMONTH(BD11,48),BP11&lt;=EOMONTH(BD11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BN11" s="16" t="e">
-        <f>IF(BO11&gt;=EOMONTH(BD11,73),"X","")</f>
+        <f>IF(BP11&gt;=EOMONTH(BD11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="17" t="s">
+      <c r="BO11" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="BP11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="BP11" s="17" t="s">
+      <c r="BQ11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="BQ11" s="22" t="e">
-        <f>(EOMONTH(BO11,0))-(BO11-DAY(BO11)+1)+1</f>
+      <c r="BR11" s="22" t="e">
+        <f>(EOMONTH(BP11,0))-(BP11-DAY(BP11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BR11" s="22" t="e">
-        <f>BP11-BO11+1</f>
+      <c r="BS11" s="22" t="e">
+        <f>BQ11-BP11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BS11" s="22" t="s">
+      <c r="BT11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="BT11" s="23" t="e">
-        <f>BR11/BQ11</f>
+      <c r="BU11" s="23" t="e">
+        <f>BS11/BR11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BU11" s="23" t="s">
+      <c r="BV11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="BV11" s="23" t="s">
+      <c r="BW11" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="BW11" s="23" t="s">
+      <c r="BX11" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="BX11" s="23" t="s">
+      <c r="BY11" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="BY11" s="23" t="s">
+      <c r="BZ11" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="BZ11" s="23" t="s">
+      <c r="CA11" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="CA11" s="23" t="s">
+      <c r="CB11" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="CB11" s="18" t="s">
+      <c r="CC11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="CC11" s="16" t="s">
+      <c r="CD11" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="CD11" s="23" t="e">
-        <f>CA11*BT11</f>
+      <c r="CE11" s="23" t="e">
+        <f>CB11*BU11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="CE11" s="18" t="s">
+      <c r="CF11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CF11" s="18" t="s">
+      <c r="CG11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CG11" s="18" t="s">
+      <c r="CH11" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="CH11" s="18" t="s">
+      <c r="CI11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="CI11" s="18" t="s">
+      <c r="CJ11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="CJ11" s="25" t="s">
+      <c r="CK11" s="25" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="65">
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="BP8:CJ8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BQ9:BQ10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="CF9:CJ9"/>
+    <mergeCell ref="BV9:CE9"/>
+    <mergeCell ref="BU9:BU10"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BB8:BO8"/>
     <mergeCell ref="AQ8:AY8"/>
     <mergeCell ref="AY9:AY10"/>
     <mergeCell ref="BI9:BI10"/>
@@ -2074,54 +2135,6 @@
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BJ9:BJ10"/>
     <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="BB8:BN8"/>
-    <mergeCell ref="BU9:CD9"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BO8:CI8"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2795 einen Kategorie "zusätzliche Felder Gemeinden"
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74B131-4375-497C-AE34-DB5DD672E828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD55F5D-9378-4D45-B67C-2CAE87671815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="165">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -519,6 +519,15 @@
   </si>
   <si>
     <t>{keinPlatzImSchulhort}</t>
+  </si>
+  <si>
+    <t>{zusatzFelderGemeinden}</t>
+  </si>
+  <si>
+    <t>{ausserordentlicherAnspruchTitle}</t>
+  </si>
+  <si>
+    <t>{ausserordentlicherAnspruch}</t>
   </si>
 </sst>
 </file>
@@ -685,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -738,53 +747,68 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1196,7 +1220,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CK11"/>
+  <dimension ref="A1:CL11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1239,26 +1263,28 @@
     <col min="61" max="61" width="22"/>
     <col min="62" max="62" width="18.109375" customWidth="1"/>
     <col min="63" max="66" width="22"/>
-    <col min="68" max="69" width="12.6640625"/>
-    <col min="70" max="70" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="16" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="16" customWidth="1"/>
-    <col min="73" max="73" width="12.6640625"/>
-    <col min="74" max="75" width="13.33203125" customWidth="1"/>
-    <col min="76" max="76" width="13.6640625" customWidth="1"/>
-    <col min="77" max="77" width="16.88671875"/>
-    <col min="78" max="79" width="12.33203125" customWidth="1"/>
-    <col min="80" max="80" width="12.6640625"/>
-    <col min="81" max="81" width="19.44140625"/>
-    <col min="83" max="83" width="16.88671875"/>
-    <col min="84" max="85" width="12.6640625"/>
-    <col min="86" max="86" width="13.5546875" customWidth="1"/>
-    <col min="87" max="87" width="12.6640625" customWidth="1"/>
-    <col min="88" max="88" width="12.6640625"/>
-    <col min="89" max="1009" width="10.44140625"/>
+    <col min="67" max="68" width="12.6640625"/>
+    <col min="69" max="69" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="16" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="16" customWidth="1"/>
+    <col min="72" max="72" width="12.6640625"/>
+    <col min="73" max="74" width="13.33203125" customWidth="1"/>
+    <col min="75" max="75" width="13.6640625" customWidth="1"/>
+    <col min="76" max="76" width="16.88671875"/>
+    <col min="77" max="78" width="12.33203125" customWidth="1"/>
+    <col min="79" max="79" width="12.6640625"/>
+    <col min="80" max="80" width="19.44140625"/>
+    <col min="82" max="82" width="16.88671875"/>
+    <col min="83" max="84" width="12.6640625"/>
+    <col min="85" max="85" width="13.5546875" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" customWidth="1"/>
+    <col min="87" max="87" width="12.6640625"/>
+    <col min="88" max="88" width="9.109375" style="44"/>
+    <col min="89" max="89" width="9.109375" style="9"/>
+    <col min="90" max="1010" width="10.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:90" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1270,10 +1296,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1284,11 +1310,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
+      <c r="BQ3" s="24"/>
       <c r="BR3" s="24"/>
       <c r="BS3" s="24"/>
-      <c r="BT3" s="24"/>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1297,7 +1323,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1306,7 +1332,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1319,336 +1345,342 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:89" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="33" t="s">
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="33"/>
-      <c r="AA8" s="33"/>
-      <c r="AB8" s="33"/>
-      <c r="AC8" s="33"/>
-      <c r="AD8" s="33"/>
-      <c r="AE8" s="33"/>
-      <c r="AF8" s="33"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="35"/>
-      <c r="AJ8" s="35"/>
-      <c r="AK8" s="35"/>
-      <c r="AL8" s="35"/>
-      <c r="AM8" s="35"/>
-      <c r="AN8" s="35"/>
-      <c r="AO8" s="34" t="s">
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="30"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="30"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="37"/>
+      <c r="AI8" s="37"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="37"/>
+      <c r="AN8" s="37"/>
+      <c r="AO8" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="34"/>
-      <c r="AQ8" s="28" t="s">
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="29"/>
-      <c r="AS8" s="29"/>
-      <c r="AT8" s="29"/>
-      <c r="AU8" s="29"/>
-      <c r="AV8" s="29"/>
-      <c r="AW8" s="29"/>
-      <c r="AX8" s="29"/>
-      <c r="AY8" s="30"/>
-      <c r="AZ8" s="34" t="s">
+      <c r="AR8" s="41"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="41"/>
+      <c r="AV8" s="41"/>
+      <c r="AW8" s="41"/>
+      <c r="AX8" s="41"/>
+      <c r="AY8" s="31"/>
+      <c r="AZ8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="33" t="s">
+      <c r="BA8" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="37" t="s">
+      <c r="BB8" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="38"/>
-      <c r="BD8" s="38"/>
-      <c r="BE8" s="38"/>
-      <c r="BF8" s="38"/>
-      <c r="BG8" s="38"/>
-      <c r="BH8" s="38"/>
-      <c r="BI8" s="38"/>
-      <c r="BJ8" s="38"/>
-      <c r="BK8" s="38"/>
-      <c r="BL8" s="38"/>
-      <c r="BM8" s="38"/>
-      <c r="BN8" s="38"/>
-      <c r="BO8" s="43"/>
-      <c r="BP8" s="33" t="s">
+      <c r="BC8" s="34"/>
+      <c r="BD8" s="34"/>
+      <c r="BE8" s="34"/>
+      <c r="BF8" s="34"/>
+      <c r="BG8" s="34"/>
+      <c r="BH8" s="34"/>
+      <c r="BI8" s="34"/>
+      <c r="BJ8" s="34"/>
+      <c r="BK8" s="34"/>
+      <c r="BL8" s="34"/>
+      <c r="BM8" s="34"/>
+      <c r="BN8" s="34"/>
+      <c r="BO8" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="BQ8" s="33"/>
-      <c r="BR8" s="33"/>
-      <c r="BS8" s="33"/>
-      <c r="BT8" s="33"/>
-      <c r="BU8" s="33"/>
-      <c r="BV8" s="33"/>
-      <c r="BW8" s="33"/>
-      <c r="BX8" s="33"/>
-      <c r="BY8" s="33"/>
-      <c r="BZ8" s="33"/>
-      <c r="CA8" s="33"/>
-      <c r="CB8" s="33"/>
-      <c r="CC8" s="33"/>
-      <c r="CD8" s="33"/>
-      <c r="CE8" s="33"/>
-      <c r="CF8" s="33"/>
-      <c r="CG8" s="33"/>
-      <c r="CH8" s="33"/>
-      <c r="CI8" s="33"/>
-      <c r="CJ8" s="33"/>
+      <c r="BP8" s="30"/>
+      <c r="BQ8" s="30"/>
+      <c r="BR8" s="30"/>
+      <c r="BS8" s="30"/>
+      <c r="BT8" s="30"/>
+      <c r="BU8" s="30"/>
+      <c r="BV8" s="30"/>
+      <c r="BW8" s="30"/>
+      <c r="BX8" s="30"/>
+      <c r="BY8" s="30"/>
+      <c r="BZ8" s="30"/>
+      <c r="CA8" s="30"/>
+      <c r="CB8" s="30"/>
+      <c r="CC8" s="30"/>
+      <c r="CD8" s="30"/>
+      <c r="CE8" s="30"/>
+      <c r="CF8" s="30"/>
+      <c r="CG8" s="30"/>
+      <c r="CH8" s="30"/>
+      <c r="CI8" s="30"/>
+      <c r="CJ8" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="CK8" s="39"/>
     </row>
-    <row r="9" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="33" t="s">
+    <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="P9" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="37" t="s">
+      <c r="Q9" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="12"/>
-      <c r="Y9" s="33" t="s">
+      <c r="Y9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="33" t="s">
+      <c r="AA9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="33" t="s">
+      <c r="AB9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="33" t="s">
+      <c r="AC9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="33" t="s">
+      <c r="AD9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="33" t="s">
+      <c r="AE9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="37" t="s">
+      <c r="AF9" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="37" t="s">
+      <c r="AG9" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="38"/>
-      <c r="AJ9" s="38"/>
-      <c r="AK9" s="38"/>
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="34"/>
       <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
       <c r="AN9" s="12"/>
-      <c r="AO9" s="30" t="s">
+      <c r="AO9" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="34" t="s">
+      <c r="AP9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="41" t="s">
+      <c r="AQ9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="41" t="s">
+      <c r="AR9" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="34" t="s">
+      <c r="AS9" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="34" t="s">
+      <c r="AT9" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="34" t="s">
+      <c r="AU9" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="41" t="s">
+      <c r="AV9" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="41" t="s">
+      <c r="AW9" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="41" t="s">
+      <c r="AX9" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="31" t="s">
+      <c r="AY9" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="34"/>
-      <c r="BA9" s="33"/>
-      <c r="BB9" s="33" t="s">
+      <c r="AZ9" s="32"/>
+      <c r="BA9" s="30"/>
+      <c r="BB9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="33" t="s">
+      <c r="BC9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="33" t="s">
+      <c r="BD9" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="33" t="s">
+      <c r="BE9" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="33" t="s">
+      <c r="BF9" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="33" t="s">
+      <c r="BG9" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="33" t="s">
+      <c r="BH9" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="33" t="s">
+      <c r="BI9" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="35" t="s">
+      <c r="BJ9" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="33" t="s">
+      <c r="BK9" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="33" t="s">
+      <c r="BL9" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="33" t="s">
+      <c r="BM9" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="33" t="s">
+      <c r="BN9" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="35" t="s">
+      <c r="BO9" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="BP9" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="BQ9" s="27"/>
+      <c r="BR9" s="27"/>
+      <c r="BS9" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT9" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU9" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="BV9" s="30"/>
+      <c r="BW9" s="30"/>
+      <c r="BX9" s="30"/>
+      <c r="BY9" s="30"/>
+      <c r="BZ9" s="30"/>
+      <c r="CA9" s="30"/>
+      <c r="CB9" s="30"/>
+      <c r="CC9" s="30"/>
+      <c r="CD9" s="30"/>
+      <c r="CE9" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="CF9" s="30"/>
+      <c r="CG9" s="30"/>
+      <c r="CH9" s="30"/>
+      <c r="CI9" s="30"/>
+      <c r="CJ9" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="BP9" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="BQ9" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="BR9" s="27"/>
-      <c r="BS9" s="27"/>
-      <c r="BT9" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="BU9" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="BV9" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="BW9" s="33"/>
-      <c r="BX9" s="33"/>
-      <c r="BY9" s="33"/>
-      <c r="BZ9" s="33"/>
-      <c r="CA9" s="33"/>
-      <c r="CB9" s="33"/>
-      <c r="CC9" s="33"/>
-      <c r="CD9" s="33"/>
-      <c r="CE9" s="33"/>
-      <c r="CF9" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="CG9" s="33"/>
-      <c r="CH9" s="33"/>
-      <c r="CI9" s="33"/>
-      <c r="CJ9" s="33"/>
+      <c r="CK9" s="45" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
+    <row r="10" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
       <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1673,14 +1705,14 @@
       <c r="X10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="33"/>
-      <c r="Z10" s="33"/>
-      <c r="AA10" s="33"/>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="33"/>
-      <c r="AD10" s="33"/>
-      <c r="AE10" s="33"/>
-      <c r="AF10" s="33"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
       <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1705,90 +1737,91 @@
       <c r="AN10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="34"/>
-      <c r="AP10" s="34"/>
-      <c r="AQ10" s="42"/>
-      <c r="AR10" s="42"/>
-      <c r="AS10" s="34"/>
-      <c r="AT10" s="34"/>
-      <c r="AU10" s="34"/>
-      <c r="AV10" s="42"/>
-      <c r="AW10" s="42"/>
-      <c r="AX10" s="42"/>
-      <c r="AY10" s="32"/>
-      <c r="AZ10" s="34"/>
-      <c r="BA10" s="33"/>
-      <c r="BB10" s="33"/>
-      <c r="BC10" s="33"/>
-      <c r="BD10" s="33"/>
-      <c r="BE10" s="33"/>
-      <c r="BF10" s="33"/>
-      <c r="BG10" s="33"/>
-      <c r="BH10" s="33"/>
-      <c r="BI10" s="33"/>
-      <c r="BJ10" s="36"/>
-      <c r="BK10" s="33"/>
-      <c r="BL10" s="33"/>
-      <c r="BM10" s="33"/>
-      <c r="BN10" s="33"/>
-      <c r="BO10" s="36"/>
-      <c r="BP10" s="33"/>
-      <c r="BQ10" s="33"/>
+      <c r="AO10" s="32"/>
+      <c r="AP10" s="32"/>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="32"/>
+      <c r="AT10" s="32"/>
+      <c r="AU10" s="32"/>
+      <c r="AV10" s="29"/>
+      <c r="AW10" s="29"/>
+      <c r="AX10" s="29"/>
+      <c r="AY10" s="43"/>
+      <c r="AZ10" s="32"/>
+      <c r="BA10" s="30"/>
+      <c r="BB10" s="30"/>
+      <c r="BC10" s="30"/>
+      <c r="BD10" s="30"/>
+      <c r="BE10" s="30"/>
+      <c r="BF10" s="30"/>
+      <c r="BG10" s="30"/>
+      <c r="BH10" s="30"/>
+      <c r="BI10" s="30"/>
+      <c r="BJ10" s="38"/>
+      <c r="BK10" s="30"/>
+      <c r="BL10" s="30"/>
+      <c r="BM10" s="30"/>
+      <c r="BN10" s="30"/>
+      <c r="BO10" s="30"/>
+      <c r="BP10" s="30"/>
+      <c r="BQ10" s="27" t="s">
+        <v>0</v>
+      </c>
       <c r="BR10" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="BS10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BT10" s="36"/>
-      <c r="BU10" s="33"/>
+      <c r="BS10" s="38"/>
+      <c r="BT10" s="30"/>
+      <c r="BU10" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="BV10" s="10" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="BW10" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BX10" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BY10" s="10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="BZ10" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="CA10" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="CB10" s="10" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="CC10" s="10" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="CD10" s="10" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="CE10" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="CF10" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="CG10" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="CH10" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="CI10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="CJ10" s="10" t="s">
         <v>129</v>
       </c>
+      <c r="CJ10" s="46"/>
+      <c r="CK10" s="46"/>
     </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
@@ -1966,7 +1999,7 @@
         <v>151</v>
       </c>
       <c r="BG11" s="16" t="e">
-        <f>IF(BP11&lt;=EOMONTH(BD11,12),"X","")</f>
+        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BH11" s="16" t="s">
@@ -1979,146 +2012,103 @@
         <v>58</v>
       </c>
       <c r="BK11" s="16" t="e">
-        <f>IF(BP11&lt;=EOMONTH(BD11,12),"X","")</f>
+        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BL11" s="16" t="e">
-        <f>IF(AND(BP11&gt;=EOMONTH(BD11,13),BP11&lt;=EOMONTH(BD11,48)),"X","")</f>
+        <f>IF(AND(BO11&gt;=EOMONTH(BD11,13),BO11&lt;=EOMONTH(BD11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BM11" s="16" t="e">
-        <f>IF(AND(BP11&gt;=EOMONTH(BD11,48),BP11&lt;=EOMONTH(BD11,72)),"X","")</f>
+        <f>IF(AND(BO11&gt;=EOMONTH(BD11,48),BO11&lt;=EOMONTH(BD11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="BN11" s="16" t="e">
-        <f>IF(BP11&gt;=EOMONTH(BD11,73),"X","")</f>
+        <f>IF(BO11&gt;=EOMONTH(BD11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="14" t="s">
+      <c r="BO11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="BP11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="BQ11" s="22" t="e">
+        <f>(EOMONTH(BO11,0))-(BO11-DAY(BO11)+1)+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BR11" s="22" t="e">
+        <f>BP11-BO11+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BS11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT11" s="23" t="e">
+        <f>BR11/BQ11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BU11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV11" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BW11" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BX11" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="BY11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="BZ11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="CA11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="CB11" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="CC11" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="CD11" s="23" t="e">
+        <f>CA11*BT11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="CE11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="CF11" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG11" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="CH11" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="CI11" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="CJ11" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="BP11" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="BQ11" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="BR11" s="22" t="e">
-        <f>(EOMONTH(BP11,0))-(BP11-DAY(BP11)+1)+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BS11" s="22" t="e">
-        <f>BQ11-BP11+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BT11" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="BU11" s="23" t="e">
-        <f>BS11/BR11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BV11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="BW11" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BX11" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="BY11" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BZ11" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="CA11" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="CB11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="CC11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="CD11" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="CE11" s="23" t="e">
-        <f>CB11*BU11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="CF11" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="CG11" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="CH11" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="CI11" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="CJ11" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="CK11" s="25" t="s">
+      <c r="CK11" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="CL11" s="25" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="BP8:CJ8"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BQ9:BQ10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="CF9:CJ9"/>
-    <mergeCell ref="BV9:CE9"/>
-    <mergeCell ref="BU9:BU10"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BB8:BO8"/>
+  <mergeCells count="67">
+    <mergeCell ref="CJ8:CK8"/>
+    <mergeCell ref="CJ9:CJ10"/>
+    <mergeCell ref="CK9:CK10"/>
     <mergeCell ref="AQ8:AY8"/>
     <mergeCell ref="AY9:AY10"/>
     <mergeCell ref="BI9:BI10"/>
@@ -2135,6 +2125,54 @@
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BJ9:BJ10"/>
     <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BO8:CI8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="BU9:CD9"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BB8:BN8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2795 ausserordentlicher Anspruch zu Statistiken hinzufügen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD55F5D-9378-4D45-B67C-2CAE87671815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C739D-635F-439A-BCA6-1F6F8A25C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -747,68 +747,71 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1279,7 +1282,7 @@
     <col min="85" max="85" width="13.5546875" customWidth="1"/>
     <col min="86" max="86" width="12.6640625" customWidth="1"/>
     <col min="87" max="87" width="12.6640625"/>
-    <col min="88" max="88" width="9.109375" style="44"/>
+    <col min="88" max="88" width="9.109375" style="28"/>
     <col min="89" max="89" width="9.109375" style="9"/>
     <col min="90" max="1010" width="10.44140625"/>
   </cols>
@@ -1349,338 +1352,338 @@
       <c r="C7"/>
     </row>
     <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="30" t="s">
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="37"/>
-      <c r="AI8" s="37"/>
-      <c r="AJ8" s="37"/>
-      <c r="AK8" s="37"/>
-      <c r="AL8" s="37"/>
-      <c r="AM8" s="37"/>
-      <c r="AN8" s="37"/>
-      <c r="AO8" s="32" t="s">
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="41"/>
+      <c r="AH8" s="41"/>
+      <c r="AI8" s="41"/>
+      <c r="AJ8" s="41"/>
+      <c r="AK8" s="41"/>
+      <c r="AL8" s="41"/>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="41"/>
+      <c r="AO8" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="32"/>
-      <c r="AQ8" s="40" t="s">
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="41"/>
-      <c r="AS8" s="41"/>
-      <c r="AT8" s="41"/>
-      <c r="AU8" s="41"/>
-      <c r="AV8" s="41"/>
-      <c r="AW8" s="41"/>
-      <c r="AX8" s="41"/>
-      <c r="AY8" s="31"/>
-      <c r="AZ8" s="32" t="s">
+      <c r="AR8" s="35"/>
+      <c r="AS8" s="35"/>
+      <c r="AT8" s="35"/>
+      <c r="AU8" s="35"/>
+      <c r="AV8" s="35"/>
+      <c r="AW8" s="35"/>
+      <c r="AX8" s="35"/>
+      <c r="AY8" s="36"/>
+      <c r="AZ8" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="30" t="s">
+      <c r="BA8" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="33" t="s">
+      <c r="BB8" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="34"/>
-      <c r="BD8" s="34"/>
-      <c r="BE8" s="34"/>
-      <c r="BF8" s="34"/>
-      <c r="BG8" s="34"/>
-      <c r="BH8" s="34"/>
-      <c r="BI8" s="34"/>
-      <c r="BJ8" s="34"/>
-      <c r="BK8" s="34"/>
-      <c r="BL8" s="34"/>
-      <c r="BM8" s="34"/>
-      <c r="BN8" s="34"/>
-      <c r="BO8" s="30" t="s">
+      <c r="BC8" s="43"/>
+      <c r="BD8" s="43"/>
+      <c r="BE8" s="43"/>
+      <c r="BF8" s="43"/>
+      <c r="BG8" s="43"/>
+      <c r="BH8" s="43"/>
+      <c r="BI8" s="43"/>
+      <c r="BJ8" s="43"/>
+      <c r="BK8" s="43"/>
+      <c r="BL8" s="43"/>
+      <c r="BM8" s="43"/>
+      <c r="BN8" s="43"/>
+      <c r="BO8" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="30"/>
-      <c r="BQ8" s="30"/>
-      <c r="BR8" s="30"/>
-      <c r="BS8" s="30"/>
-      <c r="BT8" s="30"/>
-      <c r="BU8" s="30"/>
-      <c r="BV8" s="30"/>
-      <c r="BW8" s="30"/>
-      <c r="BX8" s="30"/>
-      <c r="BY8" s="30"/>
-      <c r="BZ8" s="30"/>
-      <c r="CA8" s="30"/>
-      <c r="CB8" s="30"/>
-      <c r="CC8" s="30"/>
-      <c r="CD8" s="30"/>
-      <c r="CE8" s="30"/>
-      <c r="CF8" s="30"/>
-      <c r="CG8" s="30"/>
-      <c r="CH8" s="30"/>
-      <c r="CI8" s="30"/>
-      <c r="CJ8" s="33" t="s">
+      <c r="BP8" s="39"/>
+      <c r="BQ8" s="39"/>
+      <c r="BR8" s="39"/>
+      <c r="BS8" s="39"/>
+      <c r="BT8" s="39"/>
+      <c r="BU8" s="39"/>
+      <c r="BV8" s="39"/>
+      <c r="BW8" s="39"/>
+      <c r="BX8" s="39"/>
+      <c r="BY8" s="39"/>
+      <c r="BZ8" s="39"/>
+      <c r="CA8" s="39"/>
+      <c r="CB8" s="39"/>
+      <c r="CC8" s="39"/>
+      <c r="CD8" s="39"/>
+      <c r="CE8" s="39"/>
+      <c r="CF8" s="39"/>
+      <c r="CG8" s="39"/>
+      <c r="CH8" s="39"/>
+      <c r="CI8" s="39"/>
+      <c r="CJ8" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="CK8" s="39"/>
+      <c r="CK8" s="49"/>
     </row>
     <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="30" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="12"/>
-      <c r="Y9" s="30" t="s">
+      <c r="Y9" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="30" t="s">
+      <c r="Z9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="30" t="s">
+      <c r="AA9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="30" t="s">
+      <c r="AB9" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="30" t="s">
+      <c r="AC9" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="30" t="s">
+      <c r="AD9" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="30" t="s">
+      <c r="AE9" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="33" t="s">
+      <c r="AF9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="33" t="s">
+      <c r="AG9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="34"/>
-      <c r="AI9" s="34"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="34"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="43"/>
+      <c r="AJ9" s="43"/>
+      <c r="AK9" s="43"/>
       <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
       <c r="AN9" s="12"/>
-      <c r="AO9" s="31" t="s">
+      <c r="AO9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="32" t="s">
+      <c r="AP9" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="28" t="s">
+      <c r="AQ9" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="28" t="s">
+      <c r="AR9" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="32" t="s">
+      <c r="AS9" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="32" t="s">
+      <c r="AT9" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="32" t="s">
+      <c r="AU9" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="28" t="s">
+      <c r="AV9" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="28" t="s">
+      <c r="AW9" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="28" t="s">
+      <c r="AX9" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="42" t="s">
+      <c r="AY9" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="32"/>
-      <c r="BA9" s="30"/>
-      <c r="BB9" s="30" t="s">
+      <c r="AZ9" s="40"/>
+      <c r="BA9" s="39"/>
+      <c r="BB9" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="30" t="s">
+      <c r="BC9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="30" t="s">
+      <c r="BD9" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="30" t="s">
+      <c r="BE9" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="30" t="s">
+      <c r="BF9" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="30" t="s">
+      <c r="BG9" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="30" t="s">
+      <c r="BH9" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="30" t="s">
+      <c r="BI9" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="37" t="s">
+      <c r="BJ9" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="30" t="s">
+      <c r="BK9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="30" t="s">
+      <c r="BL9" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="30" t="s">
+      <c r="BM9" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="30" t="s">
+      <c r="BN9" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="30" t="s">
+      <c r="BO9" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="30" t="s">
+      <c r="BP9" s="39" t="s">
         <v>115</v>
       </c>
       <c r="BQ9" s="27"/>
       <c r="BR9" s="27"/>
-      <c r="BS9" s="37" t="s">
+      <c r="BS9" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="30" t="s">
+      <c r="BT9" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="30" t="s">
+      <c r="BU9" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="30"/>
-      <c r="BW9" s="30"/>
-      <c r="BX9" s="30"/>
-      <c r="BY9" s="30"/>
-      <c r="BZ9" s="30"/>
-      <c r="CA9" s="30"/>
-      <c r="CB9" s="30"/>
-      <c r="CC9" s="30"/>
-      <c r="CD9" s="30"/>
-      <c r="CE9" s="30" t="s">
+      <c r="BV9" s="39"/>
+      <c r="BW9" s="39"/>
+      <c r="BX9" s="39"/>
+      <c r="BY9" s="39"/>
+      <c r="BZ9" s="39"/>
+      <c r="CA9" s="39"/>
+      <c r="CB9" s="39"/>
+      <c r="CC9" s="39"/>
+      <c r="CD9" s="39"/>
+      <c r="CE9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="30"/>
-      <c r="CG9" s="30"/>
-      <c r="CH9" s="30"/>
-      <c r="CI9" s="30"/>
-      <c r="CJ9" s="45" t="s">
+      <c r="CF9" s="39"/>
+      <c r="CG9" s="39"/>
+      <c r="CH9" s="39"/>
+      <c r="CI9" s="39"/>
+      <c r="CJ9" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="CK9" s="32" t="s">
         <v>160</v>
-      </c>
-      <c r="CK9" s="45" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
       <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1705,14 +1708,14 @@
       <c r="X10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
       <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1737,42 +1740,42 @@
       <c r="AN10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="32"/>
-      <c r="AP10" s="32"/>
-      <c r="AQ10" s="29"/>
-      <c r="AR10" s="29"/>
-      <c r="AS10" s="32"/>
-      <c r="AT10" s="32"/>
-      <c r="AU10" s="32"/>
-      <c r="AV10" s="29"/>
-      <c r="AW10" s="29"/>
-      <c r="AX10" s="29"/>
-      <c r="AY10" s="43"/>
-      <c r="AZ10" s="32"/>
-      <c r="BA10" s="30"/>
-      <c r="BB10" s="30"/>
-      <c r="BC10" s="30"/>
-      <c r="BD10" s="30"/>
-      <c r="BE10" s="30"/>
-      <c r="BF10" s="30"/>
-      <c r="BG10" s="30"/>
-      <c r="BH10" s="30"/>
-      <c r="BI10" s="30"/>
-      <c r="BJ10" s="38"/>
-      <c r="BK10" s="30"/>
-      <c r="BL10" s="30"/>
-      <c r="BM10" s="30"/>
-      <c r="BN10" s="30"/>
-      <c r="BO10" s="30"/>
-      <c r="BP10" s="30"/>
+      <c r="AO10" s="40"/>
+      <c r="AP10" s="40"/>
+      <c r="AQ10" s="47"/>
+      <c r="AR10" s="47"/>
+      <c r="AS10" s="40"/>
+      <c r="AT10" s="40"/>
+      <c r="AU10" s="40"/>
+      <c r="AV10" s="47"/>
+      <c r="AW10" s="47"/>
+      <c r="AX10" s="47"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="40"/>
+      <c r="BA10" s="39"/>
+      <c r="BB10" s="39"/>
+      <c r="BC10" s="39"/>
+      <c r="BD10" s="39"/>
+      <c r="BE10" s="39"/>
+      <c r="BF10" s="39"/>
+      <c r="BG10" s="39"/>
+      <c r="BH10" s="39"/>
+      <c r="BI10" s="39"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="39"/>
+      <c r="BL10" s="39"/>
+      <c r="BM10" s="39"/>
+      <c r="BN10" s="39"/>
+      <c r="BO10" s="39"/>
+      <c r="BP10" s="39"/>
       <c r="BQ10" s="27" t="s">
         <v>0</v>
       </c>
       <c r="BR10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="38"/>
-      <c r="BT10" s="30"/>
+      <c r="BS10" s="42"/>
+      <c r="BT10" s="39"/>
       <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
@@ -1818,8 +1821,8 @@
       <c r="CI10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="CJ10" s="46"/>
-      <c r="CK10" s="46"/>
+      <c r="CJ10" s="33"/>
+      <c r="CK10" s="33"/>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
@@ -2094,11 +2097,11 @@
       <c r="CI11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="CJ11" s="47" t="s">
+      <c r="CJ11" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="CK11" s="29" t="s">
         <v>161</v>
-      </c>
-      <c r="CK11" s="48" t="s">
-        <v>164</v>
       </c>
       <c r="CL11" s="25" t="s">
         <v>54</v>
@@ -2106,22 +2109,42 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="CJ8:CK8"/>
-    <mergeCell ref="CJ9:CJ10"/>
-    <mergeCell ref="CK9:CK10"/>
-    <mergeCell ref="AQ8:AY8"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AZ8:AZ10"/>
-    <mergeCell ref="BA8:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="BF9:BF10"/>
     <mergeCell ref="BJ9:BJ10"/>
     <mergeCell ref="BG9:BG10"/>
@@ -2137,42 +2160,22 @@
     <mergeCell ref="BL9:BL10"/>
     <mergeCell ref="BM9:BM10"/>
     <mergeCell ref="BB8:BN8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="CJ8:CK8"/>
+    <mergeCell ref="CK9:CK10"/>
+    <mergeCell ref="CJ9:CJ10"/>
+    <mergeCell ref="AQ8:AY8"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AZ8:AZ10"/>
+    <mergeCell ref="BA8:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2795: display ausserordentlicherAnspruch in percentage instead of integer in reports
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C739D-635F-439A-BCA6-1F6F8A25C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643CF706-B584-46C8-8325-22CE5A016DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -753,12 +753,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -771,48 +804,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1225,69 +1223,71 @@
   </sheetPr>
   <dimension ref="A1:CL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CJ11" sqref="CJ11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625"/>
-    <col min="3" max="3" width="15.6640625" style="1"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.6640625"/>
-    <col min="17" max="18" width="10.6640625"/>
-    <col min="19" max="19" width="24.33203125" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
-    <col min="22" max="22" width="41.44140625" customWidth="1"/>
-    <col min="23" max="23" width="26.88671875" customWidth="1"/>
-    <col min="24" max="24" width="24.109375"/>
-    <col min="25" max="32" width="8.6640625"/>
-    <col min="33" max="34" width="10.6640625"/>
-    <col min="35" max="35" width="24.5546875" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625"/>
-    <col min="37" max="37" width="14.44140625" customWidth="1"/>
-    <col min="38" max="38" width="41.44140625" customWidth="1"/>
-    <col min="39" max="39" width="27.109375" customWidth="1"/>
-    <col min="40" max="40" width="24.109375"/>
-    <col min="41" max="41" width="9.109375" customWidth="1"/>
-    <col min="42" max="42" width="6.44140625"/>
-    <col min="43" max="43" width="18.109375"/>
-    <col min="45" max="45" width="23.33203125"/>
-    <col min="46" max="46" width="9.33203125"/>
-    <col min="47" max="47" width="25.44140625"/>
-    <col min="48" max="48" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="35.33203125" customWidth="1"/>
-    <col min="52" max="52" width="27.44140625"/>
-    <col min="53" max="53" width="10.44140625"/>
-    <col min="54" max="56" width="12.6640625"/>
-    <col min="57" max="57" width="16.6640625"/>
-    <col min="58" max="58" width="20.5546875" customWidth="1"/>
-    <col min="59" max="59" width="12.6640625"/>
-    <col min="60" max="60" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="8.7109375"/>
+    <col min="17" max="18" width="10.7109375"/>
+    <col min="19" max="19" width="24.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375"/>
+    <col min="21" max="21" width="14.42578125" customWidth="1"/>
+    <col min="22" max="22" width="41.42578125" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="24.140625"/>
+    <col min="25" max="32" width="8.7109375"/>
+    <col min="33" max="34" width="10.7109375"/>
+    <col min="35" max="35" width="24.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375"/>
+    <col min="37" max="37" width="14.42578125" customWidth="1"/>
+    <col min="38" max="38" width="41.42578125" customWidth="1"/>
+    <col min="39" max="39" width="27.140625" customWidth="1"/>
+    <col min="40" max="40" width="24.140625"/>
+    <col min="41" max="41" width="9.140625" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125"/>
+    <col min="43" max="43" width="18.140625"/>
+    <col min="45" max="45" width="23.28515625"/>
+    <col min="46" max="46" width="9.28515625"/>
+    <col min="47" max="47" width="25.42578125"/>
+    <col min="48" max="48" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="35.28515625" customWidth="1"/>
+    <col min="52" max="52" width="27.42578125"/>
+    <col min="53" max="53" width="10.42578125"/>
+    <col min="54" max="56" width="12.7109375"/>
+    <col min="57" max="57" width="16.7109375"/>
+    <col min="58" max="58" width="20.5703125" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375"/>
+    <col min="60" max="60" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="22"/>
-    <col min="62" max="62" width="18.109375" customWidth="1"/>
+    <col min="62" max="62" width="18.140625" customWidth="1"/>
     <col min="63" max="66" width="22"/>
-    <col min="67" max="68" width="12.6640625"/>
-    <col min="69" max="69" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="67" max="68" width="12.7109375"/>
+    <col min="69" max="69" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="70" max="70" width="16" hidden="1" customWidth="1"/>
     <col min="71" max="71" width="16" customWidth="1"/>
-    <col min="72" max="72" width="12.6640625"/>
-    <col min="73" max="74" width="13.33203125" customWidth="1"/>
-    <col min="75" max="75" width="13.6640625" customWidth="1"/>
-    <col min="76" max="76" width="16.88671875"/>
-    <col min="77" max="78" width="12.33203125" customWidth="1"/>
-    <col min="79" max="79" width="12.6640625"/>
-    <col min="80" max="80" width="19.44140625"/>
-    <col min="82" max="82" width="16.88671875"/>
-    <col min="83" max="84" width="12.6640625"/>
-    <col min="85" max="85" width="13.5546875" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" customWidth="1"/>
-    <col min="87" max="87" width="12.6640625"/>
-    <col min="88" max="88" width="9.109375" style="28"/>
-    <col min="89" max="89" width="9.109375" style="9"/>
-    <col min="90" max="1010" width="10.44140625"/>
+    <col min="72" max="72" width="12.7109375"/>
+    <col min="73" max="74" width="13.28515625" customWidth="1"/>
+    <col min="75" max="75" width="13.7109375" customWidth="1"/>
+    <col min="76" max="76" width="16.85546875"/>
+    <col min="77" max="78" width="12.28515625" customWidth="1"/>
+    <col min="79" max="79" width="12.7109375"/>
+    <col min="80" max="80" width="19.42578125"/>
+    <col min="82" max="82" width="16.85546875"/>
+    <col min="83" max="84" width="12.7109375"/>
+    <col min="85" max="85" width="13.5703125" customWidth="1"/>
+    <col min="86" max="86" width="12.7109375" customWidth="1"/>
+    <col min="87" max="87" width="12.7109375"/>
+    <col min="88" max="88" width="9.140625" style="28"/>
+    <col min="89" max="89" width="9.140625" style="9"/>
+    <col min="90" max="1010" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:90" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1299,10 +1299,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="BR3" s="24"/>
       <c r="BS3" s="24"/>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1348,342 +1348,342 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="39" t="s">
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="41"/>
-      <c r="AH8" s="41"/>
-      <c r="AI8" s="41"/>
-      <c r="AJ8" s="41"/>
-      <c r="AK8" s="41"/>
-      <c r="AL8" s="41"/>
-      <c r="AM8" s="41"/>
-      <c r="AN8" s="41"/>
-      <c r="AO8" s="40" t="s">
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="39"/>
+      <c r="AH8" s="39"/>
+      <c r="AI8" s="39"/>
+      <c r="AJ8" s="39"/>
+      <c r="AK8" s="39"/>
+      <c r="AL8" s="39"/>
+      <c r="AM8" s="39"/>
+      <c r="AN8" s="39"/>
+      <c r="AO8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="40"/>
-      <c r="AQ8" s="34" t="s">
+      <c r="AP8" s="34"/>
+      <c r="AQ8" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="35"/>
-      <c r="AS8" s="35"/>
-      <c r="AT8" s="35"/>
-      <c r="AU8" s="35"/>
-      <c r="AV8" s="35"/>
-      <c r="AW8" s="35"/>
-      <c r="AX8" s="35"/>
-      <c r="AY8" s="36"/>
-      <c r="AZ8" s="40" t="s">
+      <c r="AR8" s="46"/>
+      <c r="AS8" s="46"/>
+      <c r="AT8" s="46"/>
+      <c r="AU8" s="46"/>
+      <c r="AV8" s="46"/>
+      <c r="AW8" s="46"/>
+      <c r="AX8" s="46"/>
+      <c r="AY8" s="33"/>
+      <c r="AZ8" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="39" t="s">
+      <c r="BA8" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="31" t="s">
+      <c r="BB8" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="43"/>
-      <c r="BD8" s="43"/>
-      <c r="BE8" s="43"/>
-      <c r="BF8" s="43"/>
-      <c r="BG8" s="43"/>
-      <c r="BH8" s="43"/>
-      <c r="BI8" s="43"/>
-      <c r="BJ8" s="43"/>
-      <c r="BK8" s="43"/>
-      <c r="BL8" s="43"/>
-      <c r="BM8" s="43"/>
-      <c r="BN8" s="43"/>
-      <c r="BO8" s="39" t="s">
+      <c r="BC8" s="36"/>
+      <c r="BD8" s="36"/>
+      <c r="BE8" s="36"/>
+      <c r="BF8" s="36"/>
+      <c r="BG8" s="36"/>
+      <c r="BH8" s="36"/>
+      <c r="BI8" s="36"/>
+      <c r="BJ8" s="36"/>
+      <c r="BK8" s="36"/>
+      <c r="BL8" s="36"/>
+      <c r="BM8" s="36"/>
+      <c r="BN8" s="36"/>
+      <c r="BO8" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="39"/>
-      <c r="BQ8" s="39"/>
-      <c r="BR8" s="39"/>
-      <c r="BS8" s="39"/>
-      <c r="BT8" s="39"/>
-      <c r="BU8" s="39"/>
-      <c r="BV8" s="39"/>
-      <c r="BW8" s="39"/>
-      <c r="BX8" s="39"/>
-      <c r="BY8" s="39"/>
-      <c r="BZ8" s="39"/>
-      <c r="CA8" s="39"/>
-      <c r="CB8" s="39"/>
-      <c r="CC8" s="39"/>
-      <c r="CD8" s="39"/>
-      <c r="CE8" s="39"/>
-      <c r="CF8" s="39"/>
-      <c r="CG8" s="39"/>
-      <c r="CH8" s="39"/>
-      <c r="CI8" s="39"/>
-      <c r="CJ8" s="48" t="s">
+      <c r="BP8" s="32"/>
+      <c r="BQ8" s="32"/>
+      <c r="BR8" s="32"/>
+      <c r="BS8" s="32"/>
+      <c r="BT8" s="32"/>
+      <c r="BU8" s="32"/>
+      <c r="BV8" s="32"/>
+      <c r="BW8" s="32"/>
+      <c r="BX8" s="32"/>
+      <c r="BY8" s="32"/>
+      <c r="BZ8" s="32"/>
+      <c r="CA8" s="32"/>
+      <c r="CB8" s="32"/>
+      <c r="CC8" s="32"/>
+      <c r="CD8" s="32"/>
+      <c r="CE8" s="32"/>
+      <c r="CF8" s="32"/>
+      <c r="CG8" s="32"/>
+      <c r="CH8" s="32"/>
+      <c r="CI8" s="32"/>
+      <c r="CJ8" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="CK8" s="49"/>
+      <c r="CK8" s="42"/>
     </row>
-    <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="39" t="s">
+    <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="12"/>
-      <c r="Y9" s="39" t="s">
+      <c r="Y9" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="39" t="s">
+      <c r="Z9" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="39" t="s">
+      <c r="AA9" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="39" t="s">
+      <c r="AB9" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="39" t="s">
+      <c r="AC9" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="39" t="s">
+      <c r="AD9" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="39" t="s">
+      <c r="AE9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="31" t="s">
+      <c r="AF9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="31" t="s">
+      <c r="AG9" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="43"/>
-      <c r="AI9" s="43"/>
-      <c r="AJ9" s="43"/>
-      <c r="AK9" s="43"/>
+      <c r="AH9" s="36"/>
+      <c r="AI9" s="36"/>
+      <c r="AJ9" s="36"/>
+      <c r="AK9" s="36"/>
       <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
       <c r="AN9" s="12"/>
-      <c r="AO9" s="36" t="s">
+      <c r="AO9" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="40" t="s">
+      <c r="AP9" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="46" t="s">
+      <c r="AQ9" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="46" t="s">
+      <c r="AR9" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="40" t="s">
+      <c r="AS9" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="40" t="s">
+      <c r="AT9" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="40" t="s">
+      <c r="AU9" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="46" t="s">
+      <c r="AV9" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="46" t="s">
+      <c r="AW9" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="46" t="s">
+      <c r="AX9" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="37" t="s">
+      <c r="AY9" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="40"/>
-      <c r="BA9" s="39"/>
-      <c r="BB9" s="39" t="s">
+      <c r="AZ9" s="34"/>
+      <c r="BA9" s="32"/>
+      <c r="BB9" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="39" t="s">
+      <c r="BC9" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="39" t="s">
+      <c r="BD9" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="39" t="s">
+      <c r="BE9" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="39" t="s">
+      <c r="BF9" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="39" t="s">
+      <c r="BG9" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="39" t="s">
+      <c r="BH9" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="39" t="s">
+      <c r="BI9" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="41" t="s">
+      <c r="BJ9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="39" t="s">
+      <c r="BK9" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="39" t="s">
+      <c r="BL9" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="39" t="s">
+      <c r="BM9" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="39" t="s">
+      <c r="BN9" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="39" t="s">
+      <c r="BO9" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="39" t="s">
+      <c r="BP9" s="32" t="s">
         <v>115</v>
       </c>
       <c r="BQ9" s="27"/>
       <c r="BR9" s="27"/>
-      <c r="BS9" s="41" t="s">
+      <c r="BS9" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="39" t="s">
+      <c r="BT9" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="39" t="s">
+      <c r="BU9" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="39"/>
-      <c r="BW9" s="39"/>
-      <c r="BX9" s="39"/>
-      <c r="BY9" s="39"/>
-      <c r="BZ9" s="39"/>
-      <c r="CA9" s="39"/>
-      <c r="CB9" s="39"/>
-      <c r="CC9" s="39"/>
-      <c r="CD9" s="39"/>
-      <c r="CE9" s="39" t="s">
+      <c r="BV9" s="32"/>
+      <c r="BW9" s="32"/>
+      <c r="BX9" s="32"/>
+      <c r="BY9" s="32"/>
+      <c r="BZ9" s="32"/>
+      <c r="CA9" s="32"/>
+      <c r="CB9" s="32"/>
+      <c r="CC9" s="32"/>
+      <c r="CD9" s="32"/>
+      <c r="CE9" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="39"/>
-      <c r="CG9" s="39"/>
-      <c r="CH9" s="39"/>
-      <c r="CI9" s="39"/>
-      <c r="CJ9" s="32" t="s">
+      <c r="CF9" s="32"/>
+      <c r="CG9" s="32"/>
+      <c r="CH9" s="32"/>
+      <c r="CI9" s="32"/>
+      <c r="CJ9" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="CK9" s="32" t="s">
+      <c r="CK9" s="43" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
+    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
       <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1708,14 +1708,14 @@
       <c r="X10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="32"/>
+      <c r="AF10" s="32"/>
       <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1740,42 +1740,42 @@
       <c r="AN10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="40"/>
-      <c r="AP10" s="40"/>
-      <c r="AQ10" s="47"/>
-      <c r="AR10" s="47"/>
-      <c r="AS10" s="40"/>
-      <c r="AT10" s="40"/>
-      <c r="AU10" s="40"/>
-      <c r="AV10" s="47"/>
-      <c r="AW10" s="47"/>
-      <c r="AX10" s="47"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="40"/>
-      <c r="BA10" s="39"/>
-      <c r="BB10" s="39"/>
-      <c r="BC10" s="39"/>
-      <c r="BD10" s="39"/>
-      <c r="BE10" s="39"/>
-      <c r="BF10" s="39"/>
-      <c r="BG10" s="39"/>
-      <c r="BH10" s="39"/>
-      <c r="BI10" s="39"/>
-      <c r="BJ10" s="42"/>
-      <c r="BK10" s="39"/>
-      <c r="BL10" s="39"/>
-      <c r="BM10" s="39"/>
-      <c r="BN10" s="39"/>
-      <c r="BO10" s="39"/>
-      <c r="BP10" s="39"/>
+      <c r="AO10" s="34"/>
+      <c r="AP10" s="34"/>
+      <c r="AQ10" s="31"/>
+      <c r="AR10" s="31"/>
+      <c r="AS10" s="34"/>
+      <c r="AT10" s="34"/>
+      <c r="AU10" s="34"/>
+      <c r="AV10" s="31"/>
+      <c r="AW10" s="31"/>
+      <c r="AX10" s="31"/>
+      <c r="AY10" s="48"/>
+      <c r="AZ10" s="34"/>
+      <c r="BA10" s="32"/>
+      <c r="BB10" s="32"/>
+      <c r="BC10" s="32"/>
+      <c r="BD10" s="32"/>
+      <c r="BE10" s="32"/>
+      <c r="BF10" s="32"/>
+      <c r="BG10" s="32"/>
+      <c r="BH10" s="32"/>
+      <c r="BI10" s="32"/>
+      <c r="BJ10" s="40"/>
+      <c r="BK10" s="32"/>
+      <c r="BL10" s="32"/>
+      <c r="BM10" s="32"/>
+      <c r="BN10" s="32"/>
+      <c r="BO10" s="32"/>
+      <c r="BP10" s="32"/>
       <c r="BQ10" s="27" t="s">
         <v>0</v>
       </c>
       <c r="BR10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="42"/>
-      <c r="BT10" s="39"/>
+      <c r="BS10" s="40"/>
+      <c r="BT10" s="32"/>
       <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
@@ -1821,10 +1821,10 @@
       <c r="CI10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="CJ10" s="33"/>
-      <c r="CK10" s="33"/>
+      <c r="CJ10" s="44"/>
+      <c r="CK10" s="44"/>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2097,7 @@
       <c r="CI11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="CJ11" s="30" t="s">
+      <c r="CJ11" s="49" t="s">
         <v>164</v>
       </c>
       <c r="CK11" s="29" t="s">
@@ -2109,57 +2109,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BO8:CI8"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="BU9:CD9"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BB8:BN8"/>
     <mergeCell ref="CJ8:CK8"/>
     <mergeCell ref="CK9:CK10"/>
     <mergeCell ref="CJ9:CJ10"/>
@@ -2176,6 +2125,57 @@
     <mergeCell ref="BC9:BC10"/>
     <mergeCell ref="BD9:BD10"/>
     <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BO8:CI8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="BU9:CD9"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BB8:BN8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:U9"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2795 spalte KeinPlatzImSchulhort soll bei anderen Mandanten als Luzern ausgeblendet werden.
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643CF706-B584-46C8-8325-22CE5A016DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5A7ABA-F7CD-4BF3-8C4C-47CF330499D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,13 +521,13 @@
     <t>{keinPlatzImSchulhort}</t>
   </si>
   <si>
-    <t>{zusatzFelderGemeinden}</t>
-  </si>
-  <si>
     <t>{ausserordentlicherAnspruchTitle}</t>
   </si>
   <si>
     <t>{ausserordentlicherAnspruch}</t>
+  </si>
+  <si>
+    <t>{repeatSchulhort}</t>
   </si>
 </sst>
 </file>
@@ -694,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -747,70 +747,63 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1223,9 +1216,7 @@
   </sheetPr>
   <dimension ref="A1:CL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CJ11" sqref="CJ11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1278,11 +1269,10 @@
     <col min="79" max="79" width="12.7109375"/>
     <col min="80" max="80" width="19.42578125"/>
     <col min="82" max="82" width="16.85546875"/>
-    <col min="83" max="84" width="12.7109375"/>
-    <col min="85" max="85" width="13.5703125" customWidth="1"/>
-    <col min="86" max="86" width="12.7109375" customWidth="1"/>
-    <col min="87" max="87" width="12.7109375"/>
-    <col min="88" max="88" width="9.140625" style="28"/>
+    <col min="84" max="85" width="12.7109375"/>
+    <col min="86" max="86" width="13.5703125" customWidth="1"/>
+    <col min="87" max="87" width="12.7109375" customWidth="1"/>
+    <col min="88" max="88" width="12.7109375"/>
     <col min="89" max="89" width="9.140625" style="9"/>
     <col min="90" max="1010" width="10.42578125"/>
   </cols>
@@ -1352,338 +1342,336 @@
       <c r="C7"/>
     </row>
     <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="32" t="s">
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="32"/>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="32"/>
-      <c r="AF8" s="32"/>
-      <c r="AG8" s="39"/>
-      <c r="AH8" s="39"/>
-      <c r="AI8" s="39"/>
-      <c r="AJ8" s="39"/>
-      <c r="AK8" s="39"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="34" t="s">
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="38"/>
+      <c r="AJ8" s="38"/>
+      <c r="AK8" s="38"/>
+      <c r="AL8" s="38"/>
+      <c r="AM8" s="38"/>
+      <c r="AN8" s="38"/>
+      <c r="AO8" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="34"/>
-      <c r="AQ8" s="45" t="s">
+      <c r="AP8" s="37"/>
+      <c r="AQ8" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="46"/>
-      <c r="AS8" s="46"/>
-      <c r="AT8" s="46"/>
-      <c r="AU8" s="46"/>
-      <c r="AV8" s="46"/>
-      <c r="AW8" s="46"/>
-      <c r="AX8" s="46"/>
+      <c r="AR8" s="32"/>
+      <c r="AS8" s="32"/>
+      <c r="AT8" s="32"/>
+      <c r="AU8" s="32"/>
+      <c r="AV8" s="32"/>
+      <c r="AW8" s="32"/>
+      <c r="AX8" s="32"/>
       <c r="AY8" s="33"/>
-      <c r="AZ8" s="34" t="s">
+      <c r="AZ8" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="32" t="s">
+      <c r="BA8" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="35" t="s">
+      <c r="BB8" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="36"/>
-      <c r="BD8" s="36"/>
-      <c r="BE8" s="36"/>
-      <c r="BF8" s="36"/>
-      <c r="BG8" s="36"/>
-      <c r="BH8" s="36"/>
-      <c r="BI8" s="36"/>
-      <c r="BJ8" s="36"/>
-      <c r="BK8" s="36"/>
-      <c r="BL8" s="36"/>
-      <c r="BM8" s="36"/>
-      <c r="BN8" s="36"/>
-      <c r="BO8" s="32" t="s">
+      <c r="BC8" s="41"/>
+      <c r="BD8" s="41"/>
+      <c r="BE8" s="41"/>
+      <c r="BF8" s="41"/>
+      <c r="BG8" s="41"/>
+      <c r="BH8" s="41"/>
+      <c r="BI8" s="41"/>
+      <c r="BJ8" s="41"/>
+      <c r="BK8" s="41"/>
+      <c r="BL8" s="41"/>
+      <c r="BM8" s="41"/>
+      <c r="BN8" s="41"/>
+      <c r="BO8" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="32"/>
-      <c r="BQ8" s="32"/>
-      <c r="BR8" s="32"/>
-      <c r="BS8" s="32"/>
-      <c r="BT8" s="32"/>
-      <c r="BU8" s="32"/>
-      <c r="BV8" s="32"/>
-      <c r="BW8" s="32"/>
-      <c r="BX8" s="32"/>
-      <c r="BY8" s="32"/>
-      <c r="BZ8" s="32"/>
-      <c r="CA8" s="32"/>
-      <c r="CB8" s="32"/>
-      <c r="CC8" s="32"/>
-      <c r="CD8" s="32"/>
-      <c r="CE8" s="32"/>
-      <c r="CF8" s="32"/>
-      <c r="CG8" s="32"/>
-      <c r="CH8" s="32"/>
-      <c r="CI8" s="32"/>
-      <c r="CJ8" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="CK8" s="42"/>
+      <c r="BP8" s="36"/>
+      <c r="BQ8" s="36"/>
+      <c r="BR8" s="36"/>
+      <c r="BS8" s="36"/>
+      <c r="BT8" s="36"/>
+      <c r="BU8" s="36"/>
+      <c r="BV8" s="36"/>
+      <c r="BW8" s="36"/>
+      <c r="BX8" s="36"/>
+      <c r="BY8" s="36"/>
+      <c r="BZ8" s="36"/>
+      <c r="CA8" s="36"/>
+      <c r="CB8" s="36"/>
+      <c r="CC8" s="36"/>
+      <c r="CD8" s="36"/>
+      <c r="CE8" s="36"/>
+      <c r="CF8" s="36"/>
+      <c r="CG8" s="36"/>
+      <c r="CH8" s="36"/>
+      <c r="CI8" s="36"/>
+      <c r="CJ8" s="36"/>
+      <c r="CK8" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="32" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="O9" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="35" t="s">
+      <c r="Q9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="12"/>
-      <c r="Y9" s="32" t="s">
+      <c r="Y9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="32" t="s">
+      <c r="Z9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="32" t="s">
+      <c r="AA9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="32" t="s">
+      <c r="AB9" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="AC9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="32" t="s">
+      <c r="AD9" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="32" t="s">
+      <c r="AE9" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="35" t="s">
+      <c r="AF9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="35" t="s">
+      <c r="AG9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="36"/>
-      <c r="AI9" s="36"/>
-      <c r="AJ9" s="36"/>
-      <c r="AK9" s="36"/>
+      <c r="AH9" s="41"/>
+      <c r="AI9" s="41"/>
+      <c r="AJ9" s="41"/>
+      <c r="AK9" s="41"/>
       <c r="AL9" s="26"/>
       <c r="AM9" s="26"/>
       <c r="AN9" s="12"/>
       <c r="AO9" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="34" t="s">
+      <c r="AP9" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="30" t="s">
+      <c r="AQ9" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="30" t="s">
+      <c r="AR9" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="34" t="s">
+      <c r="AS9" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="34" t="s">
+      <c r="AT9" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="34" t="s">
+      <c r="AU9" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="30" t="s">
+      <c r="AV9" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="30" t="s">
+      <c r="AW9" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="30" t="s">
+      <c r="AX9" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="47" t="s">
+      <c r="AY9" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="34"/>
-      <c r="BA9" s="32"/>
-      <c r="BB9" s="32" t="s">
+      <c r="AZ9" s="37"/>
+      <c r="BA9" s="36"/>
+      <c r="BB9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="32" t="s">
+      <c r="BC9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="32" t="s">
+      <c r="BD9" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="32" t="s">
+      <c r="BE9" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="32" t="s">
+      <c r="BF9" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="32" t="s">
+      <c r="BG9" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="32" t="s">
+      <c r="BH9" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="32" t="s">
+      <c r="BI9" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="39" t="s">
+      <c r="BJ9" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="32" t="s">
+      <c r="BK9" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="32" t="s">
+      <c r="BL9" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="32" t="s">
+      <c r="BM9" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="32" t="s">
+      <c r="BN9" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="32" t="s">
+      <c r="BO9" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="32" t="s">
+      <c r="BP9" s="36" t="s">
         <v>115</v>
       </c>
       <c r="BQ9" s="27"/>
       <c r="BR9" s="27"/>
-      <c r="BS9" s="39" t="s">
+      <c r="BS9" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="32" t="s">
+      <c r="BT9" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="32" t="s">
+      <c r="BU9" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="32"/>
-      <c r="BW9" s="32"/>
-      <c r="BX9" s="32"/>
-      <c r="BY9" s="32"/>
-      <c r="BZ9" s="32"/>
-      <c r="CA9" s="32"/>
-      <c r="CB9" s="32"/>
-      <c r="CC9" s="32"/>
-      <c r="CD9" s="32"/>
-      <c r="CE9" s="32" t="s">
+      <c r="BV9" s="41"/>
+      <c r="BW9" s="41"/>
+      <c r="BX9" s="41"/>
+      <c r="BY9" s="41"/>
+      <c r="BZ9" s="41"/>
+      <c r="CA9" s="41"/>
+      <c r="CB9" s="41"/>
+      <c r="CC9" s="41"/>
+      <c r="CD9" s="41"/>
+      <c r="CE9" s="46"/>
+      <c r="CF9" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="CF9" s="32"/>
-      <c r="CG9" s="32"/>
-      <c r="CH9" s="32"/>
-      <c r="CI9" s="32"/>
-      <c r="CJ9" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="CK9" s="43" t="s">
+      <c r="CG9" s="36"/>
+      <c r="CH9" s="36"/>
+      <c r="CI9" s="36"/>
+      <c r="CJ9" s="36"/>
+      <c r="CK9" s="29" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
       <c r="Q10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1708,14 +1696,14 @@
       <c r="X10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32"/>
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="36"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="36"/>
+      <c r="AD10" s="36"/>
+      <c r="AE10" s="36"/>
+      <c r="AF10" s="36"/>
       <c r="AG10" s="15" t="s">
         <v>84</v>
       </c>
@@ -1740,42 +1728,42 @@
       <c r="AN10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="34"/>
-      <c r="AP10" s="34"/>
-      <c r="AQ10" s="31"/>
-      <c r="AR10" s="31"/>
-      <c r="AS10" s="34"/>
-      <c r="AT10" s="34"/>
-      <c r="AU10" s="34"/>
-      <c r="AV10" s="31"/>
-      <c r="AW10" s="31"/>
-      <c r="AX10" s="31"/>
-      <c r="AY10" s="48"/>
-      <c r="AZ10" s="34"/>
-      <c r="BA10" s="32"/>
-      <c r="BB10" s="32"/>
-      <c r="BC10" s="32"/>
-      <c r="BD10" s="32"/>
-      <c r="BE10" s="32"/>
-      <c r="BF10" s="32"/>
-      <c r="BG10" s="32"/>
-      <c r="BH10" s="32"/>
-      <c r="BI10" s="32"/>
-      <c r="BJ10" s="40"/>
-      <c r="BK10" s="32"/>
-      <c r="BL10" s="32"/>
-      <c r="BM10" s="32"/>
-      <c r="BN10" s="32"/>
-      <c r="BO10" s="32"/>
-      <c r="BP10" s="32"/>
+      <c r="AO10" s="37"/>
+      <c r="AP10" s="37"/>
+      <c r="AQ10" s="45"/>
+      <c r="AR10" s="45"/>
+      <c r="AS10" s="37"/>
+      <c r="AT10" s="37"/>
+      <c r="AU10" s="37"/>
+      <c r="AV10" s="45"/>
+      <c r="AW10" s="45"/>
+      <c r="AX10" s="45"/>
+      <c r="AY10" s="35"/>
+      <c r="AZ10" s="37"/>
+      <c r="BA10" s="36"/>
+      <c r="BB10" s="36"/>
+      <c r="BC10" s="36"/>
+      <c r="BD10" s="36"/>
+      <c r="BE10" s="36"/>
+      <c r="BF10" s="36"/>
+      <c r="BG10" s="36"/>
+      <c r="BH10" s="36"/>
+      <c r="BI10" s="36"/>
+      <c r="BJ10" s="39"/>
+      <c r="BK10" s="36"/>
+      <c r="BL10" s="36"/>
+      <c r="BM10" s="36"/>
+      <c r="BN10" s="36"/>
+      <c r="BO10" s="36"/>
+      <c r="BP10" s="36"/>
       <c r="BQ10" s="27" t="s">
         <v>0</v>
       </c>
       <c r="BR10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="40"/>
-      <c r="BT10" s="32"/>
+      <c r="BS10" s="39"/>
+      <c r="BT10" s="36"/>
       <c r="BU10" s="10" t="s">
         <v>113</v>
       </c>
@@ -1807,22 +1795,24 @@
         <v>121</v>
       </c>
       <c r="CE10" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="CF10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="CF10" s="10" t="s">
+      <c r="CG10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="CG10" s="10" t="s">
+      <c r="CH10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="CH10" s="10" t="s">
+      <c r="CI10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="CI10" s="10" t="s">
+      <c r="CJ10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="CJ10" s="44"/>
-      <c r="CK10" s="44"/>
+      <c r="CK10" s="30"/>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -2082,25 +2072,25 @@
         <f>CA11*BT11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="CE11" s="18" t="s">
+      <c r="CE11" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="CF11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CF11" s="18" t="s">
+      <c r="CG11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CG11" s="18" t="s">
+      <c r="CH11" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="CH11" s="18" t="s">
+      <c r="CI11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="CI11" s="18" t="s">
+      <c r="CJ11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="CJ11" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="CK11" s="29" t="s">
+      <c r="CK11" s="28" t="s">
         <v>161</v>
       </c>
       <c r="CL11" s="25" t="s">
@@ -2108,60 +2098,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="CJ8:CK8"/>
-    <mergeCell ref="CK9:CK10"/>
-    <mergeCell ref="CJ9:CJ10"/>
-    <mergeCell ref="AQ8:AY8"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AZ8:AZ10"/>
-    <mergeCell ref="BA8:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BO8:CI8"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="BU9:CD9"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BL9:BL10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BB8:BN8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="65">
     <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="AW9:AW10"/>
     <mergeCell ref="AX9:AX10"/>
@@ -2176,6 +2113,57 @@
     <mergeCell ref="Q9:U9"/>
     <mergeCell ref="AQ9:AQ10"/>
     <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:X8"/>
+    <mergeCell ref="Y8:AN8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BO8:CJ8"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="CF9:CJ9"/>
+    <mergeCell ref="BT9:BT10"/>
+    <mergeCell ref="BS9:BS10"/>
+    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BM9:BM10"/>
+    <mergeCell ref="BB8:BN8"/>
+    <mergeCell ref="BU9:CE9"/>
+    <mergeCell ref="CK9:CK10"/>
+    <mergeCell ref="AQ8:AY8"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AZ8:AZ10"/>
+    <mergeCell ref="BA8:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BE9:BE10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-3006: Add Auszahlungsdaten zu Antragstellende-Kinder Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5A7ABA-F7CD-4BF3-8C4C-47CF330499D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108DD935-6925-4EFC-B73D-AE754A94B274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="170">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -528,6 +528,21 @@
   </si>
   <si>
     <t>{repeatSchulhort}</t>
+  </si>
+  <si>
+    <t>{auszahlungsdatenGSTitel}</t>
+  </si>
+  <si>
+    <t>{ibanTitel}</t>
+  </si>
+  <si>
+    <t>{lautendAufTitel}</t>
+  </si>
+  <si>
+    <t>{lautendAuf}</t>
+  </si>
+  <si>
+    <t>{iban}</t>
   </si>
 </sst>
 </file>
@@ -789,6 +804,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -800,9 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -891,9 +906,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -931,9 +946,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -966,26 +981,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,26 +1016,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1214,70 +1195,73 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CL11"/>
+  <dimension ref="A1:CN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="9" max="16" width="8.7109375"/>
-    <col min="17" max="18" width="10.7109375"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="41.42578125" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" customWidth="1"/>
-    <col min="24" max="24" width="24.140625"/>
-    <col min="25" max="32" width="8.7109375"/>
-    <col min="33" max="34" width="10.7109375"/>
-    <col min="35" max="35" width="24.5703125" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375"/>
-    <col min="37" max="37" width="14.42578125" customWidth="1"/>
-    <col min="38" max="38" width="41.42578125" customWidth="1"/>
-    <col min="39" max="39" width="27.140625" customWidth="1"/>
-    <col min="40" max="40" width="24.140625"/>
-    <col min="41" max="41" width="9.140625" customWidth="1"/>
-    <col min="42" max="42" width="6.42578125"/>
-    <col min="43" max="43" width="18.140625"/>
-    <col min="45" max="45" width="23.28515625"/>
-    <col min="46" max="46" width="9.28515625"/>
-    <col min="47" max="47" width="25.42578125"/>
-    <col min="48" max="48" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="35.28515625" customWidth="1"/>
-    <col min="52" max="52" width="27.42578125"/>
-    <col min="53" max="53" width="10.42578125"/>
-    <col min="54" max="56" width="12.7109375"/>
-    <col min="57" max="57" width="16.7109375"/>
-    <col min="58" max="58" width="20.5703125" customWidth="1"/>
-    <col min="59" max="59" width="12.7109375"/>
-    <col min="60" max="60" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22"/>
-    <col min="62" max="62" width="18.140625" customWidth="1"/>
-    <col min="63" max="66" width="22"/>
-    <col min="67" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="16" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="16" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375"/>
-    <col min="73" max="74" width="13.28515625" customWidth="1"/>
-    <col min="75" max="75" width="13.7109375" customWidth="1"/>
-    <col min="76" max="76" width="16.85546875"/>
-    <col min="77" max="78" width="12.28515625" customWidth="1"/>
-    <col min="79" max="79" width="12.7109375"/>
-    <col min="80" max="80" width="19.42578125"/>
-    <col min="82" max="82" width="16.85546875"/>
-    <col min="84" max="85" width="12.7109375"/>
-    <col min="86" max="86" width="13.5703125" customWidth="1"/>
-    <col min="87" max="87" width="12.7109375" customWidth="1"/>
-    <col min="88" max="88" width="12.7109375"/>
-    <col min="89" max="89" width="9.140625" style="9"/>
-    <col min="90" max="1010" width="10.42578125"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="12" max="18" width="8.6640625"/>
+    <col min="19" max="20" width="10.6640625"/>
+    <col min="21" max="21" width="24.33203125" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625"/>
+    <col min="23" max="23" width="14.44140625" customWidth="1"/>
+    <col min="24" max="24" width="41.44140625" customWidth="1"/>
+    <col min="25" max="25" width="26.88671875" customWidth="1"/>
+    <col min="26" max="26" width="24.109375"/>
+    <col min="27" max="34" width="8.6640625"/>
+    <col min="35" max="36" width="10.6640625"/>
+    <col min="37" max="37" width="24.5546875" customWidth="1"/>
+    <col min="38" max="38" width="10.6640625"/>
+    <col min="39" max="39" width="14.44140625" customWidth="1"/>
+    <col min="40" max="40" width="41.44140625" customWidth="1"/>
+    <col min="41" max="41" width="27.109375" customWidth="1"/>
+    <col min="42" max="42" width="24.109375"/>
+    <col min="43" max="43" width="9.109375" customWidth="1"/>
+    <col min="44" max="44" width="6.44140625"/>
+    <col min="45" max="45" width="18.109375"/>
+    <col min="47" max="47" width="23.33203125"/>
+    <col min="48" max="48" width="9.33203125"/>
+    <col min="49" max="49" width="25.44140625"/>
+    <col min="50" max="50" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="35.33203125" customWidth="1"/>
+    <col min="54" max="54" width="27.44140625"/>
+    <col min="55" max="55" width="10.44140625"/>
+    <col min="56" max="58" width="12.6640625"/>
+    <col min="59" max="59" width="16.6640625"/>
+    <col min="60" max="60" width="20.5546875" customWidth="1"/>
+    <col min="61" max="61" width="12.6640625"/>
+    <col min="62" max="62" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22"/>
+    <col min="64" max="64" width="18.109375" customWidth="1"/>
+    <col min="65" max="68" width="22"/>
+    <col min="69" max="70" width="12.6640625"/>
+    <col min="71" max="71" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="16" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="16" customWidth="1"/>
+    <col min="74" max="74" width="12.6640625"/>
+    <col min="75" max="76" width="13.33203125" customWidth="1"/>
+    <col min="77" max="77" width="13.6640625" customWidth="1"/>
+    <col min="78" max="78" width="16.88671875"/>
+    <col min="79" max="80" width="12.33203125" customWidth="1"/>
+    <col min="81" max="81" width="12.6640625"/>
+    <col min="82" max="82" width="19.44140625"/>
+    <col min="84" max="84" width="16.88671875"/>
+    <col min="86" max="87" width="12.6640625"/>
+    <col min="88" max="88" width="13.5546875" customWidth="1"/>
+    <col min="89" max="89" width="12.6640625" customWidth="1"/>
+    <col min="90" max="90" width="12.6640625"/>
+    <col min="91" max="91" width="9.109375" style="9"/>
+    <col min="92" max="1012" width="10.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:92" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1288,11 +1272,13 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -1303,11 +1289,13 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="BQ3" s="24"/>
-      <c r="BR3" s="24"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
+      <c r="BU3" s="24"/>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1316,7 +1304,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1325,7 +1313,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1338,96 +1326,98 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:92" x14ac:dyDescent="0.3">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:90" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:92" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
       <c r="S8" s="38"/>
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
       <c r="V8" s="38"/>
       <c r="W8" s="38"/>
       <c r="X8" s="38"/>
-      <c r="Y8" s="36" t="s">
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="36"/>
       <c r="AB8" s="36"/>
       <c r="AC8" s="36"/>
       <c r="AD8" s="36"/>
       <c r="AE8" s="36"/>
       <c r="AF8" s="36"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="36"/>
       <c r="AI8" s="38"/>
       <c r="AJ8" s="38"/>
       <c r="AK8" s="38"/>
       <c r="AL8" s="38"/>
       <c r="AM8" s="38"/>
       <c r="AN8" s="38"/>
-      <c r="AO8" s="37" t="s">
+      <c r="AO8" s="38"/>
+      <c r="AP8" s="38"/>
+      <c r="AQ8" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="AP8" s="37"/>
-      <c r="AQ8" s="31" t="s">
+      <c r="AR8" s="37"/>
+      <c r="AS8" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="32"/>
-      <c r="AS8" s="32"/>
       <c r="AT8" s="32"/>
       <c r="AU8" s="32"/>
       <c r="AV8" s="32"/>
       <c r="AW8" s="32"/>
       <c r="AX8" s="32"/>
-      <c r="AY8" s="33"/>
-      <c r="AZ8" s="37" t="s">
+      <c r="AY8" s="32"/>
+      <c r="AZ8" s="32"/>
+      <c r="BA8" s="33"/>
+      <c r="BB8" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="BA8" s="36" t="s">
+      <c r="BC8" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="BB8" s="40" t="s">
+      <c r="BD8" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="BC8" s="41"/>
-      <c r="BD8" s="41"/>
       <c r="BE8" s="41"/>
       <c r="BF8" s="41"/>
       <c r="BG8" s="41"/>
@@ -1438,11 +1428,11 @@
       <c r="BL8" s="41"/>
       <c r="BM8" s="41"/>
       <c r="BN8" s="41"/>
-      <c r="BO8" s="36" t="s">
+      <c r="BO8" s="41"/>
+      <c r="BP8" s="41"/>
+      <c r="BQ8" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="BP8" s="36"/>
-      <c r="BQ8" s="36"/>
       <c r="BR8" s="36"/>
       <c r="BS8" s="36"/>
       <c r="BT8" s="36"/>
@@ -1462,180 +1452,186 @@
       <c r="CH8" s="36"/>
       <c r="CI8" s="36"/>
       <c r="CJ8" s="36"/>
-      <c r="CK8" t="s">
+      <c r="CK8" s="36"/>
+      <c r="CL8" s="36"/>
+      <c r="CM8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="36" t="s">
+    <row r="9" spans="1:92" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="K9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="L9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="M9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="N9" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="O9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="P9" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="Q9" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="40" t="s">
+      <c r="R9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="40" t="s">
+      <c r="S9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
       <c r="T9" s="41"/>
       <c r="U9" s="41"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="36" t="s">
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="Z9" s="36" t="s">
+      <c r="AB9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="36" t="s">
+      <c r="AC9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="36" t="s">
+      <c r="AD9" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="36" t="s">
+      <c r="AE9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="AD9" s="36" t="s">
+      <c r="AF9" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="36" t="s">
+      <c r="AG9" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" s="40" t="s">
+      <c r="AH9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="AG9" s="40" t="s">
+      <c r="AI9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="AH9" s="41"/>
-      <c r="AI9" s="41"/>
       <c r="AJ9" s="41"/>
       <c r="AK9" s="41"/>
-      <c r="AL9" s="26"/>
-      <c r="AM9" s="26"/>
-      <c r="AN9" s="12"/>
-      <c r="AO9" s="33" t="s">
+      <c r="AL9" s="41"/>
+      <c r="AM9" s="41"/>
+      <c r="AN9" s="26"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="12"/>
+      <c r="AQ9" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="AP9" s="37" t="s">
+      <c r="AR9" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="AQ9" s="44" t="s">
+      <c r="AS9" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="AR9" s="44" t="s">
+      <c r="AT9" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="AS9" s="37" t="s">
+      <c r="AU9" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="AT9" s="37" t="s">
+      <c r="AV9" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="AU9" s="37" t="s">
+      <c r="AW9" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="AV9" s="44" t="s">
+      <c r="AX9" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="AW9" s="44" t="s">
+      <c r="AY9" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="AX9" s="44" t="s">
+      <c r="AZ9" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="34" t="s">
+      <c r="BA9" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="AZ9" s="37"/>
-      <c r="BA9" s="36"/>
-      <c r="BB9" s="36" t="s">
+      <c r="BB9" s="37"/>
+      <c r="BC9" s="36"/>
+      <c r="BD9" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="BC9" s="36" t="s">
+      <c r="BE9" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="BD9" s="36" t="s">
+      <c r="BF9" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="BE9" s="36" t="s">
+      <c r="BG9" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="BF9" s="36" t="s">
+      <c r="BH9" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="BG9" s="36" t="s">
+      <c r="BI9" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" s="36" t="s">
+      <c r="BJ9" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" s="36" t="s">
+      <c r="BK9" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" s="38" t="s">
+      <c r="BL9" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" s="36" t="s">
+      <c r="BM9" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" s="36" t="s">
+      <c r="BN9" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" s="36" t="s">
+      <c r="BO9" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" s="36" t="s">
+      <c r="BP9" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" s="36" t="s">
+      <c r="BQ9" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="BP9" s="36" t="s">
+      <c r="BR9" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="BQ9" s="27"/>
-      <c r="BR9" s="27"/>
-      <c r="BS9" s="38" t="s">
+      <c r="BS9" s="27"/>
+      <c r="BT9" s="27"/>
+      <c r="BU9" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="BT9" s="36" t="s">
+      <c r="BV9" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="BU9" s="40" t="s">
+      <c r="BW9" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="BV9" s="41"/>
-      <c r="BW9" s="41"/>
       <c r="BX9" s="41"/>
       <c r="BY9" s="41"/>
       <c r="BZ9" s="41"/>
@@ -1643,105 +1639,107 @@
       <c r="CB9" s="41"/>
       <c r="CC9" s="41"/>
       <c r="CD9" s="41"/>
-      <c r="CE9" s="46"/>
-      <c r="CF9" s="36" t="s">
+      <c r="CE9" s="41"/>
+      <c r="CF9" s="41"/>
+      <c r="CG9" s="42"/>
+      <c r="CH9" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="CG9" s="36"/>
-      <c r="CH9" s="36"/>
       <c r="CI9" s="36"/>
       <c r="CJ9" s="36"/>
-      <c r="CK9" s="29" t="s">
+      <c r="CK9" s="36"/>
+      <c r="CL9" s="36"/>
+      <c r="CM9" s="29" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+    <row r="10" spans="1:92" x14ac:dyDescent="0.3">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="T10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="15" t="s">
+      <c r="U10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="V10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="U10" s="15" t="s">
+      <c r="W10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="X10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="Y10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="Z10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="36"/>
       <c r="AA10" s="36"/>
       <c r="AB10" s="36"/>
       <c r="AC10" s="36"/>
       <c r="AD10" s="36"/>
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
-      <c r="AG10" s="15" t="s">
+      <c r="AG10" s="36"/>
+      <c r="AH10" s="36"/>
+      <c r="AI10" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AH10" s="15" t="s">
+      <c r="AJ10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AI10" s="15" t="s">
+      <c r="AK10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AJ10" s="15" t="s">
+      <c r="AL10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AK10" s="15" t="s">
+      <c r="AM10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AL10" s="15" t="s">
+      <c r="AN10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="AM10" s="15" t="s">
+      <c r="AO10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="AN10" s="15" t="s">
+      <c r="AP10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="AO10" s="37"/>
-      <c r="AP10" s="37"/>
-      <c r="AQ10" s="45"/>
-      <c r="AR10" s="45"/>
-      <c r="AS10" s="37"/>
-      <c r="AT10" s="37"/>
+      <c r="AQ10" s="37"/>
+      <c r="AR10" s="37"/>
+      <c r="AS10" s="46"/>
+      <c r="AT10" s="46"/>
       <c r="AU10" s="37"/>
-      <c r="AV10" s="45"/>
-      <c r="AW10" s="45"/>
-      <c r="AX10" s="45"/>
-      <c r="AY10" s="35"/>
-      <c r="AZ10" s="37"/>
-      <c r="BA10" s="36"/>
-      <c r="BB10" s="36"/>
+      <c r="AV10" s="37"/>
+      <c r="AW10" s="37"/>
+      <c r="AX10" s="46"/>
+      <c r="AY10" s="46"/>
+      <c r="AZ10" s="46"/>
+      <c r="BA10" s="35"/>
+      <c r="BB10" s="37"/>
       <c r="BC10" s="36"/>
       <c r="BD10" s="36"/>
       <c r="BE10" s="36"/>
@@ -1749,72 +1747,74 @@
       <c r="BG10" s="36"/>
       <c r="BH10" s="36"/>
       <c r="BI10" s="36"/>
-      <c r="BJ10" s="39"/>
+      <c r="BJ10" s="36"/>
       <c r="BK10" s="36"/>
-      <c r="BL10" s="36"/>
+      <c r="BL10" s="39"/>
       <c r="BM10" s="36"/>
       <c r="BN10" s="36"/>
       <c r="BO10" s="36"/>
       <c r="BP10" s="36"/>
-      <c r="BQ10" s="27" t="s">
+      <c r="BQ10" s="36"/>
+      <c r="BR10" s="36"/>
+      <c r="BS10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="BR10" s="27" t="s">
+      <c r="BT10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="BS10" s="39"/>
-      <c r="BT10" s="36"/>
-      <c r="BU10" s="10" t="s">
+      <c r="BU10" s="39"/>
+      <c r="BV10" s="36"/>
+      <c r="BW10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="BV10" s="10" t="s">
+      <c r="BX10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="BW10" s="10" t="s">
+      <c r="BY10" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="BX10" s="10" t="s">
+      <c r="BZ10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="BY10" s="10" t="s">
+      <c r="CA10" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="BZ10" s="10" t="s">
+      <c r="CB10" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="CA10" s="10" t="s">
+      <c r="CC10" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="CB10" s="10" t="s">
+      <c r="CD10" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="CC10" s="10" t="s">
+      <c r="CE10" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="CD10" s="10" t="s">
+      <c r="CF10" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="CE10" s="10" t="s">
+      <c r="CG10" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="CF10" s="10" t="s">
+      <c r="CH10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="CG10" s="10" t="s">
+      <c r="CI10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="CH10" s="10" t="s">
+      <c r="CJ10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="CI10" s="10" t="s">
+      <c r="CK10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="CJ10" s="10" t="s">
+      <c r="CL10" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="CK10" s="30"/>
+      <c r="CM10" s="30"/>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
@@ -1840,279 +1840,285 @@
         <v>5</v>
       </c>
       <c r="I11" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="M11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="N11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="O11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="Q11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="R11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="20" t="e">
-        <f>R11+S11+T11+U11+V11+X11+W11</f>
+      <c r="S11" s="20" t="e">
+        <f>T11+U11+V11+W11+X11+Z11+Y11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="T11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="U11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="20" t="s">
+      <c r="V11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="20" t="s">
+      <c r="W11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="V11" s="20" t="s">
+      <c r="X11" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="W11" s="20" t="s">
+      <c r="Y11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="X11" s="20" t="s">
+      <c r="Z11" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="Y11" s="14" t="s">
+      <c r="AA11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="14" t="s">
+      <c r="AB11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AA11" s="14" t="s">
+      <c r="AC11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AB11" s="14" t="s">
+      <c r="AD11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AC11" s="14" t="s">
+      <c r="AE11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AD11" s="14" t="s">
+      <c r="AF11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AE11" s="14" t="s">
+      <c r="AG11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AF11" s="14" t="s">
+      <c r="AH11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AG11" s="20" t="e">
-        <f>IF((AH11+AI11+AJ11+AK11+AL11+AN11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AN11+AM11,)</f>
+      <c r="AI11" s="20" t="e">
+        <f>IF((AJ11+AK11+AL11+AM11+AN11+AP11+AO11)&gt;0,AJ11+AK11+AL11+AM11+AN11+AP11+AO11,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="20" t="s">
+      <c r="AJ11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AI11" s="20" t="s">
+      <c r="AK11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AJ11" s="20" t="s">
+      <c r="AL11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AK11" s="20" t="s">
+      <c r="AM11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AL11" s="20" t="s">
+      <c r="AN11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AM11" s="20" t="s">
+      <c r="AO11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AN11" s="20" t="s">
+      <c r="AP11" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="AO11" s="14" t="s">
+      <c r="AQ11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AP11" s="14" t="s">
+      <c r="AR11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AQ11" s="21" t="s">
+      <c r="AS11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AR11" s="21" t="s">
+      <c r="AT11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AS11" s="21" t="s">
+      <c r="AU11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AT11" s="14" t="s">
+      <c r="AV11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AU11" s="14" t="s">
+      <c r="AW11" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="AV11" s="14" t="s">
+      <c r="AX11" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AW11" s="14" t="s">
+      <c r="AY11" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="AX11" s="14" t="s">
+      <c r="AZ11" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="AY11" s="14" t="s">
+      <c r="BA11" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="AZ11" s="14" t="s">
+      <c r="BB11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="BA11" s="14" t="s">
+      <c r="BC11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="BB11" s="16" t="s">
+      <c r="BD11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BC11" s="16" t="s">
+      <c r="BE11" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BD11" s="17" t="s">
+      <c r="BF11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="BE11" s="16" t="s">
+      <c r="BG11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BF11" s="16" t="s">
+      <c r="BH11" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="BG11" s="16" t="e">
-        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
+      <c r="BI11" s="16" t="e">
+        <f>IF(BQ11&lt;=EOMONTH(BF11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="16" t="s">
+      <c r="BJ11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BI11" s="16" t="s">
+      <c r="BK11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="BJ11" s="16" t="s">
+      <c r="BL11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="BK11" s="16" t="e">
-        <f>IF(BO11&lt;=EOMONTH(BD11,12),"X","")</f>
+      <c r="BM11" s="16" t="e">
+        <f>IF(BQ11&lt;=EOMONTH(BF11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BL11" s="16" t="e">
-        <f>IF(AND(BO11&gt;=EOMONTH(BD11,13),BO11&lt;=EOMONTH(BD11,48)),"X","")</f>
+      <c r="BN11" s="16" t="e">
+        <f>IF(AND(BQ11&gt;=EOMONTH(BF11,13),BQ11&lt;=EOMONTH(BF11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BM11" s="16" t="e">
-        <f>IF(AND(BO11&gt;=EOMONTH(BD11,48),BO11&lt;=EOMONTH(BD11,72)),"X","")</f>
+      <c r="BO11" s="16" t="e">
+        <f>IF(AND(BQ11&gt;=EOMONTH(BF11,48),BQ11&lt;=EOMONTH(BF11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="16" t="e">
-        <f>IF(BO11&gt;=EOMONTH(BD11,73),"X","")</f>
+      <c r="BP11" s="16" t="e">
+        <f>IF(BQ11&gt;=EOMONTH(BF11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="17" t="s">
+      <c r="BQ11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="BP11" s="17" t="s">
+      <c r="BR11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="BQ11" s="22" t="e">
-        <f>(EOMONTH(BO11,0))-(BO11-DAY(BO11)+1)+1</f>
+      <c r="BS11" s="22" t="e">
+        <f>(EOMONTH(BQ11,0))-(BQ11-DAY(BQ11)+1)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BR11" s="22" t="e">
-        <f>BP11-BO11+1</f>
+      <c r="BT11" s="22" t="e">
+        <f>BR11-BQ11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BS11" s="22" t="s">
+      <c r="BU11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="BT11" s="23" t="e">
-        <f>BR11/BQ11</f>
+      <c r="BV11" s="23" t="e">
+        <f>BT11/BS11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BU11" s="23" t="s">
+      <c r="BW11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="BV11" s="23" t="s">
+      <c r="BX11" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="BW11" s="23" t="s">
+      <c r="BY11" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="BX11" s="23" t="s">
+      <c r="BZ11" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="BY11" s="23" t="s">
+      <c r="CA11" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="BZ11" s="23" t="s">
+      <c r="CB11" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="CA11" s="23" t="s">
+      <c r="CC11" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="CB11" s="18" t="s">
+      <c r="CD11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="CC11" s="16" t="s">
+      <c r="CE11" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="CD11" s="23" t="e">
-        <f>CA11*BT11</f>
+      <c r="CF11" s="23" t="e">
+        <f>CC11*BV11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="CE11" s="23" t="s">
+      <c r="CG11" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="CF11" s="18" t="s">
+      <c r="CH11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CG11" s="18" t="s">
+      <c r="CI11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CH11" s="18" t="s">
+      <c r="CJ11" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="CI11" s="18" t="s">
+      <c r="CK11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="CJ11" s="18" t="s">
+      <c r="CL11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="CK11" s="28" t="s">
+      <c r="CM11" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="CL11" s="25" t="s">
+      <c r="CN11" s="25" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="AV9:AV10"/>
-    <mergeCell ref="AW9:AW10"/>
+  <mergeCells count="68">
     <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:U9"/>
     <mergeCell ref="AQ9:AQ10"/>
     <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
@@ -2121,49 +2127,52 @@
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:X8"/>
-    <mergeCell ref="Y8:AN8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="K8:Z8"/>
+    <mergeCell ref="AA8:AP8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AB9:AB10"/>
     <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="AD9:AD10"/>
     <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BQ8:CL8"/>
+    <mergeCell ref="BP9:BP10"/>
+    <mergeCell ref="BQ9:BQ10"/>
+    <mergeCell ref="BR9:BR10"/>
     <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BO8:CJ8"/>
+    <mergeCell ref="CH9:CL9"/>
+    <mergeCell ref="BV9:BV10"/>
+    <mergeCell ref="BU9:BU10"/>
     <mergeCell ref="BN9:BN10"/>
     <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BP9:BP10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="CF9:CJ9"/>
-    <mergeCell ref="BT9:BT10"/>
-    <mergeCell ref="BS9:BS10"/>
-    <mergeCell ref="BL9:BL10"/>
+    <mergeCell ref="BD8:BP8"/>
+    <mergeCell ref="BW9:CG9"/>
+    <mergeCell ref="CM9:CM10"/>
+    <mergeCell ref="AS8:BA8"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BK9:BK10"/>
     <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BB8:BN8"/>
-    <mergeCell ref="BU9:CE9"/>
-    <mergeCell ref="CK9:CK10"/>
-    <mergeCell ref="AQ8:AY8"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
     <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AZ8:AZ10"/>
-    <mergeCell ref="BA8:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="AV9:AV10"/>
+    <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="BB8:BB10"/>
+    <mergeCell ref="BC8:BC10"/>
     <mergeCell ref="BD9:BD10"/>
     <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BL9:BL10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>